<commit_message>
Started implementing General Purpose Registers
</commit_message>
<xml_diff>
--- a/Documentation/CPU_DOC.xlsx
+++ b/Documentation/CPU_DOC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Desktop\CPU_8Bit\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F24C78A6-FA85-4110-A88D-5EE75F0DD0E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F53FBD81-AD37-4DFF-BE3A-4017675A659A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="3585" windowWidth="29040" windowHeight="16440" xr2:uid="{5BA4E079-EFAB-4B55-B322-C6522B3056FF}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="204">
   <si>
     <t>1=Read</t>
   </si>
@@ -346,12 +346,6 @@
     <t>direct</t>
   </si>
   <si>
-    <t>REG_Dest</t>
-  </si>
-  <si>
-    <t>REG_Source</t>
-  </si>
-  <si>
     <t>data</t>
   </si>
   <si>
@@ -653,6 +647,9 @@
   </si>
   <si>
     <t>UseBufAdr</t>
+  </si>
+  <si>
+    <t>REG_DS</t>
   </si>
 </sst>
 </file>
@@ -2235,6 +2232,12 @@
     <xf numFmtId="0" fontId="0" fillId="20" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2365,14 +2368,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2744,8 +2741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0373F33-972A-4E8D-B1CE-9C5EF0708B27}">
   <dimension ref="B2:AI157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B33" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J49" sqref="J49"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2772,50 +2769,50 @@
     </row>
     <row r="4" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="205" t="s">
-        <v>121</v>
-      </c>
-      <c r="D5" s="206"/>
-      <c r="E5" s="206"/>
-      <c r="F5" s="206"/>
-      <c r="G5" s="206"/>
-      <c r="H5" s="206"/>
-      <c r="I5" s="206"/>
-      <c r="J5" s="206"/>
-      <c r="K5" s="206"/>
-      <c r="L5" s="207"/>
+      <c r="C5" s="207" t="s">
+        <v>119</v>
+      </c>
+      <c r="D5" s="208"/>
+      <c r="E5" s="208"/>
+      <c r="F5" s="208"/>
+      <c r="G5" s="208"/>
+      <c r="H5" s="208"/>
+      <c r="I5" s="208"/>
+      <c r="J5" s="208"/>
+      <c r="K5" s="208"/>
+      <c r="L5" s="209"/>
       <c r="M5" s="128"/>
-      <c r="N5" s="219" t="s">
-        <v>120</v>
-      </c>
-      <c r="O5" s="219"/>
-      <c r="P5" s="219"/>
-      <c r="Q5" s="219"/>
-      <c r="R5" s="219"/>
-      <c r="S5" s="219"/>
-      <c r="T5" s="219"/>
-      <c r="U5" s="219"/>
-      <c r="V5" s="219"/>
-      <c r="W5" s="219"/>
-      <c r="X5" s="219"/>
-      <c r="Y5" s="219"/>
-      <c r="Z5" s="219"/>
-      <c r="AA5" s="219"/>
-      <c r="AB5" s="219"/>
-      <c r="AC5" s="220"/>
-      <c r="AD5" s="203"/>
+      <c r="N5" s="221" t="s">
+        <v>118</v>
+      </c>
+      <c r="O5" s="221"/>
+      <c r="P5" s="221"/>
+      <c r="Q5" s="221"/>
+      <c r="R5" s="221"/>
+      <c r="S5" s="221"/>
+      <c r="T5" s="221"/>
+      <c r="U5" s="221"/>
+      <c r="V5" s="221"/>
+      <c r="W5" s="221"/>
+      <c r="X5" s="221"/>
+      <c r="Y5" s="221"/>
+      <c r="Z5" s="221"/>
+      <c r="AA5" s="221"/>
+      <c r="AB5" s="221"/>
+      <c r="AC5" s="222"/>
+      <c r="AD5" s="205"/>
     </row>
     <row r="6" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="C6" s="208"/>
-      <c r="D6" s="209"/>
-      <c r="E6" s="209"/>
-      <c r="F6" s="209"/>
-      <c r="G6" s="209"/>
-      <c r="H6" s="209"/>
-      <c r="I6" s="209"/>
-      <c r="J6" s="209"/>
-      <c r="K6" s="209"/>
-      <c r="L6" s="210"/>
+      <c r="C6" s="210"/>
+      <c r="D6" s="211"/>
+      <c r="E6" s="211"/>
+      <c r="F6" s="211"/>
+      <c r="G6" s="211"/>
+      <c r="H6" s="211"/>
+      <c r="I6" s="211"/>
+      <c r="J6" s="211"/>
+      <c r="K6" s="211"/>
+      <c r="L6" s="212"/>
       <c r="M6" s="14"/>
       <c r="N6" s="4">
         <v>0</v>
@@ -2865,7 +2862,7 @@
       <c r="AC6" s="129">
         <v>15</v>
       </c>
-      <c r="AD6" s="204"/>
+      <c r="AD6" s="206"/>
       <c r="AE6" s="4"/>
       <c r="AF6" s="4"/>
       <c r="AG6" s="4"/>
@@ -2873,32 +2870,32 @@
       <c r="AI6" s="2"/>
     </row>
     <row r="7" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="C7" s="211"/>
-      <c r="D7" s="212"/>
-      <c r="E7" s="212"/>
-      <c r="F7" s="212"/>
-      <c r="G7" s="212"/>
+      <c r="C7" s="213"/>
+      <c r="D7" s="214"/>
+      <c r="E7" s="214"/>
+      <c r="F7" s="214"/>
+      <c r="G7" s="214"/>
       <c r="H7" s="12"/>
       <c r="I7" s="28" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J7" s="22" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="K7" s="22"/>
       <c r="L7" s="29"/>
       <c r="M7" s="126"/>
-      <c r="N7" s="221"/>
-      <c r="O7" s="221"/>
-      <c r="P7" s="221"/>
-      <c r="Q7" s="221"/>
-      <c r="R7" s="221"/>
-      <c r="S7" s="221"/>
+      <c r="N7" s="223"/>
+      <c r="O7" s="223"/>
+      <c r="P7" s="223"/>
+      <c r="Q7" s="223"/>
+      <c r="R7" s="223"/>
+      <c r="S7" s="223"/>
       <c r="T7" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="U7" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="V7" s="5" t="s">
         <v>0</v>
@@ -2910,65 +2907,65 @@
         <v>1</v>
       </c>
       <c r="Y7" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="Z7" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="AA7" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="AB7" s="222" t="s">
-        <v>155</v>
-      </c>
-      <c r="AC7" s="223"/>
-      <c r="AD7" s="204"/>
+        <v>148</v>
+      </c>
+      <c r="AB7" s="224" t="s">
+        <v>153</v>
+      </c>
+      <c r="AC7" s="225"/>
+      <c r="AD7" s="206"/>
       <c r="AE7" s="2"/>
       <c r="AF7" s="3"/>
       <c r="AG7" s="3"/>
       <c r="AH7" s="2"/>
     </row>
     <row r="8" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="C8" s="213"/>
-      <c r="D8" s="214"/>
-      <c r="E8" s="214"/>
-      <c r="F8" s="214"/>
-      <c r="G8" s="214"/>
+      <c r="C8" s="215"/>
+      <c r="D8" s="216"/>
+      <c r="E8" s="216"/>
+      <c r="F8" s="216"/>
+      <c r="G8" s="216"/>
       <c r="H8"/>
-      <c r="I8" s="215" t="s">
+      <c r="I8" s="217" t="s">
         <v>90</v>
       </c>
-      <c r="J8" s="216"/>
-      <c r="K8" s="216"/>
-      <c r="L8" s="217"/>
-      <c r="M8" s="218" t="s">
+      <c r="J8" s="218"/>
+      <c r="K8" s="218"/>
+      <c r="L8" s="219"/>
+      <c r="M8" s="220" t="s">
         <v>2</v>
       </c>
-      <c r="N8" s="218"/>
-      <c r="O8" s="218"/>
-      <c r="P8" s="218"/>
-      <c r="Q8" s="218"/>
-      <c r="R8" s="218"/>
-      <c r="S8" s="218"/>
-      <c r="T8" s="227" t="s">
-        <v>158</v>
-      </c>
-      <c r="U8" s="227"/>
-      <c r="V8" s="228" t="s">
-        <v>159</v>
-      </c>
-      <c r="W8" s="228"/>
-      <c r="X8" s="228"/>
-      <c r="Y8" s="228"/>
-      <c r="Z8" s="226" t="s">
+      <c r="N8" s="220"/>
+      <c r="O8" s="220"/>
+      <c r="P8" s="220"/>
+      <c r="Q8" s="220"/>
+      <c r="R8" s="220"/>
+      <c r="S8" s="220"/>
+      <c r="T8" s="229" t="s">
         <v>156</v>
       </c>
-      <c r="AA8" s="226"/>
-      <c r="AB8" s="224" t="s">
+      <c r="U8" s="229"/>
+      <c r="V8" s="230" t="s">
         <v>157</v>
       </c>
-      <c r="AC8" s="225"/>
-      <c r="AD8" s="204"/>
+      <c r="W8" s="230"/>
+      <c r="X8" s="230"/>
+      <c r="Y8" s="230"/>
+      <c r="Z8" s="228" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA8" s="228"/>
+      <c r="AB8" s="226" t="s">
+        <v>155</v>
+      </c>
+      <c r="AC8" s="227"/>
+      <c r="AD8" s="206"/>
       <c r="AE8" s="123"/>
       <c r="AF8" s="123"/>
       <c r="AG8" s="123"/>
@@ -2976,7 +2973,7 @@
     </row>
     <row r="9" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="45" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C9" s="130" t="s">
         <v>93</v>
@@ -3009,10 +3006,10 @@
         <v>98</v>
       </c>
       <c r="M9" s="127" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="O9" s="7" t="s">
         <v>5</v>
@@ -3033,40 +3030,40 @@
         <v>10</v>
       </c>
       <c r="U9" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="V9" s="8" t="s">
         <v>12</v>
       </c>
       <c r="W9" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="X9" s="8" t="s">
         <v>11</v>
       </c>
       <c r="Y9" s="8" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="Z9" s="8" t="s">
         <v>13</v>
       </c>
       <c r="AA9" s="8" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="AB9" s="124" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="AC9" s="131" t="s">
         <v>14</v>
       </c>
       <c r="AD9" s="167" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="AE9" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="AF9" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="AG9" s="2"/>
       <c r="AH9" s="2"/>
@@ -3280,10 +3277,10 @@
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="44" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H12" s="42"/>
       <c r="I12" s="21" t="s">
@@ -3969,7 +3966,7 @@
         <v>41</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="H19" s="16"/>
       <c r="I19" s="21" t="s">
@@ -4162,10 +4159,10 @@
       </c>
       <c r="E21" s="6"/>
       <c r="F21" s="44" t="s">
+        <v>122</v>
+      </c>
+      <c r="G21" s="10" t="s">
         <v>124</v>
-      </c>
-      <c r="G21" s="10" t="s">
-        <v>126</v>
       </c>
       <c r="H21" s="42"/>
       <c r="I21" s="21" t="s">
@@ -4958,8 +4955,8 @@
       <c r="I30" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="J30" s="21" t="s">
-        <v>99</v>
+      <c r="J30" s="21">
+        <v>1</v>
       </c>
       <c r="K30" s="21" t="s">
         <v>99</v>
@@ -5024,8 +5021,8 @@
       <c r="I31" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="J31" s="21" t="s">
-        <v>99</v>
+      <c r="J31" s="21">
+        <v>1</v>
       </c>
       <c r="K31" s="21" t="s">
         <v>99</v>
@@ -5090,8 +5087,8 @@
       <c r="I32" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="J32" s="21" t="s">
-        <v>99</v>
+      <c r="J32" s="21">
+        <v>1</v>
       </c>
       <c r="K32" s="21" t="s">
         <v>99</v>
@@ -5156,8 +5153,8 @@
       <c r="I33" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="J33" s="21" t="s">
-        <v>99</v>
+      <c r="J33" s="21">
+        <v>1</v>
       </c>
       <c r="K33" s="21" t="s">
         <v>99</v>
@@ -5222,8 +5219,8 @@
       <c r="I34" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="J34" s="21" t="s">
-        <v>99</v>
+      <c r="J34" s="21">
+        <v>1</v>
       </c>
       <c r="K34" s="21" t="s">
         <v>99</v>
@@ -5603,8 +5600,8 @@
       <c r="I39" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="J39" s="21" t="s">
-        <v>99</v>
+      <c r="J39" s="21">
+        <v>1</v>
       </c>
       <c r="K39" s="21" t="s">
         <v>99</v>
@@ -5669,8 +5666,8 @@
       <c r="I40" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="J40" s="21" t="s">
-        <v>99</v>
+      <c r="J40" s="21">
+        <v>1</v>
       </c>
       <c r="K40" s="21" t="s">
         <v>99</v>
@@ -5792,7 +5789,7 @@
       <c r="D42" s="2">
         <v>32</v>
       </c>
-      <c r="E42" s="247"/>
+      <c r="E42" s="203"/>
       <c r="F42" s="37" t="s">
         <v>17</v>
       </c>
@@ -5856,7 +5853,7 @@
       <c r="D43" s="2">
         <v>33</v>
       </c>
-      <c r="E43" s="247"/>
+      <c r="E43" s="203"/>
       <c r="F43" s="35" t="s">
         <v>63</v>
       </c>
@@ -5867,8 +5864,8 @@
       <c r="I43" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="J43" s="21" t="s">
-        <v>99</v>
+      <c r="J43" s="21">
+        <v>1</v>
       </c>
       <c r="K43" s="21" t="s">
         <v>99</v>
@@ -5920,7 +5917,7 @@
       <c r="D44" s="2">
         <v>34</v>
       </c>
-      <c r="E44" s="247"/>
+      <c r="E44" s="203"/>
       <c r="F44" s="37" t="s">
         <v>65</v>
       </c>
@@ -5928,14 +5925,14 @@
         <v>66</v>
       </c>
       <c r="H44" s="16"/>
-      <c r="I44" s="21" t="s">
-        <v>102</v>
+      <c r="I44" s="249" t="s">
+        <v>99</v>
       </c>
       <c r="J44" s="21" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="K44" s="21" t="s">
-        <v>99</v>
+        <v>203</v>
       </c>
       <c r="L44" s="9" t="s">
         <v>99</v>
@@ -5984,7 +5981,7 @@
       <c r="D45" s="2">
         <v>35</v>
       </c>
-      <c r="E45" s="247"/>
+      <c r="E45" s="203"/>
       <c r="F45" s="37" t="s">
         <v>59</v>
       </c>
@@ -5999,7 +5996,7 @@
         <v>99</v>
       </c>
       <c r="K45" s="21" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="L45" s="9" t="s">
         <v>99</v>
@@ -6048,7 +6045,7 @@
       <c r="D46" s="2">
         <v>36</v>
       </c>
-      <c r="E46" s="247"/>
+      <c r="E46" s="203"/>
       <c r="F46" s="35" t="s">
         <v>67</v>
       </c>
@@ -6063,7 +6060,7 @@
         <v>99</v>
       </c>
       <c r="K46" s="21" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="L46" s="9" t="s">
         <v>99</v>
@@ -6112,7 +6109,7 @@
       <c r="D47" s="2">
         <v>37</v>
       </c>
-      <c r="E47" s="247"/>
+      <c r="E47" s="203"/>
       <c r="F47" s="46"/>
       <c r="G47" s="10"/>
       <c r="H47" s="42"/>
@@ -6193,7 +6190,7 @@
       <c r="D48" s="2">
         <v>38</v>
       </c>
-      <c r="E48" s="247"/>
+      <c r="E48" s="203"/>
       <c r="F48" s="46"/>
       <c r="G48" s="10"/>
       <c r="H48" s="42"/>
@@ -6274,7 +6271,7 @@
       <c r="D49" s="2">
         <v>39</v>
       </c>
-      <c r="E49" s="247"/>
+      <c r="E49" s="203"/>
       <c r="F49" s="46"/>
       <c r="G49" s="10"/>
       <c r="H49" s="42"/>
@@ -6355,7 +6352,7 @@
       <c r="D50" s="2">
         <v>40</v>
       </c>
-      <c r="E50" s="247"/>
+      <c r="E50" s="203"/>
       <c r="F50" s="46"/>
       <c r="G50" s="10"/>
       <c r="H50" s="42"/>
@@ -6436,7 +6433,7 @@
       <c r="D51" s="2">
         <v>41</v>
       </c>
-      <c r="E51" s="247"/>
+      <c r="E51" s="203"/>
       <c r="F51" s="46"/>
       <c r="G51" s="10"/>
       <c r="H51" s="42"/>
@@ -6517,7 +6514,7 @@
       <c r="D52" s="2">
         <v>42</v>
       </c>
-      <c r="E52" s="247"/>
+      <c r="E52" s="203"/>
       <c r="F52" s="46"/>
       <c r="G52" s="10"/>
       <c r="H52" s="42"/>
@@ -6598,8 +6595,8 @@
       <c r="D53" s="2">
         <v>43</v>
       </c>
-      <c r="E53" s="247" t="s">
-        <v>190</v>
+      <c r="E53" s="203" t="s">
+        <v>188</v>
       </c>
       <c r="F53" s="38" t="s">
         <v>18</v>
@@ -6696,8 +6693,8 @@
       <c r="D54" s="2">
         <v>44</v>
       </c>
-      <c r="E54" s="247" t="s">
-        <v>190</v>
+      <c r="E54" s="203" t="s">
+        <v>188</v>
       </c>
       <c r="F54" s="39" t="s">
         <v>74</v>
@@ -6794,8 +6791,8 @@
       <c r="D55" s="2">
         <v>45</v>
       </c>
-      <c r="E55" s="247" t="s">
-        <v>190</v>
+      <c r="E55" s="203" t="s">
+        <v>188</v>
       </c>
       <c r="F55" s="39" t="s">
         <v>78</v>
@@ -6892,8 +6889,8 @@
       <c r="D56" s="2">
         <v>46</v>
       </c>
-      <c r="E56" s="247" t="s">
-        <v>190</v>
+      <c r="E56" s="203" t="s">
+        <v>188</v>
       </c>
       <c r="F56" s="38" t="s">
         <v>75</v>
@@ -6990,8 +6987,8 @@
       <c r="D57" s="2">
         <v>47</v>
       </c>
-      <c r="E57" s="247" t="s">
-        <v>190</v>
+      <c r="E57" s="203" t="s">
+        <v>188</v>
       </c>
       <c r="F57" s="38" t="s">
         <v>77</v>
@@ -7088,8 +7085,8 @@
       <c r="D58" s="2">
         <v>48</v>
       </c>
-      <c r="E58" s="247" t="s">
-        <v>190</v>
+      <c r="E58" s="203" t="s">
+        <v>188</v>
       </c>
       <c r="F58" s="38" t="s">
         <v>76</v>
@@ -7186,11 +7183,11 @@
       <c r="D59" s="2">
         <v>49</v>
       </c>
-      <c r="E59" s="247" t="s">
-        <v>190</v>
+      <c r="E59" s="203" t="s">
+        <v>188</v>
       </c>
       <c r="F59" s="39" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G59" s="14" t="s">
         <v>86</v>
@@ -7284,7 +7281,7 @@
       <c r="D60" s="2">
         <v>50</v>
       </c>
-      <c r="E60" s="247"/>
+      <c r="E60" s="203"/>
       <c r="F60" s="46"/>
       <c r="G60" s="10"/>
       <c r="H60" s="42"/>
@@ -7365,7 +7362,7 @@
       <c r="D61" s="2">
         <v>51</v>
       </c>
-      <c r="E61" s="247"/>
+      <c r="E61" s="203"/>
       <c r="F61" s="46"/>
       <c r="G61" s="10"/>
       <c r="H61" s="42"/>
@@ -7446,7 +7443,7 @@
       <c r="D62" s="2">
         <v>52</v>
       </c>
-      <c r="E62" s="247"/>
+      <c r="E62" s="203"/>
       <c r="F62" s="46"/>
       <c r="G62" s="10"/>
       <c r="H62" s="16"/>
@@ -7527,7 +7524,7 @@
       <c r="D63" s="2">
         <v>53</v>
       </c>
-      <c r="E63" s="247"/>
+      <c r="E63" s="203"/>
       <c r="F63" s="40" t="s">
         <v>79</v>
       </c>
@@ -7591,7 +7588,7 @@
       <c r="D64" s="2">
         <v>54</v>
       </c>
-      <c r="E64" s="247"/>
+      <c r="E64" s="203"/>
       <c r="F64" s="41" t="s">
         <v>88</v>
       </c>
@@ -7687,7 +7684,7 @@
       <c r="D65" s="2">
         <v>55</v>
       </c>
-      <c r="E65" s="247"/>
+      <c r="E65" s="203"/>
       <c r="F65" s="46"/>
       <c r="G65" s="10"/>
       <c r="H65" s="16"/>
@@ -7768,7 +7765,7 @@
       <c r="D66" s="2">
         <v>56</v>
       </c>
-      <c r="E66" s="247"/>
+      <c r="E66" s="203"/>
       <c r="F66" s="46"/>
       <c r="G66" s="10"/>
       <c r="H66" s="16"/>
@@ -7849,7 +7846,7 @@
       <c r="D67" s="2">
         <v>57</v>
       </c>
-      <c r="E67" s="247"/>
+      <c r="E67" s="203"/>
       <c r="F67" s="46"/>
       <c r="G67" s="10"/>
       <c r="H67" s="16"/>
@@ -7930,7 +7927,7 @@
       <c r="D68" s="2">
         <v>58</v>
       </c>
-      <c r="E68" s="247"/>
+      <c r="E68" s="203"/>
       <c r="F68" s="46"/>
       <c r="G68" s="10"/>
       <c r="H68" s="16"/>
@@ -8011,7 +8008,7 @@
       <c r="D69" s="2">
         <v>59</v>
       </c>
-      <c r="E69" s="247"/>
+      <c r="E69" s="203"/>
       <c r="F69" s="46"/>
       <c r="G69" s="10"/>
       <c r="H69" s="16"/>
@@ -8092,7 +8089,7 @@
       <c r="D70" s="2">
         <v>60</v>
       </c>
-      <c r="E70" s="247"/>
+      <c r="E70" s="203"/>
       <c r="F70" s="46"/>
       <c r="G70" s="10"/>
       <c r="H70" s="16"/>
@@ -8173,7 +8170,7 @@
       <c r="D71" s="2">
         <v>61</v>
       </c>
-      <c r="E71" s="247"/>
+      <c r="E71" s="203"/>
       <c r="F71" s="46"/>
       <c r="G71" s="10"/>
       <c r="H71" s="16"/>
@@ -8254,7 +8251,7 @@
       <c r="D72" s="2">
         <v>62</v>
       </c>
-      <c r="E72" s="247"/>
+      <c r="E72" s="203"/>
       <c r="F72" s="46"/>
       <c r="G72" s="46"/>
       <c r="H72" s="9"/>
@@ -8334,12 +8331,12 @@
       <c r="D73" s="157">
         <v>63</v>
       </c>
-      <c r="E73" s="248"/>
+      <c r="E73" s="204"/>
       <c r="F73" s="158" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G73" s="159" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H73" s="160"/>
       <c r="I73" s="121" t="s">
@@ -8430,12 +8427,12 @@
       <c r="D74" s="2">
         <v>64</v>
       </c>
-      <c r="E74" s="247"/>
+      <c r="E74" s="203"/>
       <c r="F74" s="125" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G74" s="10" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H74" s="16"/>
       <c r="L74" s="9"/>
@@ -8443,22 +8440,22 @@
         <v>0</v>
       </c>
       <c r="N74" s="149" t="s">
+        <v>164</v>
+      </c>
+      <c r="O74" s="149" t="s">
+        <v>165</v>
+      </c>
+      <c r="P74" s="149" t="s">
         <v>166</v>
       </c>
-      <c r="O74" s="149" t="s">
+      <c r="Q74" s="149" t="s">
         <v>167</v>
       </c>
-      <c r="P74" s="149" t="s">
+      <c r="R74" s="149" t="s">
         <v>168</v>
       </c>
-      <c r="Q74" s="149" t="s">
+      <c r="S74" s="150" t="s">
         <v>169</v>
-      </c>
-      <c r="R74" s="149" t="s">
-        <v>170</v>
-      </c>
-      <c r="S74" s="150" t="s">
-        <v>171</v>
       </c>
       <c r="T74" s="45">
         <v>0</v>
@@ -8515,12 +8512,12 @@
       <c r="D75" s="2">
         <v>65</v>
       </c>
-      <c r="E75" s="247"/>
+      <c r="E75" s="203"/>
       <c r="F75" s="46" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G75" s="10" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H75" s="16"/>
       <c r="L75" s="9"/>
@@ -8600,12 +8597,12 @@
       <c r="D76" s="2">
         <v>66</v>
       </c>
-      <c r="E76" s="247"/>
+      <c r="E76" s="203"/>
       <c r="F76" s="46" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G76" s="10" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H76" s="42"/>
       <c r="L76" s="11"/>
@@ -8685,12 +8682,12 @@
       <c r="D77" s="2">
         <v>67</v>
       </c>
-      <c r="E77" s="247"/>
+      <c r="E77" s="203"/>
       <c r="F77" s="46" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G77" s="10" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H77" s="16"/>
       <c r="L77" s="9"/>
@@ -8770,7 +8767,7 @@
       <c r="D78" s="2">
         <v>68</v>
       </c>
-      <c r="E78" s="247"/>
+      <c r="E78" s="203"/>
       <c r="F78" s="46"/>
       <c r="G78" s="10"/>
       <c r="H78" s="16"/>
@@ -8796,7 +8793,7 @@
       <c r="S78" s="45">
         <v>0</v>
       </c>
-      <c r="T78" s="249"/>
+      <c r="T78" s="45"/>
       <c r="U78" s="11"/>
       <c r="V78" s="45"/>
       <c r="W78" s="45"/>
@@ -8831,9 +8828,9 @@
       <c r="D79" s="2">
         <v>69</v>
       </c>
-      <c r="E79" s="247"/>
+      <c r="E79" s="203"/>
       <c r="F79" s="46" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G79" s="10"/>
       <c r="H79" s="16"/>
@@ -8859,7 +8856,7 @@
       <c r="S79" s="45">
         <v>0</v>
       </c>
-      <c r="T79" s="249">
+      <c r="T79" s="45">
         <v>0</v>
       </c>
       <c r="U79" s="46">
@@ -8914,7 +8911,7 @@
       <c r="D80" s="2">
         <v>70</v>
       </c>
-      <c r="E80" s="247"/>
+      <c r="E80" s="203"/>
       <c r="F80" s="46"/>
       <c r="G80" s="10"/>
       <c r="H80" s="16"/>
@@ -8969,7 +8966,7 @@
       <c r="D81" s="2">
         <v>71</v>
       </c>
-      <c r="E81" s="247"/>
+      <c r="E81" s="203"/>
       <c r="F81" s="46"/>
       <c r="G81" s="10"/>
       <c r="H81" s="16"/>
@@ -9024,7 +9021,7 @@
       <c r="D82" s="2">
         <v>72</v>
       </c>
-      <c r="E82" s="247"/>
+      <c r="E82" s="203"/>
       <c r="F82" s="46"/>
       <c r="G82" s="10"/>
       <c r="H82" s="16"/>
@@ -12159,31 +12156,31 @@
   <sheetData>
     <row r="2" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B3" s="233"/>
-      <c r="C3" s="234"/>
-      <c r="D3" s="234"/>
-      <c r="E3" s="234"/>
-      <c r="F3" s="234"/>
-      <c r="G3" s="234"/>
-      <c r="H3" s="235"/>
-      <c r="I3" s="239" t="s">
-        <v>109</v>
-      </c>
-      <c r="J3" s="240"/>
-      <c r="K3" s="240"/>
-      <c r="L3" s="240"/>
-      <c r="M3" s="240"/>
-      <c r="N3" s="240"/>
-      <c r="O3" s="240"/>
-      <c r="P3" s="240"/>
-      <c r="Q3" s="240"/>
-      <c r="R3" s="240"/>
-      <c r="S3" s="240"/>
-      <c r="T3" s="240"/>
-      <c r="U3" s="240"/>
-      <c r="V3" s="240"/>
-      <c r="W3" s="240"/>
-      <c r="X3" s="241"/>
+      <c r="B3" s="235"/>
+      <c r="C3" s="236"/>
+      <c r="D3" s="236"/>
+      <c r="E3" s="236"/>
+      <c r="F3" s="236"/>
+      <c r="G3" s="236"/>
+      <c r="H3" s="237"/>
+      <c r="I3" s="241" t="s">
+        <v>107</v>
+      </c>
+      <c r="J3" s="242"/>
+      <c r="K3" s="242"/>
+      <c r="L3" s="242"/>
+      <c r="M3" s="242"/>
+      <c r="N3" s="242"/>
+      <c r="O3" s="242"/>
+      <c r="P3" s="242"/>
+      <c r="Q3" s="242"/>
+      <c r="R3" s="242"/>
+      <c r="S3" s="242"/>
+      <c r="T3" s="242"/>
+      <c r="U3" s="242"/>
+      <c r="V3" s="242"/>
+      <c r="W3" s="242"/>
+      <c r="X3" s="243"/>
       <c r="Y3" s="81"/>
       <c r="Z3" s="56"/>
       <c r="AA3" s="56"/>
@@ -12191,20 +12188,20 @@
       <c r="AC3" s="3"/>
       <c r="AD3" s="2"/>
       <c r="AE3" s="1"/>
-      <c r="AF3" s="229"/>
-      <c r="AG3" s="229"/>
-      <c r="AH3" s="229"/>
-      <c r="AI3" s="229"/>
+      <c r="AF3" s="231"/>
+      <c r="AG3" s="231"/>
+      <c r="AH3" s="231"/>
+      <c r="AI3" s="231"/>
       <c r="AJ3" s="1"/>
     </row>
     <row r="4" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B4" s="236"/>
-      <c r="C4" s="237"/>
-      <c r="D4" s="237"/>
-      <c r="E4" s="237"/>
-      <c r="F4" s="237"/>
-      <c r="G4" s="237"/>
-      <c r="H4" s="238"/>
+      <c r="B4" s="238"/>
+      <c r="C4" s="239"/>
+      <c r="D4" s="239"/>
+      <c r="E4" s="239"/>
+      <c r="F4" s="239"/>
+      <c r="G4" s="239"/>
+      <c r="H4" s="240"/>
       <c r="I4" s="57">
         <v>0</v>
       </c>
@@ -12253,8 +12250,8 @@
       <c r="X4" s="58">
         <v>15</v>
       </c>
-      <c r="Y4" s="245" t="s">
-        <v>128</v>
+      <c r="Y4" s="247" t="s">
+        <v>126</v>
       </c>
       <c r="Z4" s="50"/>
       <c r="AA4" s="50"/>
@@ -12270,49 +12267,49 @@
     </row>
     <row r="5" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="59" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="244" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" s="245"/>
+      <c r="E5" s="245"/>
+      <c r="F5" s="245"/>
+      <c r="G5" s="245"/>
+      <c r="H5" s="246"/>
+      <c r="I5" s="232" t="s">
         <v>110</v>
       </c>
-      <c r="C5" s="242" t="s">
+      <c r="J5" s="233"/>
+      <c r="K5" s="233"/>
+      <c r="L5" s="233"/>
+      <c r="M5" s="233"/>
+      <c r="N5" s="234"/>
+      <c r="O5" s="232" t="s">
         <v>111</v>
       </c>
-      <c r="D5" s="243"/>
-      <c r="E5" s="243"/>
-      <c r="F5" s="243"/>
-      <c r="G5" s="243"/>
-      <c r="H5" s="244"/>
-      <c r="I5" s="230" t="s">
+      <c r="P5" s="233"/>
+      <c r="Q5" s="233"/>
+      <c r="R5" s="234"/>
+      <c r="S5" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="J5" s="231"/>
-      <c r="K5" s="231"/>
-      <c r="L5" s="231"/>
-      <c r="M5" s="231"/>
-      <c r="N5" s="232"/>
-      <c r="O5" s="230" t="s">
+      <c r="T5" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="P5" s="231"/>
-      <c r="Q5" s="231"/>
-      <c r="R5" s="232"/>
-      <c r="S5" s="24" t="s">
-        <v>114</v>
-      </c>
-      <c r="T5" s="24" t="s">
-        <v>115</v>
-      </c>
       <c r="U5" s="43" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="V5" s="25" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="W5" s="24" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="X5" s="60" t="s">
-        <v>123</v>
-      </c>
-      <c r="Y5" s="246"/>
+        <v>121</v>
+      </c>
+      <c r="Y5" s="248"/>
       <c r="Z5" s="3"/>
       <c r="AA5" s="3"/>
       <c r="AB5" s="3"/>
@@ -12499,7 +12496,7 @@
     </row>
     <row r="8" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B8" s="62" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C8" s="45">
         <v>0</v>
@@ -12621,7 +12618,7 @@
         <v>1</v>
       </c>
       <c r="N9" s="85" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="O9" s="86">
         <v>0</v>
@@ -13273,7 +13270,7 @@
     </row>
     <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B17" s="63" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C17" s="45">
         <v>0</v>
@@ -13359,7 +13356,7 @@
     </row>
     <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A18" s="117" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B18" s="77" t="s">
         <v>45</v>
@@ -13448,7 +13445,7 @@
     </row>
     <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19" s="117" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B19" s="77" t="s">
         <v>46</v>
@@ -13621,7 +13618,7 @@
     </row>
     <row r="21" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B21" s="69" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C21" s="70">
         <v>0</v>
@@ -15427,7 +15424,7 @@
       <c r="AD42" s="3"/>
       <c r="AE42" s="3"/>
       <c r="AG42" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="AI42" s="48">
         <v>0</v>
@@ -15549,7 +15546,7 @@
       </c>
       <c r="Z43" s="3"/>
       <c r="AG43" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="AI43" s="48">
         <v>0</v>
@@ -17533,34 +17530,34 @@
   <sheetData>
     <row r="4" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="3:19" x14ac:dyDescent="0.25">
       <c r="D5" s="119" t="s">
+        <v>133</v>
+      </c>
+      <c r="E5" s="120" t="s">
+        <v>134</v>
+      </c>
+      <c r="F5" s="119" t="s">
         <v>135</v>
       </c>
-      <c r="E5" s="120" t="s">
-        <v>136</v>
-      </c>
-      <c r="F5" s="119" t="s">
-        <v>137</v>
-      </c>
       <c r="H5" s="119" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="I5" s="120" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="J5" s="119" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="K5" s="119"/>
       <c r="L5" s="119" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M5" s="120" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="3:19" x14ac:dyDescent="0.25">
@@ -17571,7 +17568,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="45" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H6" s="45">
         <v>0</v>
@@ -17590,13 +17587,13 @@
         <v>0</v>
       </c>
       <c r="Q6" s="45" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="R6" s="45" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="S6" s="45" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="3:19" x14ac:dyDescent="0.25">
@@ -17607,7 +17604,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="45" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H7" s="45">
         <v>0</v>
@@ -17626,7 +17623,7 @@
         <v>0</v>
       </c>
       <c r="O7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="Q7" s="45">
         <v>0</v>
@@ -17635,7 +17632,7 @@
         <v>0</v>
       </c>
       <c r="S7" s="45" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="8" spans="3:19" x14ac:dyDescent="0.25">
@@ -17646,7 +17643,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="45" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H8" s="45">
         <v>0</v>
@@ -17665,7 +17662,7 @@
         <v>0</v>
       </c>
       <c r="O8" s="118" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="Q8" s="45">
         <v>0</v>
@@ -17674,7 +17671,7 @@
         <v>1</v>
       </c>
       <c r="S8" s="45" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="9" spans="3:19" x14ac:dyDescent="0.25">
@@ -17685,7 +17682,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="45" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H9" s="45">
         <v>0</v>
@@ -17710,7 +17707,7 @@
         <v>0</v>
       </c>
       <c r="S9" s="45" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10" spans="3:19" x14ac:dyDescent="0.25">
@@ -17737,7 +17734,7 @@
         <v>1</v>
       </c>
       <c r="S10" s="45" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="3:19" x14ac:dyDescent="0.25">
@@ -17770,10 +17767,10 @@
       </c>
       <c r="K12" s="45"/>
       <c r="L12" s="45" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="M12" s="45" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="3:19" x14ac:dyDescent="0.25">
@@ -17788,15 +17785,15 @@
       </c>
       <c r="K13" s="45"/>
       <c r="L13" s="45" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="M13" s="45" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="3:19" x14ac:dyDescent="0.25">
       <c r="Q15" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="16" spans="3:19" x14ac:dyDescent="0.25">
@@ -17804,34 +17801,34 @@
         <v>0</v>
       </c>
       <c r="R16" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="17" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Q17">
         <v>1</v>
       </c>
       <c r="R17" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="18" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="D18" s="237" t="s">
-        <v>178</v>
-      </c>
-      <c r="E18" s="237"/>
-      <c r="G18" s="237" t="s">
-        <v>181</v>
-      </c>
-      <c r="H18" s="237"/>
+      <c r="D18" s="239" t="s">
+        <v>176</v>
+      </c>
+      <c r="E18" s="239"/>
+      <c r="G18" s="239" t="s">
+        <v>179</v>
+      </c>
+      <c r="H18" s="239"/>
       <c r="Q18">
         <v>2</v>
       </c>
       <c r="R18" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="19" spans="3:18" x14ac:dyDescent="0.25">
@@ -17851,35 +17848,35 @@
         <v>3</v>
       </c>
       <c r="R19" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="20" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E20" t="s">
+        <v>178</v>
+      </c>
+      <c r="G20" t="s">
         <v>180</v>
       </c>
-      <c r="G20" t="s">
-        <v>182</v>
-      </c>
       <c r="H20" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="23" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C23" s="45" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D23" s="119" t="s">
         <v>18</v>
       </c>
       <c r="E23" s="120" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F23" s="119" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="24" spans="3:18" x14ac:dyDescent="0.25">
@@ -17893,16 +17890,16 @@
         <v>0</v>
       </c>
       <c r="F24" s="45" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="L24" t="s">
         <v>18</v>
       </c>
       <c r="M24" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="N24" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="25" spans="3:18" x14ac:dyDescent="0.25">
@@ -17916,7 +17913,7 @@
         <v>1</v>
       </c>
       <c r="F25" s="45" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" spans="3:18" x14ac:dyDescent="0.25">
@@ -17930,7 +17927,7 @@
         <v>0</v>
       </c>
       <c r="F26" s="45" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="27" spans="3:18" x14ac:dyDescent="0.25">
@@ -17944,7 +17941,7 @@
         <v>1</v>
       </c>
       <c r="F27" s="45" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="28" spans="3:18" x14ac:dyDescent="0.25">
@@ -17961,7 +17958,7 @@
         <v>0</v>
       </c>
       <c r="F29" s="45" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="30" spans="3:18" x14ac:dyDescent="0.25">
@@ -17975,7 +17972,7 @@
         <v>1</v>
       </c>
       <c r="F30" s="45" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="31" spans="3:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Implemented GPR Controller + Fixed RAM Paths
</commit_message>
<xml_diff>
--- a/Documentation/CPU_DOC.xlsx
+++ b/Documentation/CPU_DOC.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Desktop\CPU_8Bit\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\CPU_8Bit\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F53FBD81-AD37-4DFF-BE3A-4017675A659A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1C45EDB-9989-46B7-AF95-1DB1207B6BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="3585" windowWidth="29040" windowHeight="16440" xr2:uid="{5BA4E079-EFAB-4B55-B322-C6522B3056FF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{5BA4E079-EFAB-4B55-B322-C6522B3056FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Control-Unit" sheetId="1" r:id="rId1"/>
@@ -328,9 +328,6 @@
     <t>Bit_7</t>
   </si>
   <si>
-    <t>Bit_8</t>
-  </si>
-  <si>
     <t>Byte_0</t>
   </si>
   <si>
@@ -650,6 +647,9 @@
   </si>
   <si>
     <t>REG_DS</t>
+  </si>
+  <si>
+    <t>Bit_6</t>
   </si>
 </sst>
 </file>
@@ -2238,6 +2238,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2368,12 +2371,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2443,7 +2443,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2741,78 +2741,78 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0373F33-972A-4E8D-B1CE-9C5EF0708B27}">
   <dimension ref="B2:AI157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="K2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AC12" sqref="AC12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="12.5703125" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" style="45" customWidth="1"/>
-    <col min="6" max="6" width="22.42578125" style="45" customWidth="1"/>
-    <col min="7" max="7" width="32.28515625" style="45" customWidth="1"/>
-    <col min="8" max="8" width="6.140625" style="21" customWidth="1"/>
-    <col min="9" max="11" width="11.28515625" style="21" customWidth="1"/>
-    <col min="12" max="12" width="11.28515625" customWidth="1"/>
-    <col min="13" max="19" width="4.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" style="45" customWidth="1"/>
+    <col min="6" max="6" width="22.44140625" style="45" customWidth="1"/>
+    <col min="7" max="7" width="32.33203125" style="45" customWidth="1"/>
+    <col min="8" max="8" width="6.109375" style="21" customWidth="1"/>
+    <col min="9" max="11" width="11.33203125" style="21" customWidth="1"/>
+    <col min="12" max="12" width="11.33203125" customWidth="1"/>
+    <col min="13" max="19" width="4.44140625" customWidth="1"/>
     <col min="20" max="21" width="16" customWidth="1"/>
-    <col min="22" max="25" width="13.140625" customWidth="1"/>
-    <col min="30" max="30" width="21.85546875" style="45" customWidth="1"/>
+    <col min="22" max="25" width="13.109375" customWidth="1"/>
+    <col min="30" max="30" width="21.88671875" style="45" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="3"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="4" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="207" t="s">
-        <v>119</v>
-      </c>
-      <c r="D5" s="208"/>
-      <c r="E5" s="208"/>
-      <c r="F5" s="208"/>
-      <c r="G5" s="208"/>
-      <c r="H5" s="208"/>
-      <c r="I5" s="208"/>
-      <c r="J5" s="208"/>
-      <c r="K5" s="208"/>
-      <c r="L5" s="209"/>
+    <row r="4" spans="2:35" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="2:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C5" s="208" t="s">
+        <v>118</v>
+      </c>
+      <c r="D5" s="209"/>
+      <c r="E5" s="209"/>
+      <c r="F5" s="209"/>
+      <c r="G5" s="209"/>
+      <c r="H5" s="209"/>
+      <c r="I5" s="209"/>
+      <c r="J5" s="209"/>
+      <c r="K5" s="209"/>
+      <c r="L5" s="210"/>
       <c r="M5" s="128"/>
-      <c r="N5" s="221" t="s">
-        <v>118</v>
-      </c>
-      <c r="O5" s="221"/>
-      <c r="P5" s="221"/>
-      <c r="Q5" s="221"/>
-      <c r="R5" s="221"/>
-      <c r="S5" s="221"/>
-      <c r="T5" s="221"/>
-      <c r="U5" s="221"/>
-      <c r="V5" s="221"/>
-      <c r="W5" s="221"/>
-      <c r="X5" s="221"/>
-      <c r="Y5" s="221"/>
-      <c r="Z5" s="221"/>
-      <c r="AA5" s="221"/>
-      <c r="AB5" s="221"/>
-      <c r="AC5" s="222"/>
-      <c r="AD5" s="205"/>
-    </row>
-    <row r="6" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="C6" s="210"/>
-      <c r="D6" s="211"/>
-      <c r="E6" s="211"/>
-      <c r="F6" s="211"/>
-      <c r="G6" s="211"/>
-      <c r="H6" s="211"/>
-      <c r="I6" s="211"/>
-      <c r="J6" s="211"/>
-      <c r="K6" s="211"/>
-      <c r="L6" s="212"/>
+      <c r="N5" s="222" t="s">
+        <v>117</v>
+      </c>
+      <c r="O5" s="222"/>
+      <c r="P5" s="222"/>
+      <c r="Q5" s="222"/>
+      <c r="R5" s="222"/>
+      <c r="S5" s="222"/>
+      <c r="T5" s="222"/>
+      <c r="U5" s="222"/>
+      <c r="V5" s="222"/>
+      <c r="W5" s="222"/>
+      <c r="X5" s="222"/>
+      <c r="Y5" s="222"/>
+      <c r="Z5" s="222"/>
+      <c r="AA5" s="222"/>
+      <c r="AB5" s="222"/>
+      <c r="AC5" s="223"/>
+      <c r="AD5" s="206"/>
+    </row>
+    <row r="6" spans="2:35" x14ac:dyDescent="0.3">
+      <c r="C6" s="211"/>
+      <c r="D6" s="212"/>
+      <c r="E6" s="212"/>
+      <c r="F6" s="212"/>
+      <c r="G6" s="212"/>
+      <c r="H6" s="212"/>
+      <c r="I6" s="212"/>
+      <c r="J6" s="212"/>
+      <c r="K6" s="212"/>
+      <c r="L6" s="213"/>
       <c r="M6" s="14"/>
       <c r="N6" s="4">
         <v>0</v>
@@ -2862,118 +2862,118 @@
       <c r="AC6" s="129">
         <v>15</v>
       </c>
-      <c r="AD6" s="206"/>
+      <c r="AD6" s="207"/>
       <c r="AE6" s="4"/>
       <c r="AF6" s="4"/>
       <c r="AG6" s="4"/>
       <c r="AH6" s="4"/>
       <c r="AI6" s="2"/>
     </row>
-    <row r="7" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="C7" s="213"/>
-      <c r="D7" s="214"/>
-      <c r="E7" s="214"/>
-      <c r="F7" s="214"/>
-      <c r="G7" s="214"/>
+    <row r="7" spans="2:35" x14ac:dyDescent="0.3">
+      <c r="C7" s="214"/>
+      <c r="D7" s="215"/>
+      <c r="E7" s="215"/>
+      <c r="F7" s="215"/>
+      <c r="G7" s="215"/>
       <c r="H7" s="12"/>
       <c r="I7" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="J7" s="22" t="s">
         <v>103</v>
-      </c>
-      <c r="J7" s="22" t="s">
-        <v>104</v>
       </c>
       <c r="K7" s="22"/>
       <c r="L7" s="29"/>
       <c r="M7" s="126"/>
-      <c r="N7" s="223"/>
-      <c r="O7" s="223"/>
-      <c r="P7" s="223"/>
-      <c r="Q7" s="223"/>
-      <c r="R7" s="223"/>
-      <c r="S7" s="223"/>
+      <c r="N7" s="224"/>
+      <c r="O7" s="224"/>
+      <c r="P7" s="224"/>
+      <c r="Q7" s="224"/>
+      <c r="R7" s="224"/>
+      <c r="S7" s="224"/>
       <c r="T7" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="U7" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="V7" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="W7" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="X7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="Z7" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="U7" s="5" t="s">
+      <c r="AA7" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="V7" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="W7" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="X7" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y7" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="Z7" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="AA7" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="AB7" s="224" t="s">
-        <v>153</v>
-      </c>
-      <c r="AC7" s="225"/>
-      <c r="AD7" s="206"/>
+      <c r="AB7" s="225" t="s">
+        <v>152</v>
+      </c>
+      <c r="AC7" s="226"/>
+      <c r="AD7" s="207"/>
       <c r="AE7" s="2"/>
       <c r="AF7" s="3"/>
       <c r="AG7" s="3"/>
       <c r="AH7" s="2"/>
     </row>
-    <row r="8" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="C8" s="215"/>
-      <c r="D8" s="216"/>
-      <c r="E8" s="216"/>
-      <c r="F8" s="216"/>
-      <c r="G8" s="216"/>
+    <row r="8" spans="2:35" x14ac:dyDescent="0.3">
+      <c r="C8" s="216"/>
+      <c r="D8" s="217"/>
+      <c r="E8" s="217"/>
+      <c r="F8" s="217"/>
+      <c r="G8" s="217"/>
       <c r="H8"/>
-      <c r="I8" s="217" t="s">
+      <c r="I8" s="218" t="s">
         <v>90</v>
       </c>
-      <c r="J8" s="218"/>
-      <c r="K8" s="218"/>
-      <c r="L8" s="219"/>
-      <c r="M8" s="220" t="s">
+      <c r="J8" s="219"/>
+      <c r="K8" s="219"/>
+      <c r="L8" s="220"/>
+      <c r="M8" s="221" t="s">
         <v>2</v>
       </c>
-      <c r="N8" s="220"/>
-      <c r="O8" s="220"/>
-      <c r="P8" s="220"/>
-      <c r="Q8" s="220"/>
-      <c r="R8" s="220"/>
-      <c r="S8" s="220"/>
-      <c r="T8" s="229" t="s">
+      <c r="N8" s="221"/>
+      <c r="O8" s="221"/>
+      <c r="P8" s="221"/>
+      <c r="Q8" s="221"/>
+      <c r="R8" s="221"/>
+      <c r="S8" s="221"/>
+      <c r="T8" s="230" t="s">
+        <v>155</v>
+      </c>
+      <c r="U8" s="230"/>
+      <c r="V8" s="231" t="s">
         <v>156</v>
       </c>
-      <c r="U8" s="229"/>
-      <c r="V8" s="230" t="s">
-        <v>157</v>
-      </c>
-      <c r="W8" s="230"/>
-      <c r="X8" s="230"/>
-      <c r="Y8" s="230"/>
-      <c r="Z8" s="228" t="s">
+      <c r="W8" s="231"/>
+      <c r="X8" s="231"/>
+      <c r="Y8" s="231"/>
+      <c r="Z8" s="229" t="s">
+        <v>153</v>
+      </c>
+      <c r="AA8" s="229"/>
+      <c r="AB8" s="227" t="s">
         <v>154</v>
       </c>
-      <c r="AA8" s="228"/>
-      <c r="AB8" s="226" t="s">
-        <v>155</v>
-      </c>
-      <c r="AC8" s="227"/>
-      <c r="AD8" s="206"/>
+      <c r="AC8" s="228"/>
+      <c r="AD8" s="207"/>
       <c r="AE8" s="123"/>
       <c r="AF8" s="123"/>
       <c r="AG8" s="123"/>
       <c r="AH8" s="2"/>
     </row>
-    <row r="9" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="45" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C9" s="130" t="s">
         <v>93</v>
@@ -2994,22 +2994,22 @@
         <v>94</v>
       </c>
       <c r="I9" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="J9" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="J9" s="20" t="s">
+      <c r="K9" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="K9" s="20" t="s">
+      <c r="L9" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="L9" s="20" t="s">
-        <v>98</v>
-      </c>
       <c r="M9" s="127" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="O9" s="7" t="s">
         <v>5</v>
@@ -3030,45 +3030,45 @@
         <v>10</v>
       </c>
       <c r="U9" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="V9" s="8" t="s">
         <v>12</v>
       </c>
       <c r="W9" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="X9" s="8" t="s">
         <v>11</v>
       </c>
       <c r="Y9" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="Z9" s="8" t="s">
         <v>13</v>
       </c>
       <c r="AA9" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AB9" s="124" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AC9" s="131" t="s">
         <v>14</v>
       </c>
       <c r="AD9" s="167" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AE9" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="AF9" s="3" t="s">
         <v>183</v>
-      </c>
-      <c r="AF9" s="3" t="s">
-        <v>184</v>
       </c>
       <c r="AG9" s="2"/>
       <c r="AH9" s="2"/>
     </row>
-    <row r="10" spans="2:35" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:35" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B10" s="45" t="str">
         <f>DEC2HEX(D10)</f>
         <v>0</v>
@@ -3088,16 +3088,16 @@
       </c>
       <c r="H10" s="18"/>
       <c r="I10" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J10" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K10" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L10" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M10" s="163">
         <v>1</v>
@@ -3166,7 +3166,7 @@
       <c r="AH10" s="2"/>
       <c r="AI10" s="2"/>
     </row>
-    <row r="11" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B11" s="45" t="str">
         <f t="shared" ref="B11:B74" si="0">DEC2HEX(D11)</f>
         <v>1</v>
@@ -3186,16 +3186,16 @@
       </c>
       <c r="H11" s="16"/>
       <c r="I11" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J11" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K11" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L11" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M11" s="164">
         <v>1</v>
@@ -3264,7 +3264,7 @@
       <c r="AH11" s="2"/>
       <c r="AI11" s="2"/>
     </row>
-    <row r="12" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B12" s="45" t="str">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -3277,23 +3277,23 @@
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="44" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H12" s="42"/>
       <c r="I12" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J12" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K12" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L12" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M12" s="164">
         <v>1</v>
@@ -3362,7 +3362,7 @@
       <c r="AH12" s="2"/>
       <c r="AI12" s="2"/>
     </row>
-    <row r="13" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B13" s="45" t="str">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -3382,16 +3382,16 @@
       </c>
       <c r="H13" s="16"/>
       <c r="I13" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J13" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K13" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L13" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M13" s="164">
         <v>1</v>
@@ -3460,7 +3460,7 @@
       <c r="AH13" s="2"/>
       <c r="AI13" s="2"/>
     </row>
-    <row r="14" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B14" s="45" t="str">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -3480,16 +3480,16 @@
       </c>
       <c r="H14" s="16"/>
       <c r="I14" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J14" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K14" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L14" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M14" s="164">
         <v>1</v>
@@ -3558,7 +3558,7 @@
       <c r="AH14" s="2"/>
       <c r="AI14" s="2"/>
     </row>
-    <row r="15" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B15" s="45" t="str">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -3578,16 +3578,16 @@
       </c>
       <c r="H15" s="16"/>
       <c r="I15" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J15" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K15" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L15" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M15" s="164">
         <v>1</v>
@@ -3656,7 +3656,7 @@
       <c r="AH15" s="2"/>
       <c r="AI15" s="2"/>
     </row>
-    <row r="16" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B16" s="45" t="str">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -3676,16 +3676,16 @@
       </c>
       <c r="H16" s="16"/>
       <c r="I16" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J16" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K16" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L16" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M16" s="164">
         <v>1</v>
@@ -3754,7 +3754,7 @@
       <c r="AH16" s="2"/>
       <c r="AI16" s="2"/>
     </row>
-    <row r="17" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B17" s="45" t="str">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -3774,16 +3774,16 @@
       </c>
       <c r="H17" s="16"/>
       <c r="I17" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J17" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K17" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L17" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M17" s="164">
         <v>1</v>
@@ -3852,7 +3852,7 @@
       <c r="AH17" s="2"/>
       <c r="AI17" s="2"/>
     </row>
-    <row r="18" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B18" s="45" t="str">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -3872,16 +3872,16 @@
       </c>
       <c r="H18" s="16"/>
       <c r="I18" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J18" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K18" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L18" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M18" s="164">
         <v>1</v>
@@ -3950,7 +3950,7 @@
       <c r="AH18" s="2"/>
       <c r="AI18" s="2"/>
     </row>
-    <row r="19" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B19" s="45" t="str">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -3966,20 +3966,20 @@
         <v>41</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H19" s="16"/>
       <c r="I19" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J19" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K19" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L19" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M19" s="164">
         <v>1</v>
@@ -4048,7 +4048,7 @@
       <c r="AH19" s="2"/>
       <c r="AI19" s="2"/>
     </row>
-    <row r="20" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B20" s="45" t="str">
         <f t="shared" si="0"/>
         <v>A</v>
@@ -4068,16 +4068,16 @@
       </c>
       <c r="H20" s="16"/>
       <c r="I20" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J20" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K20" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L20" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M20" s="164">
         <v>1</v>
@@ -4146,7 +4146,7 @@
       <c r="AH20" s="2"/>
       <c r="AI20" s="2"/>
     </row>
-    <row r="21" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B21" s="45" t="str">
         <f t="shared" si="0"/>
         <v>B</v>
@@ -4159,23 +4159,23 @@
       </c>
       <c r="E21" s="6"/>
       <c r="F21" s="44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H21" s="42"/>
       <c r="I21" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J21" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K21" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L21" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M21" s="164">
         <v>1</v>
@@ -4244,7 +4244,7 @@
       <c r="AH21" s="2"/>
       <c r="AI21" s="2"/>
     </row>
-    <row r="22" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B22" s="45" t="str">
         <f t="shared" si="0"/>
         <v>C</v>
@@ -4264,16 +4264,16 @@
       </c>
       <c r="H22" s="16"/>
       <c r="I22" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J22" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K22" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L22" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M22" s="164">
         <v>1</v>
@@ -4342,7 +4342,7 @@
       <c r="AH22" s="2"/>
       <c r="AI22" s="2"/>
     </row>
-    <row r="23" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B23" s="45" t="str">
         <f t="shared" si="0"/>
         <v>D</v>
@@ -4362,16 +4362,16 @@
       </c>
       <c r="H23" s="16"/>
       <c r="I23" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J23" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K23" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L23" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M23" s="164">
         <v>1</v>
@@ -4440,7 +4440,7 @@
       <c r="AH23" s="2"/>
       <c r="AI23" s="2"/>
     </row>
-    <row r="24" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B24" s="45" t="str">
         <f t="shared" si="0"/>
         <v>E</v>
@@ -4522,7 +4522,7 @@
       <c r="AH24" s="2"/>
       <c r="AI24" s="2"/>
     </row>
-    <row r="25" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B25" s="45" t="str">
         <f t="shared" si="0"/>
         <v>F</v>
@@ -4604,7 +4604,7 @@
       <c r="AH25" s="2"/>
       <c r="AI25" s="2"/>
     </row>
-    <row r="26" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B26" s="45" t="str">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -4624,16 +4624,16 @@
       </c>
       <c r="H26" s="16"/>
       <c r="I26" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J26" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K26" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L26" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M26" s="170">
         <v>1</v>
@@ -4670,7 +4670,7 @@
       <c r="AH26" s="2"/>
       <c r="AI26" s="2"/>
     </row>
-    <row r="27" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B27" s="45" t="str">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -4690,16 +4690,16 @@
       </c>
       <c r="H27" s="16"/>
       <c r="I27" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J27" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K27" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L27" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M27" s="170">
         <v>1</v>
@@ -4768,7 +4768,7 @@
       <c r="AH27" s="2"/>
       <c r="AI27" s="2"/>
     </row>
-    <row r="28" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B28" s="45" t="str">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -4850,7 +4850,7 @@
       <c r="AH28" s="2"/>
       <c r="AI28" s="2"/>
     </row>
-    <row r="29" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B29" s="45" t="str">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -4933,7 +4933,7 @@
       <c r="AH29" s="2"/>
       <c r="AI29" s="2"/>
     </row>
-    <row r="30" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B30" s="45" t="str">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -4953,16 +4953,16 @@
       </c>
       <c r="H30" s="16"/>
       <c r="I30" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J30" s="21">
         <v>1</v>
       </c>
       <c r="K30" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L30" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M30" s="165">
         <v>1</v>
@@ -4999,7 +4999,7 @@
       <c r="AH30" s="2"/>
       <c r="AI30" s="2"/>
     </row>
-    <row r="31" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B31" s="45" t="str">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -5019,16 +5019,16 @@
       </c>
       <c r="H31" s="16"/>
       <c r="I31" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J31" s="21">
         <v>1</v>
       </c>
       <c r="K31" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L31" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M31" s="165">
         <v>1</v>
@@ -5065,7 +5065,7 @@
       <c r="AH31" s="2"/>
       <c r="AI31" s="2"/>
     </row>
-    <row r="32" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B32" s="45" t="str">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -5085,16 +5085,16 @@
       </c>
       <c r="H32" s="16"/>
       <c r="I32" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J32" s="21">
         <v>1</v>
       </c>
       <c r="K32" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L32" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M32" s="165">
         <v>1</v>
@@ -5131,7 +5131,7 @@
       <c r="AH32" s="2"/>
       <c r="AI32" s="2"/>
     </row>
-    <row r="33" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B33" s="45" t="str">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -5151,16 +5151,16 @@
       </c>
       <c r="H33" s="16"/>
       <c r="I33" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J33" s="21">
         <v>1</v>
       </c>
       <c r="K33" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L33" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M33" s="165">
         <v>1</v>
@@ -5197,7 +5197,7 @@
       <c r="AH33" s="2"/>
       <c r="AI33" s="2"/>
     </row>
-    <row r="34" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B34" s="45" t="str">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -5217,16 +5217,16 @@
       </c>
       <c r="H34" s="16"/>
       <c r="I34" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J34" s="21">
         <v>1</v>
       </c>
       <c r="K34" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L34" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M34" s="165">
         <v>1</v>
@@ -5263,7 +5263,7 @@
       <c r="AH34" s="2"/>
       <c r="AI34" s="2"/>
     </row>
-    <row r="35" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B35" s="45" t="str">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -5346,7 +5346,7 @@
       <c r="AH35" s="2"/>
       <c r="AI35" s="2"/>
     </row>
-    <row r="36" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B36" s="45" t="str">
         <f t="shared" si="0"/>
         <v>1A</v>
@@ -5429,7 +5429,7 @@
       <c r="AH36" s="2"/>
       <c r="AI36" s="2"/>
     </row>
-    <row r="37" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B37" s="45" t="str">
         <f t="shared" si="0"/>
         <v>1B</v>
@@ -5512,7 +5512,7 @@
       <c r="AH37" s="2"/>
       <c r="AI37" s="2"/>
     </row>
-    <row r="38" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B38" s="45" t="str">
         <f t="shared" si="0"/>
         <v>1C</v>
@@ -5532,16 +5532,16 @@
       </c>
       <c r="H38" s="16"/>
       <c r="I38" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J38" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K38" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L38" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M38" s="165">
         <v>1</v>
@@ -5578,7 +5578,7 @@
       <c r="AH38" s="2"/>
       <c r="AI38" s="2"/>
     </row>
-    <row r="39" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B39" s="45" t="str">
         <f t="shared" si="0"/>
         <v>1D</v>
@@ -5598,16 +5598,16 @@
       </c>
       <c r="H39" s="16"/>
       <c r="I39" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J39" s="21">
         <v>1</v>
       </c>
       <c r="K39" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L39" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M39" s="165">
         <v>1</v>
@@ -5644,7 +5644,7 @@
       <c r="AH39" s="2"/>
       <c r="AI39" s="2"/>
     </row>
-    <row r="40" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B40" s="45" t="str">
         <f t="shared" si="0"/>
         <v>1E</v>
@@ -5664,16 +5664,16 @@
       </c>
       <c r="H40" s="16"/>
       <c r="I40" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J40" s="21">
         <v>1</v>
       </c>
       <c r="K40" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L40" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M40" s="165">
         <v>1</v>
@@ -5710,7 +5710,7 @@
       <c r="AH40" s="2"/>
       <c r="AI40" s="2"/>
     </row>
-    <row r="41" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B41" s="45" t="str">
         <f t="shared" si="0"/>
         <v>1F</v>
@@ -5731,16 +5731,16 @@
       </c>
       <c r="H41" s="16"/>
       <c r="I41" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J41" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K41" s="21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L41" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M41" s="165">
         <v>1</v>
@@ -5777,7 +5777,7 @@
       <c r="AH41" s="2"/>
       <c r="AI41" s="2"/>
     </row>
-    <row r="42" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B42" s="45" t="str">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -5798,16 +5798,16 @@
       </c>
       <c r="H42" s="16"/>
       <c r="I42" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J42" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K42" s="21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L42" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M42" s="165">
         <v>1</v>
@@ -5841,7 +5841,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="43" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B43" s="45" t="str">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -5862,16 +5862,16 @@
       </c>
       <c r="H43" s="16"/>
       <c r="I43" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J43" s="21">
         <v>1</v>
       </c>
       <c r="K43" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L43" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M43" s="165">
         <v>1</v>
@@ -5905,7 +5905,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="44" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B44" s="45" t="str">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -5925,17 +5925,17 @@
         <v>66</v>
       </c>
       <c r="H44" s="16"/>
-      <c r="I44" s="249" t="s">
-        <v>99</v>
+      <c r="I44" s="205" t="s">
+        <v>98</v>
       </c>
       <c r="J44" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K44" s="21" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L44" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M44" s="165">
         <v>1</v>
@@ -5969,7 +5969,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="45" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B45" s="45" t="str">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -5990,16 +5990,16 @@
       </c>
       <c r="H45" s="16"/>
       <c r="I45" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J45" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K45" s="21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L45" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M45" s="165">
         <v>1</v>
@@ -6033,7 +6033,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="46" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B46" s="45" t="str">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -6054,16 +6054,16 @@
       </c>
       <c r="H46" s="16"/>
       <c r="I46" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J46" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K46" s="21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L46" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M46" s="165">
         <v>1</v>
@@ -6097,7 +6097,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="47" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B47" s="45" t="str">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -6178,7 +6178,7 @@
         <v>C0</v>
       </c>
     </row>
-    <row r="48" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B48" s="45" t="str">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -6259,7 +6259,7 @@
         <v>C0</v>
       </c>
     </row>
-    <row r="49" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B49" s="45" t="str">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -6340,7 +6340,7 @@
         <v>C0</v>
       </c>
     </row>
-    <row r="50" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B50" s="45" t="str">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -6421,7 +6421,7 @@
         <v>C0</v>
       </c>
     </row>
-    <row r="51" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B51" s="45" t="str">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -6502,7 +6502,7 @@
         <v>C0</v>
       </c>
     </row>
-    <row r="52" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B52" s="45" t="str">
         <f t="shared" si="0"/>
         <v>2A</v>
@@ -6583,7 +6583,7 @@
         <v>C0</v>
       </c>
     </row>
-    <row r="53" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B53" s="45" t="str">
         <f t="shared" si="0"/>
         <v>2B</v>
@@ -6596,7 +6596,7 @@
         <v>43</v>
       </c>
       <c r="E53" s="203" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F53" s="38" t="s">
         <v>18</v>
@@ -6606,16 +6606,16 @@
       </c>
       <c r="H53" s="16"/>
       <c r="I53" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J53" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K53" s="21" t="s">
         <v>93</v>
       </c>
       <c r="L53" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M53" s="165">
         <v>1</v>
@@ -6681,7 +6681,7 @@
         <v>A8</v>
       </c>
     </row>
-    <row r="54" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B54" s="45" t="str">
         <f t="shared" si="0"/>
         <v>2C</v>
@@ -6694,7 +6694,7 @@
         <v>44</v>
       </c>
       <c r="E54" s="203" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F54" s="39" t="s">
         <v>74</v>
@@ -6704,16 +6704,16 @@
       </c>
       <c r="H54" s="16"/>
       <c r="I54" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J54" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K54" s="21" t="s">
         <v>93</v>
       </c>
       <c r="L54" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M54" s="165">
         <v>1</v>
@@ -6779,7 +6779,7 @@
         <v>A8</v>
       </c>
     </row>
-    <row r="55" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B55" s="45" t="str">
         <f t="shared" si="0"/>
         <v>2D</v>
@@ -6792,7 +6792,7 @@
         <v>45</v>
       </c>
       <c r="E55" s="203" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F55" s="39" t="s">
         <v>78</v>
@@ -6802,16 +6802,16 @@
       </c>
       <c r="H55" s="16"/>
       <c r="I55" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J55" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K55" s="21" t="s">
         <v>93</v>
       </c>
       <c r="L55" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M55" s="165">
         <v>1</v>
@@ -6877,7 +6877,7 @@
         <v>A8</v>
       </c>
     </row>
-    <row r="56" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B56" s="45" t="str">
         <f t="shared" si="0"/>
         <v>2E</v>
@@ -6890,7 +6890,7 @@
         <v>46</v>
       </c>
       <c r="E56" s="203" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F56" s="38" t="s">
         <v>75</v>
@@ -6900,16 +6900,16 @@
       </c>
       <c r="H56" s="16"/>
       <c r="I56" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J56" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K56" s="21" t="s">
         <v>93</v>
       </c>
       <c r="L56" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M56" s="165">
         <v>1</v>
@@ -6975,7 +6975,7 @@
         <v>A8</v>
       </c>
     </row>
-    <row r="57" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B57" s="45" t="str">
         <f t="shared" si="0"/>
         <v>2F</v>
@@ -6988,7 +6988,7 @@
         <v>47</v>
       </c>
       <c r="E57" s="203" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F57" s="38" t="s">
         <v>77</v>
@@ -6998,16 +6998,16 @@
       </c>
       <c r="H57" s="16"/>
       <c r="I57" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J57" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K57" s="21" t="s">
         <v>93</v>
       </c>
       <c r="L57" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M57" s="165">
         <v>1</v>
@@ -7073,7 +7073,7 @@
         <v>A8</v>
       </c>
     </row>
-    <row r="58" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B58" s="45" t="str">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -7086,7 +7086,7 @@
         <v>48</v>
       </c>
       <c r="E58" s="203" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F58" s="38" t="s">
         <v>76</v>
@@ -7096,16 +7096,16 @@
       </c>
       <c r="H58" s="16"/>
       <c r="I58" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J58" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K58" s="21" t="s">
         <v>93</v>
       </c>
       <c r="L58" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M58" s="165">
         <v>1</v>
@@ -7171,7 +7171,7 @@
         <v>A8</v>
       </c>
     </row>
-    <row r="59" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B59" s="45" t="str">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -7184,26 +7184,26 @@
         <v>49</v>
       </c>
       <c r="E59" s="203" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F59" s="39" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G59" s="14" t="s">
         <v>86</v>
       </c>
       <c r="H59" s="16"/>
       <c r="I59" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J59" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K59" s="21" t="s">
         <v>93</v>
       </c>
       <c r="L59" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M59" s="165">
         <v>1</v>
@@ -7269,7 +7269,7 @@
         <v>A8</v>
       </c>
     </row>
-    <row r="60" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B60" s="45" t="str">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -7350,7 +7350,7 @@
         <v>C0</v>
       </c>
     </row>
-    <row r="61" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B61" s="45" t="str">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -7431,7 +7431,7 @@
         <v>C0</v>
       </c>
     </row>
-    <row r="62" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B62" s="45" t="str">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -7512,7 +7512,7 @@
         <v>C0</v>
       </c>
     </row>
-    <row r="63" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B63" s="45" t="str">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -7533,16 +7533,16 @@
       </c>
       <c r="H63" s="16"/>
       <c r="I63" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J63" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K63" s="21" t="s">
         <v>93</v>
       </c>
       <c r="L63" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M63" s="165">
         <v>1</v>
@@ -7576,7 +7576,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="64" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B64" s="45" t="str">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -7597,16 +7597,16 @@
       </c>
       <c r="H64" s="16"/>
       <c r="I64" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J64" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K64" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L64" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M64" s="165">
         <v>1</v>
@@ -7672,7 +7672,7 @@
         <v>C0</v>
       </c>
     </row>
-    <row r="65" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B65" s="45" t="str">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -7753,7 +7753,7 @@
         <v>C0</v>
       </c>
     </row>
-    <row r="66" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B66" s="45" t="str">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -7834,7 +7834,7 @@
         <v>C0</v>
       </c>
     </row>
-    <row r="67" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B67" s="45" t="str">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -7915,7 +7915,7 @@
         <v>C0</v>
       </c>
     </row>
-    <row r="68" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B68" s="45" t="str">
         <f t="shared" si="0"/>
         <v>3A</v>
@@ -7996,7 +7996,7 @@
         <v>C0</v>
       </c>
     </row>
-    <row r="69" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B69" s="45" t="str">
         <f t="shared" si="0"/>
         <v>3B</v>
@@ -8077,7 +8077,7 @@
         <v>C0</v>
       </c>
     </row>
-    <row r="70" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B70" s="45" t="str">
         <f t="shared" si="0"/>
         <v>3C</v>
@@ -8158,7 +8158,7 @@
         <v>C0</v>
       </c>
     </row>
-    <row r="71" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B71" s="45" t="str">
         <f t="shared" si="0"/>
         <v>3D</v>
@@ -8239,7 +8239,7 @@
         <v>C0</v>
       </c>
     </row>
-    <row r="72" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B72" s="45" t="str">
         <f t="shared" si="0"/>
         <v>3E</v>
@@ -8319,7 +8319,7 @@
         <v>C0</v>
       </c>
     </row>
-    <row r="73" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B73" s="45" t="str">
         <f t="shared" si="0"/>
         <v>3F</v>
@@ -8333,23 +8333,23 @@
       </c>
       <c r="E73" s="204"/>
       <c r="F73" s="158" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G73" s="159" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H73" s="160"/>
       <c r="I73" s="121" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J73" s="121" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K73" s="121" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L73" s="122" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M73" s="166">
         <v>0</v>
@@ -8415,7 +8415,7 @@
         <v>FF</v>
       </c>
     </row>
-    <row r="74" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B74" s="45" t="str">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -8429,10 +8429,10 @@
       </c>
       <c r="E74" s="203"/>
       <c r="F74" s="125" t="s">
+        <v>157</v>
+      </c>
+      <c r="G74" s="10" t="s">
         <v>158</v>
-      </c>
-      <c r="G74" s="10" t="s">
-        <v>159</v>
       </c>
       <c r="H74" s="16"/>
       <c r="L74" s="9"/>
@@ -8440,22 +8440,22 @@
         <v>0</v>
       </c>
       <c r="N74" s="149" t="s">
+        <v>163</v>
+      </c>
+      <c r="O74" s="149" t="s">
         <v>164</v>
       </c>
-      <c r="O74" s="149" t="s">
+      <c r="P74" s="149" t="s">
         <v>165</v>
       </c>
-      <c r="P74" s="149" t="s">
+      <c r="Q74" s="149" t="s">
         <v>166</v>
       </c>
-      <c r="Q74" s="149" t="s">
+      <c r="R74" s="149" t="s">
         <v>167</v>
       </c>
-      <c r="R74" s="149" t="s">
+      <c r="S74" s="150" t="s">
         <v>168</v>
-      </c>
-      <c r="S74" s="150" t="s">
-        <v>169</v>
       </c>
       <c r="T74" s="45">
         <v>0</v>
@@ -8500,7 +8500,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="75" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B75" s="45" t="str">
         <f t="shared" ref="B75:B137" si="5">DEC2HEX(D75)</f>
         <v>41</v>
@@ -8514,10 +8514,10 @@
       </c>
       <c r="E75" s="203"/>
       <c r="F75" s="46" t="s">
+        <v>160</v>
+      </c>
+      <c r="G75" s="10" t="s">
         <v>161</v>
-      </c>
-      <c r="G75" s="10" t="s">
-        <v>162</v>
       </c>
       <c r="H75" s="16"/>
       <c r="L75" s="9"/>
@@ -8585,7 +8585,7 @@
         <v>C0</v>
       </c>
     </row>
-    <row r="76" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B76" s="45" t="str">
         <f t="shared" si="5"/>
         <v>42</v>
@@ -8599,10 +8599,10 @@
       </c>
       <c r="E76" s="203"/>
       <c r="F76" s="46" t="s">
+        <v>169</v>
+      </c>
+      <c r="G76" s="10" t="s">
         <v>170</v>
-      </c>
-      <c r="G76" s="10" t="s">
-        <v>171</v>
       </c>
       <c r="H76" s="42"/>
       <c r="L76" s="11"/>
@@ -8670,7 +8670,7 @@
         <v>C0</v>
       </c>
     </row>
-    <row r="77" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B77" s="45" t="str">
         <f t="shared" si="5"/>
         <v>43</v>
@@ -8684,10 +8684,10 @@
       </c>
       <c r="E77" s="203"/>
       <c r="F77" s="46" t="s">
+        <v>171</v>
+      </c>
+      <c r="G77" s="10" t="s">
         <v>172</v>
-      </c>
-      <c r="G77" s="10" t="s">
-        <v>173</v>
       </c>
       <c r="H77" s="16"/>
       <c r="L77" s="9"/>
@@ -8755,7 +8755,7 @@
         <v>C0</v>
       </c>
     </row>
-    <row r="78" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B78" s="45" t="str">
         <f t="shared" si="5"/>
         <v>44</v>
@@ -8816,7 +8816,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="79" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B79" s="45" t="str">
         <f t="shared" si="5"/>
         <v>45</v>
@@ -8830,7 +8830,7 @@
       </c>
       <c r="E79" s="203"/>
       <c r="F79" s="46" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G79" s="10"/>
       <c r="H79" s="16"/>
@@ -8899,7 +8899,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="80" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B80" s="45" t="str">
         <f t="shared" si="5"/>
         <v>46</v>
@@ -8954,7 +8954,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="81" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B81" s="45" t="str">
         <f t="shared" si="5"/>
         <v>47</v>
@@ -9009,7 +9009,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="82" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B82" s="45" t="str">
         <f t="shared" si="5"/>
         <v>48</v>
@@ -9064,7 +9064,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="83" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B83" s="45" t="str">
         <f t="shared" si="5"/>
         <v>49</v>
@@ -9118,7 +9118,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="84" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B84" s="45" t="str">
         <f t="shared" si="5"/>
         <v>4A</v>
@@ -9172,7 +9172,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="85" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B85" s="45" t="str">
         <f t="shared" si="5"/>
         <v>4B</v>
@@ -9226,7 +9226,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="86" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B86" s="45" t="str">
         <f t="shared" si="5"/>
         <v>4C</v>
@@ -9280,7 +9280,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="87" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B87" s="45" t="str">
         <f t="shared" si="5"/>
         <v>4D</v>
@@ -9334,7 +9334,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="88" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B88" s="45" t="str">
         <f t="shared" si="5"/>
         <v>4E</v>
@@ -9388,7 +9388,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="89" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B89" s="45" t="str">
         <f t="shared" si="5"/>
         <v>4F</v>
@@ -9442,7 +9442,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="90" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B90" s="45" t="str">
         <f t="shared" si="5"/>
         <v>50</v>
@@ -9496,7 +9496,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="91" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B91" s="45" t="str">
         <f t="shared" si="5"/>
         <v>51</v>
@@ -9550,7 +9550,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="92" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B92" s="45" t="str">
         <f t="shared" si="5"/>
         <v>52</v>
@@ -9604,7 +9604,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="93" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B93" s="45" t="str">
         <f t="shared" si="5"/>
         <v>53</v>
@@ -9658,7 +9658,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="94" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B94" s="45" t="str">
         <f t="shared" si="5"/>
         <v>54</v>
@@ -9712,7 +9712,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="95" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B95" s="45" t="str">
         <f t="shared" si="5"/>
         <v>55</v>
@@ -9766,7 +9766,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="96" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B96" s="45" t="str">
         <f t="shared" si="5"/>
         <v>56</v>
@@ -9820,7 +9820,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="97" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B97" s="45" t="str">
         <f t="shared" si="5"/>
         <v>57</v>
@@ -9874,7 +9874,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="98" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B98" s="45" t="str">
         <f t="shared" si="5"/>
         <v>58</v>
@@ -9928,7 +9928,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="99" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B99" s="45" t="str">
         <f t="shared" si="5"/>
         <v>59</v>
@@ -9982,7 +9982,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="100" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B100" s="45" t="str">
         <f t="shared" si="5"/>
         <v>5A</v>
@@ -10036,7 +10036,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="101" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B101" s="45" t="str">
         <f t="shared" si="5"/>
         <v>5B</v>
@@ -10090,7 +10090,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="102" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B102" s="45" t="str">
         <f t="shared" si="5"/>
         <v>5C</v>
@@ -10144,7 +10144,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="103" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B103" s="45" t="str">
         <f t="shared" si="5"/>
         <v>5D</v>
@@ -10198,7 +10198,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="104" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B104" s="45" t="str">
         <f t="shared" si="5"/>
         <v>5E</v>
@@ -10252,7 +10252,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="105" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B105" s="45" t="str">
         <f t="shared" si="5"/>
         <v>5F</v>
@@ -10306,7 +10306,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="106" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B106" s="45" t="str">
         <f t="shared" si="5"/>
         <v>60</v>
@@ -10360,7 +10360,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="107" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B107" s="45" t="str">
         <f t="shared" si="5"/>
         <v>61</v>
@@ -10414,7 +10414,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="108" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B108" s="45" t="str">
         <f t="shared" si="5"/>
         <v>62</v>
@@ -10468,7 +10468,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="109" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B109" s="45" t="str">
         <f t="shared" si="5"/>
         <v>63</v>
@@ -10522,7 +10522,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="110" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B110" s="45" t="str">
         <f t="shared" si="5"/>
         <v>64</v>
@@ -10576,7 +10576,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="111" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B111" s="45" t="str">
         <f t="shared" si="5"/>
         <v>65</v>
@@ -10630,7 +10630,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="112" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B112" s="45" t="str">
         <f t="shared" si="5"/>
         <v>66</v>
@@ -10684,7 +10684,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="113" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B113" s="45" t="str">
         <f t="shared" si="5"/>
         <v>67</v>
@@ -10738,7 +10738,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="114" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B114" s="45" t="str">
         <f t="shared" si="5"/>
         <v>68</v>
@@ -10792,7 +10792,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="115" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B115" s="45" t="str">
         <f t="shared" si="5"/>
         <v>69</v>
@@ -10846,7 +10846,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="116" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B116" s="45" t="str">
         <f t="shared" si="5"/>
         <v>6A</v>
@@ -10900,7 +10900,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="117" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B117" s="45" t="str">
         <f t="shared" si="5"/>
         <v>6B</v>
@@ -10954,7 +10954,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="118" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B118" s="45" t="str">
         <f t="shared" si="5"/>
         <v>6C</v>
@@ -11008,7 +11008,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="119" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B119" s="45" t="str">
         <f t="shared" si="5"/>
         <v>6D</v>
@@ -11062,7 +11062,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="120" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B120" s="45" t="str">
         <f t="shared" si="5"/>
         <v>6E</v>
@@ -11116,7 +11116,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="121" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B121" s="45" t="str">
         <f t="shared" si="5"/>
         <v>6F</v>
@@ -11170,7 +11170,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="122" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B122" s="45" t="str">
         <f t="shared" si="5"/>
         <v>70</v>
@@ -11224,7 +11224,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="123" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B123" s="45" t="str">
         <f t="shared" si="5"/>
         <v>71</v>
@@ -11278,7 +11278,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="124" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B124" s="45" t="str">
         <f t="shared" si="5"/>
         <v>72</v>
@@ -11332,7 +11332,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="125" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B125" s="45" t="str">
         <f t="shared" si="5"/>
         <v>73</v>
@@ -11386,7 +11386,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="126" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B126" s="45" t="str">
         <f t="shared" si="5"/>
         <v>74</v>
@@ -11440,7 +11440,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="127" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B127" s="45" t="str">
         <f t="shared" si="5"/>
         <v>75</v>
@@ -11494,7 +11494,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="128" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B128" s="45" t="str">
         <f t="shared" si="5"/>
         <v>76</v>
@@ -11548,7 +11548,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="129" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B129" s="45" t="str">
         <f t="shared" si="5"/>
         <v>77</v>
@@ -11602,7 +11602,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="130" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B130" s="45" t="str">
         <f t="shared" si="5"/>
         <v>78</v>
@@ -11656,7 +11656,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="131" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B131" s="45" t="str">
         <f t="shared" si="5"/>
         <v>79</v>
@@ -11710,7 +11710,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="132" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B132" s="45" t="str">
         <f t="shared" si="5"/>
         <v>7A</v>
@@ -11764,7 +11764,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="133" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B133" s="45" t="str">
         <f t="shared" si="5"/>
         <v>7B</v>
@@ -11818,7 +11818,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="134" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B134" s="45" t="str">
         <f t="shared" si="5"/>
         <v>7C</v>
@@ -11872,7 +11872,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="135" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B135" s="45" t="str">
         <f t="shared" si="5"/>
         <v>7D</v>
@@ -11926,7 +11926,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="136" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B136" s="45" t="str">
         <f t="shared" si="5"/>
         <v>7E</v>
@@ -11980,7 +11980,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="137" spans="2:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B137" s="45" t="str">
         <f t="shared" si="5"/>
         <v>7F</v>
@@ -12044,13 +12044,13 @@
         <v>00</v>
       </c>
     </row>
-    <row r="138" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:32" x14ac:dyDescent="0.3">
       <c r="C138" t="s">
         <v>71</v>
       </c>
       <c r="AC138" s="11"/>
     </row>
-    <row r="139" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:32" x14ac:dyDescent="0.3">
       <c r="D139" t="s">
         <v>72</v>
       </c>
@@ -12059,58 +12059,58 @@
       </c>
       <c r="AC139" s="11"/>
     </row>
-    <row r="140" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:32" x14ac:dyDescent="0.3">
       <c r="AC140" s="11"/>
     </row>
-    <row r="141" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:32" x14ac:dyDescent="0.3">
       <c r="AC141" s="11"/>
     </row>
-    <row r="142" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:32" x14ac:dyDescent="0.3">
       <c r="AC142" s="11"/>
     </row>
-    <row r="143" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:32" x14ac:dyDescent="0.3">
       <c r="AC143" s="11"/>
     </row>
-    <row r="144" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:32" x14ac:dyDescent="0.3">
       <c r="AC144" s="11"/>
     </row>
-    <row r="145" spans="29:29" x14ac:dyDescent="0.25">
+    <row r="145" spans="29:29" x14ac:dyDescent="0.3">
       <c r="AC145" s="11"/>
     </row>
-    <row r="146" spans="29:29" x14ac:dyDescent="0.25">
+    <row r="146" spans="29:29" x14ac:dyDescent="0.3">
       <c r="AC146" s="11"/>
     </row>
-    <row r="147" spans="29:29" x14ac:dyDescent="0.25">
+    <row r="147" spans="29:29" x14ac:dyDescent="0.3">
       <c r="AC147" s="11"/>
     </row>
-    <row r="148" spans="29:29" x14ac:dyDescent="0.25">
+    <row r="148" spans="29:29" x14ac:dyDescent="0.3">
       <c r="AC148" s="11"/>
     </row>
-    <row r="149" spans="29:29" x14ac:dyDescent="0.25">
+    <row r="149" spans="29:29" x14ac:dyDescent="0.3">
       <c r="AC149" s="11"/>
     </row>
-    <row r="150" spans="29:29" x14ac:dyDescent="0.25">
+    <row r="150" spans="29:29" x14ac:dyDescent="0.3">
       <c r="AC150" s="11"/>
     </row>
-    <row r="151" spans="29:29" x14ac:dyDescent="0.25">
+    <row r="151" spans="29:29" x14ac:dyDescent="0.3">
       <c r="AC151" s="11"/>
     </row>
-    <row r="152" spans="29:29" x14ac:dyDescent="0.25">
+    <row r="152" spans="29:29" x14ac:dyDescent="0.3">
       <c r="AC152" s="11"/>
     </row>
-    <row r="153" spans="29:29" x14ac:dyDescent="0.25">
+    <row r="153" spans="29:29" x14ac:dyDescent="0.3">
       <c r="AC153" s="11"/>
     </row>
-    <row r="154" spans="29:29" x14ac:dyDescent="0.25">
+    <row r="154" spans="29:29" x14ac:dyDescent="0.3">
       <c r="AC154" s="11"/>
     </row>
-    <row r="155" spans="29:29" x14ac:dyDescent="0.25">
+    <row r="155" spans="29:29" x14ac:dyDescent="0.3">
       <c r="AC155" s="11"/>
     </row>
-    <row r="156" spans="29:29" x14ac:dyDescent="0.25">
+    <row r="156" spans="29:29" x14ac:dyDescent="0.3">
       <c r="AC156" s="11"/>
     </row>
-    <row r="157" spans="29:29" x14ac:dyDescent="0.25">
+    <row r="157" spans="29:29" x14ac:dyDescent="0.3">
       <c r="AC157" s="11"/>
     </row>
   </sheetData>
@@ -12142,45 +12142,45 @@
       <selection activeCell="Y6" sqref="Y6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="45"/>
+    <col min="1" max="1" width="11.44140625" style="45"/>
     <col min="3" max="3" width="4" style="45" customWidth="1"/>
     <col min="4" max="8" width="4" customWidth="1"/>
-    <col min="9" max="17" width="4.42578125" customWidth="1"/>
-    <col min="18" max="21" width="6.85546875" customWidth="1"/>
+    <col min="9" max="17" width="4.44140625" customWidth="1"/>
+    <col min="18" max="21" width="6.88671875" customWidth="1"/>
     <col min="22" max="24" width="9" customWidth="1"/>
-    <col min="25" max="25" width="15.42578125" style="45" customWidth="1"/>
-    <col min="30" max="30" width="25.7109375" customWidth="1"/>
+    <col min="25" max="25" width="15.44140625" style="45" customWidth="1"/>
+    <col min="30" max="30" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B3" s="235"/>
-      <c r="C3" s="236"/>
-      <c r="D3" s="236"/>
-      <c r="E3" s="236"/>
-      <c r="F3" s="236"/>
-      <c r="G3" s="236"/>
-      <c r="H3" s="237"/>
-      <c r="I3" s="241" t="s">
-        <v>107</v>
-      </c>
-      <c r="J3" s="242"/>
-      <c r="K3" s="242"/>
-      <c r="L3" s="242"/>
-      <c r="M3" s="242"/>
-      <c r="N3" s="242"/>
-      <c r="O3" s="242"/>
-      <c r="P3" s="242"/>
-      <c r="Q3" s="242"/>
-      <c r="R3" s="242"/>
-      <c r="S3" s="242"/>
-      <c r="T3" s="242"/>
-      <c r="U3" s="242"/>
-      <c r="V3" s="242"/>
-      <c r="W3" s="242"/>
-      <c r="X3" s="243"/>
+    <row r="2" spans="2:36" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:36" x14ac:dyDescent="0.3">
+      <c r="B3" s="236"/>
+      <c r="C3" s="237"/>
+      <c r="D3" s="237"/>
+      <c r="E3" s="237"/>
+      <c r="F3" s="237"/>
+      <c r="G3" s="237"/>
+      <c r="H3" s="238"/>
+      <c r="I3" s="242" t="s">
+        <v>106</v>
+      </c>
+      <c r="J3" s="243"/>
+      <c r="K3" s="243"/>
+      <c r="L3" s="243"/>
+      <c r="M3" s="243"/>
+      <c r="N3" s="243"/>
+      <c r="O3" s="243"/>
+      <c r="P3" s="243"/>
+      <c r="Q3" s="243"/>
+      <c r="R3" s="243"/>
+      <c r="S3" s="243"/>
+      <c r="T3" s="243"/>
+      <c r="U3" s="243"/>
+      <c r="V3" s="243"/>
+      <c r="W3" s="243"/>
+      <c r="X3" s="244"/>
       <c r="Y3" s="81"/>
       <c r="Z3" s="56"/>
       <c r="AA3" s="56"/>
@@ -12188,20 +12188,20 @@
       <c r="AC3" s="3"/>
       <c r="AD3" s="2"/>
       <c r="AE3" s="1"/>
-      <c r="AF3" s="231"/>
-      <c r="AG3" s="231"/>
-      <c r="AH3" s="231"/>
-      <c r="AI3" s="231"/>
+      <c r="AF3" s="232"/>
+      <c r="AG3" s="232"/>
+      <c r="AH3" s="232"/>
+      <c r="AI3" s="232"/>
       <c r="AJ3" s="1"/>
     </row>
-    <row r="4" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B4" s="238"/>
-      <c r="C4" s="239"/>
-      <c r="D4" s="239"/>
-      <c r="E4" s="239"/>
-      <c r="F4" s="239"/>
-      <c r="G4" s="239"/>
-      <c r="H4" s="240"/>
+    <row r="4" spans="2:36" x14ac:dyDescent="0.3">
+      <c r="B4" s="239"/>
+      <c r="C4" s="240"/>
+      <c r="D4" s="240"/>
+      <c r="E4" s="240"/>
+      <c r="F4" s="240"/>
+      <c r="G4" s="240"/>
+      <c r="H4" s="241"/>
       <c r="I4" s="57">
         <v>0</v>
       </c>
@@ -12250,8 +12250,8 @@
       <c r="X4" s="58">
         <v>15</v>
       </c>
-      <c r="Y4" s="247" t="s">
-        <v>126</v>
+      <c r="Y4" s="248" t="s">
+        <v>125</v>
       </c>
       <c r="Z4" s="50"/>
       <c r="AA4" s="50"/>
@@ -12265,51 +12265,51 @@
       <c r="AI4" s="1"/>
       <c r="AJ4" s="1"/>
     </row>
-    <row r="5" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:36" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="59" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" s="245" t="s">
         <v>108</v>
       </c>
-      <c r="C5" s="244" t="s">
+      <c r="D5" s="246"/>
+      <c r="E5" s="246"/>
+      <c r="F5" s="246"/>
+      <c r="G5" s="246"/>
+      <c r="H5" s="247"/>
+      <c r="I5" s="233" t="s">
         <v>109</v>
       </c>
-      <c r="D5" s="245"/>
-      <c r="E5" s="245"/>
-      <c r="F5" s="245"/>
-      <c r="G5" s="245"/>
-      <c r="H5" s="246"/>
-      <c r="I5" s="232" t="s">
+      <c r="J5" s="234"/>
+      <c r="K5" s="234"/>
+      <c r="L5" s="234"/>
+      <c r="M5" s="234"/>
+      <c r="N5" s="235"/>
+      <c r="O5" s="233" t="s">
         <v>110</v>
       </c>
-      <c r="J5" s="233"/>
-      <c r="K5" s="233"/>
-      <c r="L5" s="233"/>
-      <c r="M5" s="233"/>
-      <c r="N5" s="234"/>
-      <c r="O5" s="232" t="s">
+      <c r="P5" s="234"/>
+      <c r="Q5" s="234"/>
+      <c r="R5" s="235"/>
+      <c r="S5" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="P5" s="233"/>
-      <c r="Q5" s="233"/>
-      <c r="R5" s="234"/>
-      <c r="S5" s="24" t="s">
+      <c r="T5" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="T5" s="24" t="s">
-        <v>113</v>
-      </c>
       <c r="U5" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="V5" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="W5" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="X5" s="60" t="s">
         <v>120</v>
       </c>
-      <c r="V5" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="W5" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="X5" s="60" t="s">
-        <v>121</v>
-      </c>
-      <c r="Y5" s="248"/>
+      <c r="Y5" s="249"/>
       <c r="Z5" s="3"/>
       <c r="AA5" s="3"/>
       <c r="AB5" s="3"/>
@@ -12322,7 +12322,7 @@
       <c r="AI5" s="1"/>
       <c r="AJ5" s="1"/>
     </row>
-    <row r="6" spans="2:36" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:36" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B6" s="61" t="s">
         <v>15</v>
       </c>
@@ -12408,7 +12408,7 @@
       <c r="AI6" s="1"/>
       <c r="AJ6" s="1"/>
     </row>
-    <row r="7" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:36" x14ac:dyDescent="0.3">
       <c r="B7" s="73" t="s">
         <v>19</v>
       </c>
@@ -12494,9 +12494,9 @@
       <c r="AI7" s="1"/>
       <c r="AJ7" s="1"/>
     </row>
-    <row r="8" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:36" x14ac:dyDescent="0.3">
       <c r="B8" s="62" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C8" s="45">
         <v>0</v>
@@ -12580,7 +12580,7 @@
       <c r="AI8" s="1"/>
       <c r="AJ8" s="1"/>
     </row>
-    <row r="9" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:36" x14ac:dyDescent="0.3">
       <c r="B9" s="73" t="s">
         <v>20</v>
       </c>
@@ -12618,7 +12618,7 @@
         <v>1</v>
       </c>
       <c r="N9" s="85" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="O9" s="86">
         <v>0</v>
@@ -12666,7 +12666,7 @@
       <c r="AI9" s="1"/>
       <c r="AJ9" s="1"/>
     </row>
-    <row r="10" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:36" x14ac:dyDescent="0.3">
       <c r="B10" s="62" t="s">
         <v>24</v>
       </c>
@@ -12752,7 +12752,7 @@
       <c r="AI10" s="1"/>
       <c r="AJ10" s="1"/>
     </row>
-    <row r="11" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:36" x14ac:dyDescent="0.3">
       <c r="B11" s="62" t="s">
         <v>28</v>
       </c>
@@ -12838,7 +12838,7 @@
       <c r="AI11" s="1"/>
       <c r="AJ11" s="1"/>
     </row>
-    <row r="12" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:36" x14ac:dyDescent="0.3">
       <c r="B12" s="62" t="s">
         <v>32</v>
       </c>
@@ -12924,7 +12924,7 @@
       <c r="AI12" s="1"/>
       <c r="AJ12" s="1"/>
     </row>
-    <row r="13" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:36" x14ac:dyDescent="0.3">
       <c r="B13" s="62" t="s">
         <v>16</v>
       </c>
@@ -13010,7 +13010,7 @@
       <c r="AI13" s="1"/>
       <c r="AJ13" s="1"/>
     </row>
-    <row r="14" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:36" x14ac:dyDescent="0.3">
       <c r="B14" s="63" t="s">
         <v>39</v>
       </c>
@@ -13096,7 +13096,7 @@
       <c r="AI14" s="1"/>
       <c r="AJ14" s="1"/>
     </row>
-    <row r="15" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:36" x14ac:dyDescent="0.3">
       <c r="B15" s="63" t="s">
         <v>41</v>
       </c>
@@ -13182,7 +13182,7 @@
       <c r="AI15" s="1"/>
       <c r="AJ15" s="1"/>
     </row>
-    <row r="16" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:36" x14ac:dyDescent="0.3">
       <c r="B16" s="63" t="s">
         <v>44</v>
       </c>
@@ -13268,9 +13268,9 @@
       <c r="AI16" s="1"/>
       <c r="AJ16" s="1"/>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.3">
       <c r="B17" s="63" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C17" s="45">
         <v>0</v>
@@ -13354,9 +13354,9 @@
       <c r="AI17" s="1"/>
       <c r="AJ17" s="1"/>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A18" s="117" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B18" s="77" t="s">
         <v>45</v>
@@ -13443,9 +13443,9 @@
       <c r="AI18" s="1"/>
       <c r="AJ18" s="1"/>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A19" s="117" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B19" s="77" t="s">
         <v>46</v>
@@ -13532,7 +13532,7 @@
       <c r="AI19" s="1"/>
       <c r="AJ19" s="1"/>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.3">
       <c r="B20" s="64"/>
       <c r="C20" s="45">
         <v>0</v>
@@ -13616,9 +13616,9 @@
       <c r="AI20" s="1"/>
       <c r="AJ20" s="1"/>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.3">
       <c r="B21" s="69" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C21" s="70">
         <v>0</v>
@@ -13702,7 +13702,7 @@
       <c r="AI21" s="1"/>
       <c r="AJ21" s="1"/>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.3">
       <c r="B22" s="65"/>
       <c r="C22" s="45">
         <v>0</v>
@@ -13786,7 +13786,7 @@
       <c r="AI22" s="1"/>
       <c r="AJ22" s="1"/>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.3">
       <c r="B23" s="65"/>
       <c r="C23" s="45">
         <v>0</v>
@@ -13870,7 +13870,7 @@
       <c r="AI23" s="1"/>
       <c r="AJ23" s="1"/>
     </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.3">
       <c r="B24" s="65"/>
       <c r="C24" s="45">
         <v>0</v>
@@ -13954,7 +13954,7 @@
       <c r="AI24" s="1"/>
       <c r="AJ24" s="1"/>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.3">
       <c r="B25" s="65"/>
       <c r="C25" s="45">
         <v>0</v>
@@ -14038,7 +14038,7 @@
       <c r="AI25" s="1"/>
       <c r="AJ25" s="1"/>
     </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.3">
       <c r="B26" s="65"/>
       <c r="C26" s="45">
         <v>0</v>
@@ -14122,7 +14122,7 @@
       <c r="AI26" s="1"/>
       <c r="AJ26" s="1"/>
     </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:36" x14ac:dyDescent="0.3">
       <c r="B27" s="65"/>
       <c r="C27" s="45">
         <v>0</v>
@@ -14206,7 +14206,7 @@
       <c r="AI27" s="1"/>
       <c r="AJ27" s="1"/>
     </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:36" x14ac:dyDescent="0.3">
       <c r="B28" s="65"/>
       <c r="C28" s="45">
         <v>0</v>
@@ -14290,7 +14290,7 @@
       <c r="AI28" s="1"/>
       <c r="AJ28" s="1"/>
     </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:36" x14ac:dyDescent="0.3">
       <c r="B29" s="65"/>
       <c r="C29" s="45">
         <v>0</v>
@@ -14374,7 +14374,7 @@
       <c r="AI29" s="1"/>
       <c r="AJ29" s="1"/>
     </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:36" x14ac:dyDescent="0.3">
       <c r="B30" s="63"/>
       <c r="C30" s="45">
         <v>0</v>
@@ -14458,7 +14458,7 @@
       <c r="AI30" s="1"/>
       <c r="AJ30" s="1"/>
     </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:36" x14ac:dyDescent="0.3">
       <c r="B31" s="63"/>
       <c r="C31" s="45">
         <v>0</v>
@@ -14542,7 +14542,7 @@
       <c r="AI31" s="1"/>
       <c r="AJ31" s="1"/>
     </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:36" x14ac:dyDescent="0.3">
       <c r="B32" s="64"/>
       <c r="C32" s="45">
         <v>0</v>
@@ -14626,7 +14626,7 @@
       <c r="AI32" s="1"/>
       <c r="AJ32" s="1"/>
     </row>
-    <row r="33" spans="2:50" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:50" x14ac:dyDescent="0.3">
       <c r="B33" s="66"/>
       <c r="C33" s="45">
         <v>0</v>
@@ -14710,7 +14710,7 @@
       <c r="AI33" s="1"/>
       <c r="AJ33" s="1"/>
     </row>
-    <row r="34" spans="2:50" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:50" x14ac:dyDescent="0.3">
       <c r="B34" s="65"/>
       <c r="C34" s="45">
         <v>0</v>
@@ -14794,7 +14794,7 @@
       <c r="AI34" s="1"/>
       <c r="AJ34" s="1"/>
     </row>
-    <row r="35" spans="2:50" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:50" x14ac:dyDescent="0.3">
       <c r="B35" s="65"/>
       <c r="C35" s="45">
         <v>0</v>
@@ -14878,7 +14878,7 @@
       <c r="AI35" s="1"/>
       <c r="AJ35" s="1"/>
     </row>
-    <row r="36" spans="2:50" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:50" x14ac:dyDescent="0.3">
       <c r="B36" s="65"/>
       <c r="C36" s="45">
         <v>0</v>
@@ -14962,7 +14962,7 @@
       <c r="AI36" s="1"/>
       <c r="AJ36" s="1"/>
     </row>
-    <row r="37" spans="2:50" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:50" x14ac:dyDescent="0.3">
       <c r="B37" s="65"/>
       <c r="C37" s="45">
         <v>0</v>
@@ -15046,7 +15046,7 @@
       <c r="AI37" s="1"/>
       <c r="AJ37" s="1"/>
     </row>
-    <row r="38" spans="2:50" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:50" x14ac:dyDescent="0.3">
       <c r="B38" s="65"/>
       <c r="C38" s="3">
         <v>1</v>
@@ -15130,7 +15130,7 @@
       <c r="AI38" s="1"/>
       <c r="AJ38" s="1"/>
     </row>
-    <row r="39" spans="2:50" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:50" x14ac:dyDescent="0.3">
       <c r="B39" s="65"/>
       <c r="C39" s="3">
         <v>1</v>
@@ -15203,7 +15203,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="40" spans="2:50" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:50" x14ac:dyDescent="0.3">
       <c r="B40" s="65"/>
       <c r="C40" s="3">
         <v>1</v>
@@ -15276,7 +15276,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="41" spans="2:50" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:50" x14ac:dyDescent="0.3">
       <c r="B41" s="65"/>
       <c r="C41" s="3">
         <v>1</v>
@@ -15349,7 +15349,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="42" spans="2:50" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:50" x14ac:dyDescent="0.3">
       <c r="B42" s="65"/>
       <c r="C42" s="3">
         <v>1</v>
@@ -15424,7 +15424,7 @@
       <c r="AD42" s="3"/>
       <c r="AE42" s="3"/>
       <c r="AG42" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AI42" s="48">
         <v>0</v>
@@ -15472,7 +15472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:50" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:50" x14ac:dyDescent="0.3">
       <c r="B43" s="65"/>
       <c r="C43" s="3">
         <v>1</v>
@@ -15546,7 +15546,7 @@
       </c>
       <c r="Z43" s="3"/>
       <c r="AG43" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AI43" s="48">
         <v>0</v>
@@ -15594,7 +15594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="2:50" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:50" x14ac:dyDescent="0.3">
       <c r="B44" s="65"/>
       <c r="C44" s="3">
         <v>1</v>
@@ -15668,7 +15668,7 @@
       </c>
       <c r="Z44" s="3"/>
     </row>
-    <row r="45" spans="2:50" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:50" x14ac:dyDescent="0.3">
       <c r="B45" s="65"/>
       <c r="C45" s="3">
         <v>1</v>
@@ -15742,7 +15742,7 @@
       </c>
       <c r="Z45" s="3"/>
     </row>
-    <row r="46" spans="2:50" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:50" x14ac:dyDescent="0.3">
       <c r="B46" s="65"/>
       <c r="C46" s="3">
         <v>1</v>
@@ -15815,7 +15815,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="47" spans="2:50" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:50" x14ac:dyDescent="0.3">
       <c r="B47" s="65"/>
       <c r="C47" s="3">
         <v>1</v>
@@ -15889,7 +15889,7 @@
       </c>
       <c r="Z47" s="3"/>
     </row>
-    <row r="48" spans="2:50" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:50" x14ac:dyDescent="0.3">
       <c r="B48" s="65"/>
       <c r="C48" s="3">
         <v>1</v>
@@ -15963,7 +15963,7 @@
       </c>
       <c r="Z48" s="3"/>
     </row>
-    <row r="49" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B49" s="65"/>
       <c r="C49" s="3">
         <v>1</v>
@@ -16036,7 +16036,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="50" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B50" s="65"/>
       <c r="C50" s="3">
         <v>1</v>
@@ -16109,7 +16109,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="51" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B51" s="65"/>
       <c r="C51" s="3">
         <v>1</v>
@@ -16182,7 +16182,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="52" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B52" s="65"/>
       <c r="C52" s="3">
         <v>1</v>
@@ -16255,7 +16255,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="53" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B53" s="65"/>
       <c r="C53" s="3">
         <v>1</v>
@@ -16328,7 +16328,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="54" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B54" s="65"/>
       <c r="C54" s="3">
         <v>1</v>
@@ -16401,7 +16401,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="55" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B55" s="65"/>
       <c r="C55" s="3">
         <v>1</v>
@@ -16474,7 +16474,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="56" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B56" s="65"/>
       <c r="C56" s="3">
         <v>1</v>
@@ -16547,7 +16547,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="57" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B57" s="65"/>
       <c r="C57" s="3">
         <v>1</v>
@@ -16620,7 +16620,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="58" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B58" s="65"/>
       <c r="C58" s="3">
         <v>1</v>
@@ -16693,7 +16693,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="59" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B59" s="65"/>
       <c r="C59" s="3">
         <v>1</v>
@@ -16766,7 +16766,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="60" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B60" s="65"/>
       <c r="C60" s="3">
         <v>1</v>
@@ -16839,7 +16839,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="61" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B61" s="65"/>
       <c r="C61" s="3">
         <v>1</v>
@@ -16912,7 +16912,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="62" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B62" s="65"/>
       <c r="C62" s="3">
         <v>1</v>
@@ -16985,7 +16985,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="63" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B63" s="65"/>
       <c r="C63" s="3">
         <v>1</v>
@@ -17058,7 +17058,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="64" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B64" s="65"/>
       <c r="C64" s="3">
         <v>1</v>
@@ -17131,7 +17131,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="65" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B65" s="65"/>
       <c r="C65" s="3">
         <v>1</v>
@@ -17204,7 +17204,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="66" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B66" s="65"/>
       <c r="C66" s="3">
         <v>1</v>
@@ -17277,7 +17277,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="67" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B67" s="65"/>
       <c r="C67" s="3">
         <v>1</v>
@@ -17350,7 +17350,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="68" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B68" s="65"/>
       <c r="C68" s="3">
         <v>1</v>
@@ -17423,7 +17423,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="69" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B69" s="67"/>
       <c r="C69" s="68">
         <v>1</v>
@@ -17516,51 +17516,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F461F9F-87D6-4C96-820F-6111A3E2F850}">
   <dimension ref="C4:S33"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="18.42578125" customWidth="1"/>
-    <col min="15" max="15" width="19.42578125" customWidth="1"/>
-    <col min="17" max="18" width="12.42578125" customWidth="1"/>
-    <col min="19" max="19" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.44140625" customWidth="1"/>
+    <col min="15" max="15" width="19.44140625" customWidth="1"/>
+    <col min="17" max="18" width="12.44140625" customWidth="1"/>
+    <col min="19" max="19" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="D5" s="119" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="5" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="D5" s="119" t="s">
+      <c r="E5" s="120" t="s">
         <v>133</v>
       </c>
-      <c r="E5" s="120" t="s">
+      <c r="F5" s="119" t="s">
         <v>134</v>
       </c>
-      <c r="F5" s="119" t="s">
-        <v>135</v>
-      </c>
       <c r="H5" s="119" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I5" s="120" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J5" s="119" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K5" s="119"/>
       <c r="L5" s="119" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="M5" s="120" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="6" spans="3:19" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="3:19" x14ac:dyDescent="0.3">
       <c r="D6" s="45">
         <v>0</v>
       </c>
@@ -17568,7 +17568,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="45" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H6" s="45">
         <v>0</v>
@@ -17587,16 +17587,16 @@
         <v>0</v>
       </c>
       <c r="Q6" s="45" t="s">
+        <v>189</v>
+      </c>
+      <c r="R6" s="45" t="s">
         <v>190</v>
       </c>
-      <c r="R6" s="45" t="s">
-        <v>191</v>
-      </c>
       <c r="S6" s="45" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="7" spans="3:19" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="3:19" x14ac:dyDescent="0.3">
       <c r="D7" s="45">
         <v>0</v>
       </c>
@@ -17604,7 +17604,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="45" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H7" s="45">
         <v>0</v>
@@ -17623,7 +17623,7 @@
         <v>0</v>
       </c>
       <c r="O7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="Q7" s="45">
         <v>0</v>
@@ -17632,10 +17632,10 @@
         <v>0</v>
       </c>
       <c r="S7" s="45" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="8" spans="3:19" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="8" spans="3:19" x14ac:dyDescent="0.3">
       <c r="D8" s="45">
         <v>1</v>
       </c>
@@ -17643,7 +17643,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="45" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H8" s="45">
         <v>0</v>
@@ -17662,7 +17662,7 @@
         <v>0</v>
       </c>
       <c r="O8" s="118" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Q8" s="45">
         <v>0</v>
@@ -17671,10 +17671,10 @@
         <v>1</v>
       </c>
       <c r="S8" s="45" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="9" spans="3:19" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="9" spans="3:19" x14ac:dyDescent="0.3">
       <c r="D9" s="45">
         <v>1</v>
       </c>
@@ -17682,7 +17682,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="45" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H9" s="45">
         <v>0</v>
@@ -17707,10 +17707,10 @@
         <v>0</v>
       </c>
       <c r="S9" s="45" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="10" spans="3:19" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="10" spans="3:19" x14ac:dyDescent="0.3">
       <c r="H10" s="45">
         <v>1</v>
       </c>
@@ -17734,10 +17734,10 @@
         <v>1</v>
       </c>
       <c r="S10" s="45" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="11" spans="3:19" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="11" spans="3:19" x14ac:dyDescent="0.3">
       <c r="H11" s="45">
         <v>1</v>
       </c>
@@ -17755,7 +17755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:19" x14ac:dyDescent="0.3">
       <c r="H12" s="45">
         <v>1</v>
       </c>
@@ -17767,13 +17767,13 @@
       </c>
       <c r="K12" s="45"/>
       <c r="L12" s="45" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="M12" s="45" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="13" spans="3:19" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="3:19" x14ac:dyDescent="0.3">
       <c r="H13" s="45">
         <v>1</v>
       </c>
@@ -17785,53 +17785,53 @@
       </c>
       <c r="K13" s="45"/>
       <c r="L13" s="45" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="M13" s="45" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="15" spans="3:19" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="3:19" x14ac:dyDescent="0.3">
       <c r="Q15" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="16" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="16" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="Q16">
-        <v>0</v>
-      </c>
-      <c r="R16" t="s">
+    <row r="17" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q17">
+        <v>1</v>
+      </c>
+      <c r="R17" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="17" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
+    <row r="18" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="D18" s="240" t="s">
         <v>175</v>
       </c>
-      <c r="Q17">
-        <v>1</v>
-      </c>
-      <c r="R17" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="18" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="D18" s="239" t="s">
-        <v>176</v>
-      </c>
-      <c r="E18" s="239"/>
-      <c r="G18" s="239" t="s">
-        <v>179</v>
-      </c>
-      <c r="H18" s="239"/>
+      <c r="E18" s="240"/>
+      <c r="G18" s="240" t="s">
+        <v>178</v>
+      </c>
+      <c r="H18" s="240"/>
       <c r="Q18">
         <v>2</v>
       </c>
       <c r="R18" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="19" spans="3:18" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="19" spans="3:18" x14ac:dyDescent="0.3">
       <c r="D19" s="45">
         <v>0</v>
       </c>
@@ -17848,38 +17848,38 @@
         <v>3</v>
       </c>
       <c r="R19" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="20" spans="3:18" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="20" spans="3:18" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
+        <v>176</v>
+      </c>
+      <c r="E20" t="s">
         <v>177</v>
       </c>
-      <c r="E20" t="s">
-        <v>178</v>
-      </c>
       <c r="G20" t="s">
+        <v>179</v>
+      </c>
+      <c r="H20" t="s">
         <v>180</v>
       </c>
-      <c r="H20" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="23" spans="3:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C23" s="45" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D23" s="119" t="s">
         <v>18</v>
       </c>
       <c r="E23" s="120" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F23" s="119" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="24" spans="3:18" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="24" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C24" s="45">
         <v>0</v>
       </c>
@@ -17890,19 +17890,19 @@
         <v>0</v>
       </c>
       <c r="F24" s="45" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L24" t="s">
         <v>18</v>
       </c>
       <c r="M24" t="s">
+        <v>185</v>
+      </c>
+      <c r="N24" t="s">
         <v>186</v>
       </c>
-      <c r="N24" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="25" spans="3:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C25" s="45">
         <v>0</v>
       </c>
@@ -17913,10 +17913,10 @@
         <v>1</v>
       </c>
       <c r="F25" s="45" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="26" spans="3:18" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="26" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C26" s="45">
         <v>0</v>
       </c>
@@ -17927,10 +17927,10 @@
         <v>0</v>
       </c>
       <c r="F26" s="45" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="27" spans="3:18" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="27" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C27" s="45">
         <v>0</v>
       </c>
@@ -17941,13 +17941,13 @@
         <v>1</v>
       </c>
       <c r="F27" s="45" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="28" spans="3:18" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="28" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C28" s="45"/>
     </row>
-    <row r="29" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C29" s="45">
         <v>1</v>
       </c>
@@ -17958,10 +17958,10 @@
         <v>0</v>
       </c>
       <c r="F29" s="45" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="30" spans="3:18" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="30" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C30" s="45">
         <v>1</v>
       </c>
@@ -17972,10 +17972,10 @@
         <v>1</v>
       </c>
       <c r="F30" s="45" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="31" spans="3:18" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="31" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C31" s="45">
         <v>1</v>
       </c>
@@ -17989,7 +17989,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C32" s="45">
         <v>1</v>
       </c>
@@ -18003,7 +18003,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C33" s="45"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed GPREG Controller and created Test
</commit_message>
<xml_diff>
--- a/Documentation/CPU_DOC.xlsx
+++ b/Documentation/CPU_DOC.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\CPU_8Bit\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Desktop\CPU_8Bit\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1C45EDB-9989-46B7-AF95-1DB1207B6BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB7415A8-CEF0-40B8-ACC6-F315A2A81A2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{5BA4E079-EFAB-4B55-B322-C6522B3056FF}"/>
+    <workbookView xWindow="38280" yWindow="3585" windowWidth="29040" windowHeight="16440" xr2:uid="{5BA4E079-EFAB-4B55-B322-C6522B3056FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Control-Unit" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="210">
   <si>
     <t>1=Read</t>
   </si>
@@ -650,6 +650,24 @@
   </si>
   <si>
     <t>Bit_6</t>
+  </si>
+  <si>
+    <t>RAM -&gt; REG</t>
+  </si>
+  <si>
+    <t>REG -&gt; RAM</t>
+  </si>
+  <si>
+    <t>REG -&gt; ACC</t>
+  </si>
+  <si>
+    <t>ACC -&gt; REG</t>
+  </si>
+  <si>
+    <t>RAM -&gt; ACC</t>
+  </si>
+  <si>
+    <t>ACC -&gt; RAM</t>
   </si>
 </sst>
 </file>
@@ -713,7 +731,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="21">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -831,6 +849,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1658,7 +1682,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="250">
+  <cellXfs count="251">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2371,9 +2395,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2443,7 +2470,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2741,34 +2768,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0373F33-972A-4E8D-B1CE-9C5EF0708B27}">
   <dimension ref="B2:AI157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AC12" sqref="AC12"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.5546875" customWidth="1"/>
-    <col min="5" max="5" width="8.44140625" style="45" customWidth="1"/>
-    <col min="6" max="6" width="22.44140625" style="45" customWidth="1"/>
-    <col min="7" max="7" width="32.33203125" style="45" customWidth="1"/>
-    <col min="8" max="8" width="6.109375" style="21" customWidth="1"/>
-    <col min="9" max="11" width="11.33203125" style="21" customWidth="1"/>
-    <col min="12" max="12" width="11.33203125" customWidth="1"/>
-    <col min="13" max="19" width="4.44140625" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" style="45" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" style="45" customWidth="1"/>
+    <col min="7" max="7" width="32.28515625" style="45" customWidth="1"/>
+    <col min="8" max="8" width="6.140625" style="21" customWidth="1"/>
+    <col min="9" max="11" width="11.28515625" style="21" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" customWidth="1"/>
+    <col min="13" max="19" width="4.42578125" customWidth="1"/>
     <col min="20" max="21" width="16" customWidth="1"/>
-    <col min="22" max="25" width="13.109375" customWidth="1"/>
-    <col min="30" max="30" width="21.88671875" style="45" customWidth="1"/>
+    <col min="22" max="25" width="13.140625" customWidth="1"/>
+    <col min="30" max="30" width="21.85546875" style="45" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="3"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="4" spans="2:35" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="2:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="208" t="s">
         <v>118</v>
       </c>
@@ -2802,7 +2829,7 @@
       <c r="AC5" s="223"/>
       <c r="AD5" s="206"/>
     </row>
-    <row r="6" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:35" x14ac:dyDescent="0.25">
       <c r="C6" s="211"/>
       <c r="D6" s="212"/>
       <c r="E6" s="212"/>
@@ -2869,7 +2896,7 @@
       <c r="AH6" s="4"/>
       <c r="AI6" s="2"/>
     </row>
-    <row r="7" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:35" x14ac:dyDescent="0.25">
       <c r="C7" s="214"/>
       <c r="D7" s="215"/>
       <c r="E7" s="215"/>
@@ -2925,7 +2952,7 @@
       <c r="AG7" s="3"/>
       <c r="AH7" s="2"/>
     </row>
-    <row r="8" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:35" x14ac:dyDescent="0.25">
       <c r="C8" s="216"/>
       <c r="D8" s="217"/>
       <c r="E8" s="217"/>
@@ -2971,7 +2998,7 @@
       <c r="AG8" s="123"/>
       <c r="AH8" s="2"/>
     </row>
-    <row r="9" spans="2:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="45" t="s">
         <v>184</v>
       </c>
@@ -3068,7 +3095,7 @@
       <c r="AG9" s="2"/>
       <c r="AH9" s="2"/>
     </row>
-    <row r="10" spans="2:35" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:35" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B10" s="45" t="str">
         <f>DEC2HEX(D10)</f>
         <v>0</v>
@@ -3166,7 +3193,7 @@
       <c r="AH10" s="2"/>
       <c r="AI10" s="2"/>
     </row>
-    <row r="11" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B11" s="45" t="str">
         <f t="shared" ref="B11:B74" si="0">DEC2HEX(D11)</f>
         <v>1</v>
@@ -3264,7 +3291,7 @@
       <c r="AH11" s="2"/>
       <c r="AI11" s="2"/>
     </row>
-    <row r="12" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B12" s="45" t="str">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -3362,7 +3389,7 @@
       <c r="AH12" s="2"/>
       <c r="AI12" s="2"/>
     </row>
-    <row r="13" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B13" s="45" t="str">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -3460,7 +3487,7 @@
       <c r="AH13" s="2"/>
       <c r="AI13" s="2"/>
     </row>
-    <row r="14" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B14" s="45" t="str">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -3558,7 +3585,7 @@
       <c r="AH14" s="2"/>
       <c r="AI14" s="2"/>
     </row>
-    <row r="15" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B15" s="45" t="str">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -3656,7 +3683,7 @@
       <c r="AH15" s="2"/>
       <c r="AI15" s="2"/>
     </row>
-    <row r="16" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B16" s="45" t="str">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -3754,7 +3781,7 @@
       <c r="AH16" s="2"/>
       <c r="AI16" s="2"/>
     </row>
-    <row r="17" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B17" s="45" t="str">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -3852,7 +3879,7 @@
       <c r="AH17" s="2"/>
       <c r="AI17" s="2"/>
     </row>
-    <row r="18" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B18" s="45" t="str">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -3950,7 +3977,7 @@
       <c r="AH18" s="2"/>
       <c r="AI18" s="2"/>
     </row>
-    <row r="19" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B19" s="45" t="str">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -4048,7 +4075,7 @@
       <c r="AH19" s="2"/>
       <c r="AI19" s="2"/>
     </row>
-    <row r="20" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B20" s="45" t="str">
         <f t="shared" si="0"/>
         <v>A</v>
@@ -4146,7 +4173,7 @@
       <c r="AH20" s="2"/>
       <c r="AI20" s="2"/>
     </row>
-    <row r="21" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B21" s="45" t="str">
         <f t="shared" si="0"/>
         <v>B</v>
@@ -4244,7 +4271,7 @@
       <c r="AH21" s="2"/>
       <c r="AI21" s="2"/>
     </row>
-    <row r="22" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B22" s="45" t="str">
         <f t="shared" si="0"/>
         <v>C</v>
@@ -4342,7 +4369,7 @@
       <c r="AH22" s="2"/>
       <c r="AI22" s="2"/>
     </row>
-    <row r="23" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B23" s="45" t="str">
         <f t="shared" si="0"/>
         <v>D</v>
@@ -4440,7 +4467,7 @@
       <c r="AH23" s="2"/>
       <c r="AI23" s="2"/>
     </row>
-    <row r="24" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B24" s="45" t="str">
         <f t="shared" si="0"/>
         <v>E</v>
@@ -4522,7 +4549,7 @@
       <c r="AH24" s="2"/>
       <c r="AI24" s="2"/>
     </row>
-    <row r="25" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B25" s="45" t="str">
         <f t="shared" si="0"/>
         <v>F</v>
@@ -4604,7 +4631,7 @@
       <c r="AH25" s="2"/>
       <c r="AI25" s="2"/>
     </row>
-    <row r="26" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B26" s="45" t="str">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -4670,7 +4697,7 @@
       <c r="AH26" s="2"/>
       <c r="AI26" s="2"/>
     </row>
-    <row r="27" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B27" s="45" t="str">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -4768,7 +4795,7 @@
       <c r="AH27" s="2"/>
       <c r="AI27" s="2"/>
     </row>
-    <row r="28" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B28" s="45" t="str">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -4850,7 +4877,7 @@
       <c r="AH28" s="2"/>
       <c r="AI28" s="2"/>
     </row>
-    <row r="29" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B29" s="45" t="str">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -4933,7 +4960,7 @@
       <c r="AH29" s="2"/>
       <c r="AI29" s="2"/>
     </row>
-    <row r="30" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B30" s="45" t="str">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -4955,8 +4982,8 @@
       <c r="I30" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="J30" s="21">
-        <v>1</v>
+      <c r="J30" s="21" t="s">
+        <v>98</v>
       </c>
       <c r="K30" s="21" t="s">
         <v>98</v>
@@ -4999,7 +5026,7 @@
       <c r="AH30" s="2"/>
       <c r="AI30" s="2"/>
     </row>
-    <row r="31" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B31" s="45" t="str">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -5021,8 +5048,8 @@
       <c r="I31" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="J31" s="21">
-        <v>1</v>
+      <c r="J31" s="21" t="s">
+        <v>98</v>
       </c>
       <c r="K31" s="21" t="s">
         <v>98</v>
@@ -5065,7 +5092,7 @@
       <c r="AH31" s="2"/>
       <c r="AI31" s="2"/>
     </row>
-    <row r="32" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B32" s="45" t="str">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -5087,8 +5114,8 @@
       <c r="I32" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="J32" s="21">
-        <v>1</v>
+      <c r="J32" s="21" t="s">
+        <v>98</v>
       </c>
       <c r="K32" s="21" t="s">
         <v>98</v>
@@ -5131,7 +5158,7 @@
       <c r="AH32" s="2"/>
       <c r="AI32" s="2"/>
     </row>
-    <row r="33" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B33" s="45" t="str">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -5153,8 +5180,8 @@
       <c r="I33" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="J33" s="21">
-        <v>1</v>
+      <c r="J33" s="21" t="s">
+        <v>98</v>
       </c>
       <c r="K33" s="21" t="s">
         <v>98</v>
@@ -5197,7 +5224,7 @@
       <c r="AH33" s="2"/>
       <c r="AI33" s="2"/>
     </row>
-    <row r="34" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B34" s="45" t="str">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -5219,8 +5246,8 @@
       <c r="I34" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="J34" s="21">
-        <v>1</v>
+      <c r="J34" s="21" t="s">
+        <v>98</v>
       </c>
       <c r="K34" s="21" t="s">
         <v>98</v>
@@ -5263,7 +5290,7 @@
       <c r="AH34" s="2"/>
       <c r="AI34" s="2"/>
     </row>
-    <row r="35" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B35" s="45" t="str">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -5346,7 +5373,7 @@
       <c r="AH35" s="2"/>
       <c r="AI35" s="2"/>
     </row>
-    <row r="36" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B36" s="45" t="str">
         <f t="shared" si="0"/>
         <v>1A</v>
@@ -5429,7 +5456,7 @@
       <c r="AH36" s="2"/>
       <c r="AI36" s="2"/>
     </row>
-    <row r="37" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B37" s="45" t="str">
         <f t="shared" si="0"/>
         <v>1B</v>
@@ -5512,7 +5539,7 @@
       <c r="AH37" s="2"/>
       <c r="AI37" s="2"/>
     </row>
-    <row r="38" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B38" s="45" t="str">
         <f t="shared" si="0"/>
         <v>1C</v>
@@ -5578,7 +5605,7 @@
       <c r="AH38" s="2"/>
       <c r="AI38" s="2"/>
     </row>
-    <row r="39" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B39" s="45" t="str">
         <f t="shared" si="0"/>
         <v>1D</v>
@@ -5600,8 +5627,8 @@
       <c r="I39" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="J39" s="21">
-        <v>1</v>
+      <c r="J39" s="21" t="s">
+        <v>98</v>
       </c>
       <c r="K39" s="21" t="s">
         <v>98</v>
@@ -5612,39 +5639,71 @@
       <c r="M39" s="165">
         <v>1</v>
       </c>
-      <c r="N39" s="190"/>
-      <c r="O39" s="190"/>
-      <c r="P39" s="190"/>
-      <c r="Q39" s="190"/>
-      <c r="R39" s="191"/>
-      <c r="S39" s="37"/>
-      <c r="T39" s="192"/>
-      <c r="U39" s="35"/>
-      <c r="V39" s="192"/>
-      <c r="W39" s="192"/>
-      <c r="X39" s="192"/>
-      <c r="Y39" s="35"/>
-      <c r="Z39" s="192"/>
-      <c r="AA39" s="35"/>
-      <c r="AB39" s="192"/>
-      <c r="AC39" s="193"/>
+      <c r="N39" s="190">
+        <v>0</v>
+      </c>
+      <c r="O39" s="190">
+        <v>0</v>
+      </c>
+      <c r="P39" s="190">
+        <v>0</v>
+      </c>
+      <c r="Q39" s="190">
+        <v>0</v>
+      </c>
+      <c r="R39" s="190">
+        <v>0</v>
+      </c>
+      <c r="S39" s="190">
+        <v>0</v>
+      </c>
+      <c r="T39" s="192">
+        <v>1</v>
+      </c>
+      <c r="U39" s="35">
+        <v>1</v>
+      </c>
+      <c r="V39" s="192">
+        <v>0</v>
+      </c>
+      <c r="W39" s="192">
+        <v>0</v>
+      </c>
+      <c r="X39" s="192">
+        <v>0</v>
+      </c>
+      <c r="Y39" s="35">
+        <v>1</v>
+      </c>
+      <c r="Z39" s="192">
+        <v>0</v>
+      </c>
+      <c r="AA39" s="35">
+        <v>0</v>
+      </c>
+      <c r="AB39" s="192">
+        <v>0</v>
+      </c>
+      <c r="AC39" s="193">
+        <v>1</v>
+      </c>
       <c r="AD39" s="168" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>88C0</v>
       </c>
       <c r="AE39" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>00</v>
+        <v>88</v>
       </c>
       <c r="AF39" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>00</v>
+        <v>C0</v>
       </c>
       <c r="AG39" s="3"/>
       <c r="AH39" s="2"/>
       <c r="AI39" s="2"/>
     </row>
-    <row r="40" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B40" s="45" t="str">
         <f t="shared" si="0"/>
         <v>1E</v>
@@ -5666,8 +5725,8 @@
       <c r="I40" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="J40" s="21">
-        <v>1</v>
+      <c r="J40" s="21" t="s">
+        <v>98</v>
       </c>
       <c r="K40" s="21" t="s">
         <v>98</v>
@@ -5678,39 +5737,71 @@
       <c r="M40" s="165">
         <v>1</v>
       </c>
-      <c r="N40" s="190"/>
-      <c r="O40" s="190"/>
-      <c r="P40" s="190"/>
-      <c r="Q40" s="190"/>
-      <c r="R40" s="191"/>
-      <c r="S40" s="37"/>
-      <c r="T40" s="192"/>
-      <c r="U40" s="35"/>
-      <c r="V40" s="192"/>
-      <c r="W40" s="192"/>
-      <c r="X40" s="192"/>
-      <c r="Y40" s="35"/>
-      <c r="Z40" s="192"/>
-      <c r="AA40" s="35"/>
-      <c r="AB40" s="192"/>
-      <c r="AC40" s="193"/>
+      <c r="N40" s="190">
+        <v>0</v>
+      </c>
+      <c r="O40" s="190">
+        <v>0</v>
+      </c>
+      <c r="P40" s="190">
+        <v>0</v>
+      </c>
+      <c r="Q40" s="190">
+        <v>0</v>
+      </c>
+      <c r="R40" s="190">
+        <v>0</v>
+      </c>
+      <c r="S40" s="190">
+        <v>0</v>
+      </c>
+      <c r="T40" s="192">
+        <v>1</v>
+      </c>
+      <c r="U40" s="35">
+        <v>1</v>
+      </c>
+      <c r="V40" s="192">
+        <v>0</v>
+      </c>
+      <c r="W40" s="192">
+        <v>1</v>
+      </c>
+      <c r="X40" s="192">
+        <v>0</v>
+      </c>
+      <c r="Y40" s="35">
+        <v>1</v>
+      </c>
+      <c r="Z40" s="192">
+        <v>0</v>
+      </c>
+      <c r="AA40" s="35">
+        <v>0</v>
+      </c>
+      <c r="AB40" s="192">
+        <v>1</v>
+      </c>
+      <c r="AC40" s="193">
+        <v>0</v>
+      </c>
       <c r="AD40" s="168" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>4AC0</v>
       </c>
       <c r="AE40" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>00</v>
+        <v>4A</v>
       </c>
       <c r="AF40" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>00</v>
+        <v>C0</v>
       </c>
       <c r="AG40" s="3"/>
       <c r="AH40" s="2"/>
       <c r="AI40" s="2"/>
     </row>
-    <row r="41" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B41" s="45" t="str">
         <f t="shared" si="0"/>
         <v>1F</v>
@@ -5753,7 +5844,9 @@
       <c r="S41" s="37"/>
       <c r="T41" s="192"/>
       <c r="U41" s="35"/>
-      <c r="V41" s="192"/>
+      <c r="V41" s="192">
+        <v>0</v>
+      </c>
       <c r="W41" s="192"/>
       <c r="X41" s="192"/>
       <c r="Y41" s="35"/>
@@ -5777,7 +5870,7 @@
       <c r="AH41" s="2"/>
       <c r="AI41" s="2"/>
     </row>
-    <row r="42" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B42" s="45" t="str">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -5820,7 +5913,9 @@
       <c r="S42" s="37"/>
       <c r="T42" s="191"/>
       <c r="U42" s="37"/>
-      <c r="V42" s="191"/>
+      <c r="V42" s="192">
+        <v>0</v>
+      </c>
       <c r="W42" s="191"/>
       <c r="X42" s="191"/>
       <c r="Y42" s="37"/>
@@ -5841,7 +5936,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="43" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B43" s="45" t="str">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -5864,8 +5959,8 @@
       <c r="I43" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="J43" s="21">
-        <v>1</v>
+      <c r="J43" s="21" t="s">
+        <v>98</v>
       </c>
       <c r="K43" s="21" t="s">
         <v>98</v>
@@ -5884,7 +5979,9 @@
       <c r="S43" s="37"/>
       <c r="T43" s="191"/>
       <c r="U43" s="37"/>
-      <c r="V43" s="191"/>
+      <c r="V43" s="192">
+        <v>0</v>
+      </c>
       <c r="W43" s="191"/>
       <c r="X43" s="191"/>
       <c r="Y43" s="37"/>
@@ -5905,7 +6002,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="44" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B44" s="45" t="str">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -5926,7 +6023,7 @@
       </c>
       <c r="H44" s="16"/>
       <c r="I44" s="205" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J44" s="21" t="s">
         <v>98</v>
@@ -5948,7 +6045,9 @@
       <c r="S44" s="37"/>
       <c r="T44" s="191"/>
       <c r="U44" s="37"/>
-      <c r="V44" s="191"/>
+      <c r="V44" s="192">
+        <v>0</v>
+      </c>
       <c r="W44" s="191"/>
       <c r="X44" s="191"/>
       <c r="Y44" s="37"/>
@@ -5957,11 +6056,11 @@
       <c r="AB44" s="191"/>
       <c r="AC44" s="194"/>
       <c r="AD44" s="168" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(BIN2HEX(_xlfn.CONCAT(AC44,AB44,AA44,Z44)), BIN2HEX(_xlfn.CONCAT(Y44,X44,W44,V44)), BIN2HEX(_xlfn.CONCAT(U44,T44,S44,R44)), BIN2HEX(_xlfn.CONCAT(Q44,P44,O44,N44)))</f>
         <v>0000</v>
       </c>
       <c r="AE44" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT(BIN2HEX(_xlfn.CONCAT(AC44,AB44,AA44,Z44)), BIN2HEX(_xlfn.CONCAT(Y44,X44,W44,V44)))</f>
         <v>00</v>
       </c>
       <c r="AF44" s="2" t="str">
@@ -5969,7 +6068,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="45" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B45" s="45" t="str">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -6004,36 +6103,68 @@
       <c r="M45" s="165">
         <v>1</v>
       </c>
-      <c r="N45" s="191"/>
-      <c r="O45" s="191"/>
-      <c r="P45" s="191"/>
-      <c r="Q45" s="191"/>
-      <c r="R45" s="191"/>
-      <c r="S45" s="37"/>
-      <c r="T45" s="191"/>
-      <c r="U45" s="37"/>
-      <c r="V45" s="191"/>
-      <c r="W45" s="191"/>
-      <c r="X45" s="191"/>
-      <c r="Y45" s="37"/>
-      <c r="Z45" s="191"/>
-      <c r="AA45" s="37"/>
-      <c r="AB45" s="191"/>
-      <c r="AC45" s="194"/>
+      <c r="N45" s="190">
+        <v>0</v>
+      </c>
+      <c r="O45" s="190">
+        <v>0</v>
+      </c>
+      <c r="P45" s="190">
+        <v>0</v>
+      </c>
+      <c r="Q45" s="190">
+        <v>0</v>
+      </c>
+      <c r="R45" s="190">
+        <v>0</v>
+      </c>
+      <c r="S45" s="190">
+        <v>0</v>
+      </c>
+      <c r="T45" s="191">
+        <v>0</v>
+      </c>
+      <c r="U45" s="37">
+        <v>1</v>
+      </c>
+      <c r="V45" s="192">
+        <v>0</v>
+      </c>
+      <c r="W45" s="191">
+        <v>0</v>
+      </c>
+      <c r="X45" s="191">
+        <v>0</v>
+      </c>
+      <c r="Y45" s="37">
+        <v>1</v>
+      </c>
+      <c r="Z45" s="191">
+        <v>1</v>
+      </c>
+      <c r="AA45" s="37">
+        <v>0</v>
+      </c>
+      <c r="AB45" s="191">
+        <v>0</v>
+      </c>
+      <c r="AC45" s="194">
+        <v>0</v>
+      </c>
       <c r="AD45" s="168" t="str">
-        <f t="shared" si="1"/>
-        <v>0000</v>
+        <f>_xlfn.CONCAT(BIN2HEX(_xlfn.CONCAT(AC45,AB45,AA45,Z45)), BIN2HEX(_xlfn.CONCAT(Y45,X45,W45,V45)), BIN2HEX(_xlfn.CONCAT(U45,T45,S45,R45)), BIN2HEX(_xlfn.CONCAT(Q45,P45,O45,N45)))</f>
+        <v>1880</v>
       </c>
       <c r="AE45" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>00</v>
+        <f>_xlfn.CONCAT(BIN2HEX(_xlfn.CONCAT(AC45,AB45,AA45,Z45)), BIN2HEX(_xlfn.CONCAT(Y45,X45,W45,V45)))</f>
+        <v>18</v>
       </c>
       <c r="AF45" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>00</v>
-      </c>
-    </row>
-    <row r="46" spans="2:35" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B46" s="45" t="str">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -6054,7 +6185,7 @@
       </c>
       <c r="H46" s="16"/>
       <c r="I46" s="21" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J46" s="21" t="s">
         <v>98</v>
@@ -6068,36 +6199,68 @@
       <c r="M46" s="165">
         <v>1</v>
       </c>
-      <c r="N46" s="191"/>
-      <c r="O46" s="191"/>
-      <c r="P46" s="191"/>
-      <c r="Q46" s="191"/>
-      <c r="R46" s="191"/>
-      <c r="S46" s="37"/>
-      <c r="T46" s="191"/>
-      <c r="U46" s="37"/>
-      <c r="V46" s="191"/>
-      <c r="W46" s="191"/>
-      <c r="X46" s="191"/>
-      <c r="Y46" s="37"/>
-      <c r="Z46" s="191"/>
-      <c r="AA46" s="37"/>
-      <c r="AB46" s="191"/>
-      <c r="AC46" s="194"/>
+      <c r="N46" s="190">
+        <v>0</v>
+      </c>
+      <c r="O46" s="190">
+        <v>0</v>
+      </c>
+      <c r="P46" s="190">
+        <v>0</v>
+      </c>
+      <c r="Q46" s="190">
+        <v>0</v>
+      </c>
+      <c r="R46" s="190">
+        <v>0</v>
+      </c>
+      <c r="S46" s="190">
+        <v>0</v>
+      </c>
+      <c r="T46" s="191">
+        <v>0</v>
+      </c>
+      <c r="U46" s="37">
+        <v>1</v>
+      </c>
+      <c r="V46" s="192">
+        <v>0</v>
+      </c>
+      <c r="W46" s="191">
+        <v>1</v>
+      </c>
+      <c r="X46" s="191">
+        <v>0</v>
+      </c>
+      <c r="Y46" s="37">
+        <v>1</v>
+      </c>
+      <c r="Z46" s="191">
+        <v>1</v>
+      </c>
+      <c r="AA46" s="37">
+        <v>0</v>
+      </c>
+      <c r="AB46" s="191">
+        <v>1</v>
+      </c>
+      <c r="AC46" s="194">
+        <v>0</v>
+      </c>
       <c r="AD46" s="168" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>5A80</v>
       </c>
       <c r="AE46" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>00</v>
+        <v>5A</v>
       </c>
       <c r="AF46" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>00</v>
-      </c>
-    </row>
-    <row r="47" spans="2:35" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="47" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B47" s="45" t="str">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -6178,7 +6341,7 @@
         <v>C0</v>
       </c>
     </row>
-    <row r="48" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B48" s="45" t="str">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -6259,7 +6422,7 @@
         <v>C0</v>
       </c>
     </row>
-    <row r="49" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B49" s="45" t="str">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -6340,7 +6503,7 @@
         <v>C0</v>
       </c>
     </row>
-    <row r="50" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B50" s="45" t="str">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -6421,7 +6584,7 @@
         <v>C0</v>
       </c>
     </row>
-    <row r="51" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B51" s="45" t="str">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -6502,7 +6665,7 @@
         <v>C0</v>
       </c>
     </row>
-    <row r="52" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B52" s="45" t="str">
         <f t="shared" si="0"/>
         <v>2A</v>
@@ -6583,7 +6746,7 @@
         <v>C0</v>
       </c>
     </row>
-    <row r="53" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B53" s="45" t="str">
         <f t="shared" si="0"/>
         <v>2B</v>
@@ -6681,7 +6844,7 @@
         <v>A8</v>
       </c>
     </row>
-    <row r="54" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B54" s="45" t="str">
         <f t="shared" si="0"/>
         <v>2C</v>
@@ -6779,7 +6942,7 @@
         <v>A8</v>
       </c>
     </row>
-    <row r="55" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B55" s="45" t="str">
         <f t="shared" si="0"/>
         <v>2D</v>
@@ -6877,7 +7040,7 @@
         <v>A8</v>
       </c>
     </row>
-    <row r="56" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B56" s="45" t="str">
         <f t="shared" si="0"/>
         <v>2E</v>
@@ -6975,7 +7138,7 @@
         <v>A8</v>
       </c>
     </row>
-    <row r="57" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B57" s="45" t="str">
         <f t="shared" si="0"/>
         <v>2F</v>
@@ -7073,7 +7236,7 @@
         <v>A8</v>
       </c>
     </row>
-    <row r="58" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B58" s="45" t="str">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -7171,7 +7334,7 @@
         <v>A8</v>
       </c>
     </row>
-    <row r="59" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B59" s="45" t="str">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -7269,7 +7432,7 @@
         <v>A8</v>
       </c>
     </row>
-    <row r="60" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B60" s="45" t="str">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -7350,7 +7513,7 @@
         <v>C0</v>
       </c>
     </row>
-    <row r="61" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B61" s="45" t="str">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -7431,7 +7594,7 @@
         <v>C0</v>
       </c>
     </row>
-    <row r="62" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B62" s="45" t="str">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -7512,7 +7675,7 @@
         <v>C0</v>
       </c>
     </row>
-    <row r="63" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B63" s="45" t="str">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -7576,7 +7739,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="64" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B64" s="45" t="str">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -7672,7 +7835,7 @@
         <v>C0</v>
       </c>
     </row>
-    <row r="65" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B65" s="45" t="str">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -7753,7 +7916,7 @@
         <v>C0</v>
       </c>
     </row>
-    <row r="66" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B66" s="45" t="str">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -7834,7 +7997,7 @@
         <v>C0</v>
       </c>
     </row>
-    <row r="67" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B67" s="45" t="str">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -7915,7 +8078,7 @@
         <v>C0</v>
       </c>
     </row>
-    <row r="68" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B68" s="45" t="str">
         <f t="shared" si="0"/>
         <v>3A</v>
@@ -7996,7 +8159,7 @@
         <v>C0</v>
       </c>
     </row>
-    <row r="69" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B69" s="45" t="str">
         <f t="shared" si="0"/>
         <v>3B</v>
@@ -8077,7 +8240,7 @@
         <v>C0</v>
       </c>
     </row>
-    <row r="70" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B70" s="45" t="str">
         <f t="shared" si="0"/>
         <v>3C</v>
@@ -8158,7 +8321,7 @@
         <v>C0</v>
       </c>
     </row>
-    <row r="71" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B71" s="45" t="str">
         <f t="shared" si="0"/>
         <v>3D</v>
@@ -8239,7 +8402,7 @@
         <v>C0</v>
       </c>
     </row>
-    <row r="72" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B72" s="45" t="str">
         <f t="shared" si="0"/>
         <v>3E</v>
@@ -8319,7 +8482,7 @@
         <v>C0</v>
       </c>
     </row>
-    <row r="73" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B73" s="45" t="str">
         <f t="shared" si="0"/>
         <v>3F</v>
@@ -8332,7 +8495,7 @@
         <v>63</v>
       </c>
       <c r="E73" s="204"/>
-      <c r="F73" s="158" t="s">
+      <c r="F73" s="250" t="s">
         <v>159</v>
       </c>
       <c r="G73" s="159" t="s">
@@ -8415,7 +8578,7 @@
         <v>FF</v>
       </c>
     </row>
-    <row r="74" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B74" s="45" t="str">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -8500,7 +8663,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="75" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B75" s="45" t="str">
         <f t="shared" ref="B75:B137" si="5">DEC2HEX(D75)</f>
         <v>41</v>
@@ -8585,7 +8748,7 @@
         <v>C0</v>
       </c>
     </row>
-    <row r="76" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B76" s="45" t="str">
         <f t="shared" si="5"/>
         <v>42</v>
@@ -8670,7 +8833,7 @@
         <v>C0</v>
       </c>
     </row>
-    <row r="77" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B77" s="45" t="str">
         <f t="shared" si="5"/>
         <v>43</v>
@@ -8755,7 +8918,7 @@
         <v>C0</v>
       </c>
     </row>
-    <row r="78" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B78" s="45" t="str">
         <f t="shared" si="5"/>
         <v>44</v>
@@ -8816,7 +8979,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="79" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B79" s="45" t="str">
         <f t="shared" si="5"/>
         <v>45</v>
@@ -8899,7 +9062,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="80" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B80" s="45" t="str">
         <f t="shared" si="5"/>
         <v>46</v>
@@ -8954,7 +9117,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="81" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B81" s="45" t="str">
         <f t="shared" si="5"/>
         <v>47</v>
@@ -9009,7 +9172,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="82" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B82" s="45" t="str">
         <f t="shared" si="5"/>
         <v>48</v>
@@ -9064,7 +9227,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="83" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B83" s="45" t="str">
         <f t="shared" si="5"/>
         <v>49</v>
@@ -9118,7 +9281,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="84" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B84" s="45" t="str">
         <f t="shared" si="5"/>
         <v>4A</v>
@@ -9172,7 +9335,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="85" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B85" s="45" t="str">
         <f t="shared" si="5"/>
         <v>4B</v>
@@ -9226,7 +9389,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="86" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B86" s="45" t="str">
         <f t="shared" si="5"/>
         <v>4C</v>
@@ -9280,7 +9443,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="87" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B87" s="45" t="str">
         <f t="shared" si="5"/>
         <v>4D</v>
@@ -9334,7 +9497,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="88" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B88" s="45" t="str">
         <f t="shared" si="5"/>
         <v>4E</v>
@@ -9388,7 +9551,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="89" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B89" s="45" t="str">
         <f t="shared" si="5"/>
         <v>4F</v>
@@ -9442,7 +9605,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="90" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B90" s="45" t="str">
         <f t="shared" si="5"/>
         <v>50</v>
@@ -9496,7 +9659,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="91" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B91" s="45" t="str">
         <f t="shared" si="5"/>
         <v>51</v>
@@ -9550,7 +9713,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="92" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B92" s="45" t="str">
         <f t="shared" si="5"/>
         <v>52</v>
@@ -9604,7 +9767,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="93" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B93" s="45" t="str">
         <f t="shared" si="5"/>
         <v>53</v>
@@ -9658,7 +9821,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="94" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B94" s="45" t="str">
         <f t="shared" si="5"/>
         <v>54</v>
@@ -9712,7 +9875,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="95" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B95" s="45" t="str">
         <f t="shared" si="5"/>
         <v>55</v>
@@ -9766,7 +9929,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="96" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B96" s="45" t="str">
         <f t="shared" si="5"/>
         <v>56</v>
@@ -9820,7 +9983,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="97" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B97" s="45" t="str">
         <f t="shared" si="5"/>
         <v>57</v>
@@ -9874,7 +10037,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="98" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B98" s="45" t="str">
         <f t="shared" si="5"/>
         <v>58</v>
@@ -9928,7 +10091,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="99" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B99" s="45" t="str">
         <f t="shared" si="5"/>
         <v>59</v>
@@ -9982,7 +10145,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="100" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B100" s="45" t="str">
         <f t="shared" si="5"/>
         <v>5A</v>
@@ -10036,7 +10199,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="101" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B101" s="45" t="str">
         <f t="shared" si="5"/>
         <v>5B</v>
@@ -10090,7 +10253,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="102" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B102" s="45" t="str">
         <f t="shared" si="5"/>
         <v>5C</v>
@@ -10144,7 +10307,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="103" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B103" s="45" t="str">
         <f t="shared" si="5"/>
         <v>5D</v>
@@ -10198,7 +10361,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="104" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B104" s="45" t="str">
         <f t="shared" si="5"/>
         <v>5E</v>
@@ -10252,7 +10415,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="105" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B105" s="45" t="str">
         <f t="shared" si="5"/>
         <v>5F</v>
@@ -10306,7 +10469,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="106" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B106" s="45" t="str">
         <f t="shared" si="5"/>
         <v>60</v>
@@ -10360,7 +10523,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="107" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B107" s="45" t="str">
         <f t="shared" si="5"/>
         <v>61</v>
@@ -10414,7 +10577,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="108" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B108" s="45" t="str">
         <f t="shared" si="5"/>
         <v>62</v>
@@ -10468,7 +10631,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="109" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B109" s="45" t="str">
         <f t="shared" si="5"/>
         <v>63</v>
@@ -10522,7 +10685,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="110" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B110" s="45" t="str">
         <f t="shared" si="5"/>
         <v>64</v>
@@ -10576,7 +10739,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="111" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B111" s="45" t="str">
         <f t="shared" si="5"/>
         <v>65</v>
@@ -10630,7 +10793,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="112" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B112" s="45" t="str">
         <f t="shared" si="5"/>
         <v>66</v>
@@ -10684,7 +10847,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="113" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B113" s="45" t="str">
         <f t="shared" si="5"/>
         <v>67</v>
@@ -10738,7 +10901,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="114" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B114" s="45" t="str">
         <f t="shared" si="5"/>
         <v>68</v>
@@ -10792,7 +10955,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="115" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B115" s="45" t="str">
         <f t="shared" si="5"/>
         <v>69</v>
@@ -10846,7 +11009,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="116" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B116" s="45" t="str">
         <f t="shared" si="5"/>
         <v>6A</v>
@@ -10900,7 +11063,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="117" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B117" s="45" t="str">
         <f t="shared" si="5"/>
         <v>6B</v>
@@ -10954,7 +11117,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="118" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B118" s="45" t="str">
         <f t="shared" si="5"/>
         <v>6C</v>
@@ -11008,7 +11171,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="119" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B119" s="45" t="str">
         <f t="shared" si="5"/>
         <v>6D</v>
@@ -11062,7 +11225,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="120" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B120" s="45" t="str">
         <f t="shared" si="5"/>
         <v>6E</v>
@@ -11116,7 +11279,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="121" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B121" s="45" t="str">
         <f t="shared" si="5"/>
         <v>6F</v>
@@ -11170,7 +11333,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="122" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B122" s="45" t="str">
         <f t="shared" si="5"/>
         <v>70</v>
@@ -11224,7 +11387,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="123" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B123" s="45" t="str">
         <f t="shared" si="5"/>
         <v>71</v>
@@ -11278,7 +11441,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="124" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B124" s="45" t="str">
         <f t="shared" si="5"/>
         <v>72</v>
@@ -11332,7 +11495,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="125" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B125" s="45" t="str">
         <f t="shared" si="5"/>
         <v>73</v>
@@ -11386,7 +11549,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="126" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B126" s="45" t="str">
         <f t="shared" si="5"/>
         <v>74</v>
@@ -11440,7 +11603,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="127" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B127" s="45" t="str">
         <f t="shared" si="5"/>
         <v>75</v>
@@ -11494,7 +11657,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="128" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B128" s="45" t="str">
         <f t="shared" si="5"/>
         <v>76</v>
@@ -11548,7 +11711,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="129" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B129" s="45" t="str">
         <f t="shared" si="5"/>
         <v>77</v>
@@ -11602,7 +11765,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="130" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B130" s="45" t="str">
         <f t="shared" si="5"/>
         <v>78</v>
@@ -11656,7 +11819,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="131" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B131" s="45" t="str">
         <f t="shared" si="5"/>
         <v>79</v>
@@ -11710,7 +11873,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="132" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B132" s="45" t="str">
         <f t="shared" si="5"/>
         <v>7A</v>
@@ -11764,7 +11927,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="133" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B133" s="45" t="str">
         <f t="shared" si="5"/>
         <v>7B</v>
@@ -11818,7 +11981,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="134" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B134" s="45" t="str">
         <f t="shared" si="5"/>
         <v>7C</v>
@@ -11872,7 +12035,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="135" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B135" s="45" t="str">
         <f t="shared" si="5"/>
         <v>7D</v>
@@ -11926,7 +12089,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="136" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B136" s="45" t="str">
         <f t="shared" si="5"/>
         <v>7E</v>
@@ -11980,7 +12143,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="137" spans="2:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="2:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B137" s="45" t="str">
         <f t="shared" si="5"/>
         <v>7F</v>
@@ -12044,13 +12207,13 @@
         <v>00</v>
       </c>
     </row>
-    <row r="138" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:32" x14ac:dyDescent="0.25">
       <c r="C138" t="s">
         <v>71</v>
       </c>
       <c r="AC138" s="11"/>
     </row>
-    <row r="139" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:32" x14ac:dyDescent="0.25">
       <c r="D139" t="s">
         <v>72</v>
       </c>
@@ -12059,58 +12222,58 @@
       </c>
       <c r="AC139" s="11"/>
     </row>
-    <row r="140" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:32" x14ac:dyDescent="0.25">
       <c r="AC140" s="11"/>
     </row>
-    <row r="141" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:32" x14ac:dyDescent="0.25">
       <c r="AC141" s="11"/>
     </row>
-    <row r="142" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:32" x14ac:dyDescent="0.25">
       <c r="AC142" s="11"/>
     </row>
-    <row r="143" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:32" x14ac:dyDescent="0.25">
       <c r="AC143" s="11"/>
     </row>
-    <row r="144" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:32" x14ac:dyDescent="0.25">
       <c r="AC144" s="11"/>
     </row>
-    <row r="145" spans="29:29" x14ac:dyDescent="0.3">
+    <row r="145" spans="29:29" x14ac:dyDescent="0.25">
       <c r="AC145" s="11"/>
     </row>
-    <row r="146" spans="29:29" x14ac:dyDescent="0.3">
+    <row r="146" spans="29:29" x14ac:dyDescent="0.25">
       <c r="AC146" s="11"/>
     </row>
-    <row r="147" spans="29:29" x14ac:dyDescent="0.3">
+    <row r="147" spans="29:29" x14ac:dyDescent="0.25">
       <c r="AC147" s="11"/>
     </row>
-    <row r="148" spans="29:29" x14ac:dyDescent="0.3">
+    <row r="148" spans="29:29" x14ac:dyDescent="0.25">
       <c r="AC148" s="11"/>
     </row>
-    <row r="149" spans="29:29" x14ac:dyDescent="0.3">
+    <row r="149" spans="29:29" x14ac:dyDescent="0.25">
       <c r="AC149" s="11"/>
     </row>
-    <row r="150" spans="29:29" x14ac:dyDescent="0.3">
+    <row r="150" spans="29:29" x14ac:dyDescent="0.25">
       <c r="AC150" s="11"/>
     </row>
-    <row r="151" spans="29:29" x14ac:dyDescent="0.3">
+    <row r="151" spans="29:29" x14ac:dyDescent="0.25">
       <c r="AC151" s="11"/>
     </row>
-    <row r="152" spans="29:29" x14ac:dyDescent="0.3">
+    <row r="152" spans="29:29" x14ac:dyDescent="0.25">
       <c r="AC152" s="11"/>
     </row>
-    <row r="153" spans="29:29" x14ac:dyDescent="0.3">
+    <row r="153" spans="29:29" x14ac:dyDescent="0.25">
       <c r="AC153" s="11"/>
     </row>
-    <row r="154" spans="29:29" x14ac:dyDescent="0.3">
+    <row r="154" spans="29:29" x14ac:dyDescent="0.25">
       <c r="AC154" s="11"/>
     </row>
-    <row r="155" spans="29:29" x14ac:dyDescent="0.3">
+    <row r="155" spans="29:29" x14ac:dyDescent="0.25">
       <c r="AC155" s="11"/>
     </row>
-    <row r="156" spans="29:29" x14ac:dyDescent="0.3">
+    <row r="156" spans="29:29" x14ac:dyDescent="0.25">
       <c r="AC156" s="11"/>
     </row>
-    <row r="157" spans="29:29" x14ac:dyDescent="0.3">
+    <row r="157" spans="29:29" x14ac:dyDescent="0.25">
       <c r="AC157" s="11"/>
     </row>
   </sheetData>
@@ -12142,20 +12305,20 @@
       <selection activeCell="Y6" sqref="Y6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" style="45"/>
+    <col min="1" max="1" width="11.42578125" style="45"/>
     <col min="3" max="3" width="4" style="45" customWidth="1"/>
     <col min="4" max="8" width="4" customWidth="1"/>
-    <col min="9" max="17" width="4.44140625" customWidth="1"/>
-    <col min="18" max="21" width="6.88671875" customWidth="1"/>
+    <col min="9" max="17" width="4.42578125" customWidth="1"/>
+    <col min="18" max="21" width="6.85546875" customWidth="1"/>
     <col min="22" max="24" width="9" customWidth="1"/>
-    <col min="25" max="25" width="15.44140625" style="45" customWidth="1"/>
-    <col min="30" max="30" width="25.6640625" customWidth="1"/>
+    <col min="25" max="25" width="15.42578125" style="45" customWidth="1"/>
+    <col min="30" max="30" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:36" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="2:36" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B3" s="236"/>
       <c r="C3" s="237"/>
       <c r="D3" s="237"/>
@@ -12194,7 +12357,7 @@
       <c r="AI3" s="232"/>
       <c r="AJ3" s="1"/>
     </row>
-    <row r="4" spans="2:36" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B4" s="239"/>
       <c r="C4" s="240"/>
       <c r="D4" s="240"/>
@@ -12265,7 +12428,7 @@
       <c r="AI4" s="1"/>
       <c r="AJ4" s="1"/>
     </row>
-    <row r="5" spans="2:36" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="59" t="s">
         <v>107</v>
       </c>
@@ -12322,7 +12485,7 @@
       <c r="AI5" s="1"/>
       <c r="AJ5" s="1"/>
     </row>
-    <row r="6" spans="2:36" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:36" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B6" s="61" t="s">
         <v>15</v>
       </c>
@@ -12408,7 +12571,7 @@
       <c r="AI6" s="1"/>
       <c r="AJ6" s="1"/>
     </row>
-    <row r="7" spans="2:36" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B7" s="73" t="s">
         <v>19</v>
       </c>
@@ -12494,7 +12657,7 @@
       <c r="AI7" s="1"/>
       <c r="AJ7" s="1"/>
     </row>
-    <row r="8" spans="2:36" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B8" s="62" t="s">
         <v>113</v>
       </c>
@@ -12580,7 +12743,7 @@
       <c r="AI8" s="1"/>
       <c r="AJ8" s="1"/>
     </row>
-    <row r="9" spans="2:36" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B9" s="73" t="s">
         <v>20</v>
       </c>
@@ -12666,7 +12829,7 @@
       <c r="AI9" s="1"/>
       <c r="AJ9" s="1"/>
     </row>
-    <row r="10" spans="2:36" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B10" s="62" t="s">
         <v>24</v>
       </c>
@@ -12752,7 +12915,7 @@
       <c r="AI10" s="1"/>
       <c r="AJ10" s="1"/>
     </row>
-    <row r="11" spans="2:36" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B11" s="62" t="s">
         <v>28</v>
       </c>
@@ -12838,7 +13001,7 @@
       <c r="AI11" s="1"/>
       <c r="AJ11" s="1"/>
     </row>
-    <row r="12" spans="2:36" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B12" s="62" t="s">
         <v>32</v>
       </c>
@@ -12924,7 +13087,7 @@
       <c r="AI12" s="1"/>
       <c r="AJ12" s="1"/>
     </row>
-    <row r="13" spans="2:36" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B13" s="62" t="s">
         <v>16</v>
       </c>
@@ -13010,7 +13173,7 @@
       <c r="AI13" s="1"/>
       <c r="AJ13" s="1"/>
     </row>
-    <row r="14" spans="2:36" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B14" s="63" t="s">
         <v>39</v>
       </c>
@@ -13096,7 +13259,7 @@
       <c r="AI14" s="1"/>
       <c r="AJ14" s="1"/>
     </row>
-    <row r="15" spans="2:36" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B15" s="63" t="s">
         <v>41</v>
       </c>
@@ -13182,7 +13345,7 @@
       <c r="AI15" s="1"/>
       <c r="AJ15" s="1"/>
     </row>
-    <row r="16" spans="2:36" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B16" s="63" t="s">
         <v>44</v>
       </c>
@@ -13268,7 +13431,7 @@
       <c r="AI16" s="1"/>
       <c r="AJ16" s="1"/>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B17" s="63" t="s">
         <v>121</v>
       </c>
@@ -13354,7 +13517,7 @@
       <c r="AI17" s="1"/>
       <c r="AJ17" s="1"/>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A18" s="117" t="s">
         <v>129</v>
       </c>
@@ -13443,7 +13606,7 @@
       <c r="AI18" s="1"/>
       <c r="AJ18" s="1"/>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19" s="117" t="s">
         <v>129</v>
       </c>
@@ -13532,7 +13695,7 @@
       <c r="AI19" s="1"/>
       <c r="AJ19" s="1"/>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B20" s="64"/>
       <c r="C20" s="45">
         <v>0</v>
@@ -13616,7 +13779,7 @@
       <c r="AI20" s="1"/>
       <c r="AJ20" s="1"/>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B21" s="69" t="s">
         <v>116</v>
       </c>
@@ -13702,7 +13865,7 @@
       <c r="AI21" s="1"/>
       <c r="AJ21" s="1"/>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B22" s="65"/>
       <c r="C22" s="45">
         <v>0</v>
@@ -13786,7 +13949,7 @@
       <c r="AI22" s="1"/>
       <c r="AJ22" s="1"/>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B23" s="65"/>
       <c r="C23" s="45">
         <v>0</v>
@@ -13870,7 +14033,7 @@
       <c r="AI23" s="1"/>
       <c r="AJ23" s="1"/>
     </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B24" s="65"/>
       <c r="C24" s="45">
         <v>0</v>
@@ -13954,7 +14117,7 @@
       <c r="AI24" s="1"/>
       <c r="AJ24" s="1"/>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B25" s="65"/>
       <c r="C25" s="45">
         <v>0</v>
@@ -14038,7 +14201,7 @@
       <c r="AI25" s="1"/>
       <c r="AJ25" s="1"/>
     </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B26" s="65"/>
       <c r="C26" s="45">
         <v>0</v>
@@ -14122,7 +14285,7 @@
       <c r="AI26" s="1"/>
       <c r="AJ26" s="1"/>
     </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B27" s="65"/>
       <c r="C27" s="45">
         <v>0</v>
@@ -14206,7 +14369,7 @@
       <c r="AI27" s="1"/>
       <c r="AJ27" s="1"/>
     </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B28" s="65"/>
       <c r="C28" s="45">
         <v>0</v>
@@ -14290,7 +14453,7 @@
       <c r="AI28" s="1"/>
       <c r="AJ28" s="1"/>
     </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B29" s="65"/>
       <c r="C29" s="45">
         <v>0</v>
@@ -14374,7 +14537,7 @@
       <c r="AI29" s="1"/>
       <c r="AJ29" s="1"/>
     </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B30" s="63"/>
       <c r="C30" s="45">
         <v>0</v>
@@ -14458,7 +14621,7 @@
       <c r="AI30" s="1"/>
       <c r="AJ30" s="1"/>
     </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B31" s="63"/>
       <c r="C31" s="45">
         <v>0</v>
@@ -14542,7 +14705,7 @@
       <c r="AI31" s="1"/>
       <c r="AJ31" s="1"/>
     </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B32" s="64"/>
       <c r="C32" s="45">
         <v>0</v>
@@ -14626,7 +14789,7 @@
       <c r="AI32" s="1"/>
       <c r="AJ32" s="1"/>
     </row>
-    <row r="33" spans="2:50" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:50" x14ac:dyDescent="0.25">
       <c r="B33" s="66"/>
       <c r="C33" s="45">
         <v>0</v>
@@ -14710,7 +14873,7 @@
       <c r="AI33" s="1"/>
       <c r="AJ33" s="1"/>
     </row>
-    <row r="34" spans="2:50" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:50" x14ac:dyDescent="0.25">
       <c r="B34" s="65"/>
       <c r="C34" s="45">
         <v>0</v>
@@ -14794,7 +14957,7 @@
       <c r="AI34" s="1"/>
       <c r="AJ34" s="1"/>
     </row>
-    <row r="35" spans="2:50" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:50" x14ac:dyDescent="0.25">
       <c r="B35" s="65"/>
       <c r="C35" s="45">
         <v>0</v>
@@ -14878,7 +15041,7 @@
       <c r="AI35" s="1"/>
       <c r="AJ35" s="1"/>
     </row>
-    <row r="36" spans="2:50" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:50" x14ac:dyDescent="0.25">
       <c r="B36" s="65"/>
       <c r="C36" s="45">
         <v>0</v>
@@ -14962,7 +15125,7 @@
       <c r="AI36" s="1"/>
       <c r="AJ36" s="1"/>
     </row>
-    <row r="37" spans="2:50" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:50" x14ac:dyDescent="0.25">
       <c r="B37" s="65"/>
       <c r="C37" s="45">
         <v>0</v>
@@ -15046,7 +15209,7 @@
       <c r="AI37" s="1"/>
       <c r="AJ37" s="1"/>
     </row>
-    <row r="38" spans="2:50" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:50" x14ac:dyDescent="0.25">
       <c r="B38" s="65"/>
       <c r="C38" s="3">
         <v>1</v>
@@ -15130,7 +15293,7 @@
       <c r="AI38" s="1"/>
       <c r="AJ38" s="1"/>
     </row>
-    <row r="39" spans="2:50" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:50" x14ac:dyDescent="0.25">
       <c r="B39" s="65"/>
       <c r="C39" s="3">
         <v>1</v>
@@ -15203,7 +15366,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="40" spans="2:50" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:50" x14ac:dyDescent="0.25">
       <c r="B40" s="65"/>
       <c r="C40" s="3">
         <v>1</v>
@@ -15276,7 +15439,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="41" spans="2:50" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:50" x14ac:dyDescent="0.25">
       <c r="B41" s="65"/>
       <c r="C41" s="3">
         <v>1</v>
@@ -15349,7 +15512,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="42" spans="2:50" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:50" x14ac:dyDescent="0.25">
       <c r="B42" s="65"/>
       <c r="C42" s="3">
         <v>1</v>
@@ -15472,7 +15635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:50" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:50" x14ac:dyDescent="0.25">
       <c r="B43" s="65"/>
       <c r="C43" s="3">
         <v>1</v>
@@ -15594,7 +15757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="2:50" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:50" x14ac:dyDescent="0.25">
       <c r="B44" s="65"/>
       <c r="C44" s="3">
         <v>1</v>
@@ -15668,7 +15831,7 @@
       </c>
       <c r="Z44" s="3"/>
     </row>
-    <row r="45" spans="2:50" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:50" x14ac:dyDescent="0.25">
       <c r="B45" s="65"/>
       <c r="C45" s="3">
         <v>1</v>
@@ -15742,7 +15905,7 @@
       </c>
       <c r="Z45" s="3"/>
     </row>
-    <row r="46" spans="2:50" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:50" x14ac:dyDescent="0.25">
       <c r="B46" s="65"/>
       <c r="C46" s="3">
         <v>1</v>
@@ -15815,7 +15978,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="47" spans="2:50" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:50" x14ac:dyDescent="0.25">
       <c r="B47" s="65"/>
       <c r="C47" s="3">
         <v>1</v>
@@ -15889,7 +16052,7 @@
       </c>
       <c r="Z47" s="3"/>
     </row>
-    <row r="48" spans="2:50" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:50" x14ac:dyDescent="0.25">
       <c r="B48" s="65"/>
       <c r="C48" s="3">
         <v>1</v>
@@ -15963,7 +16126,7 @@
       </c>
       <c r="Z48" s="3"/>
     </row>
-    <row r="49" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B49" s="65"/>
       <c r="C49" s="3">
         <v>1</v>
@@ -16036,7 +16199,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="50" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B50" s="65"/>
       <c r="C50" s="3">
         <v>1</v>
@@ -16109,7 +16272,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="51" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B51" s="65"/>
       <c r="C51" s="3">
         <v>1</v>
@@ -16182,7 +16345,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="52" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B52" s="65"/>
       <c r="C52" s="3">
         <v>1</v>
@@ -16255,7 +16418,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="53" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B53" s="65"/>
       <c r="C53" s="3">
         <v>1</v>
@@ -16328,7 +16491,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="54" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B54" s="65"/>
       <c r="C54" s="3">
         <v>1</v>
@@ -16401,7 +16564,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="55" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B55" s="65"/>
       <c r="C55" s="3">
         <v>1</v>
@@ -16474,7 +16637,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="56" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B56" s="65"/>
       <c r="C56" s="3">
         <v>1</v>
@@ -16547,7 +16710,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="57" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B57" s="65"/>
       <c r="C57" s="3">
         <v>1</v>
@@ -16620,7 +16783,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="58" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B58" s="65"/>
       <c r="C58" s="3">
         <v>1</v>
@@ -16693,7 +16856,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="59" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B59" s="65"/>
       <c r="C59" s="3">
         <v>1</v>
@@ -16766,7 +16929,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="60" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B60" s="65"/>
       <c r="C60" s="3">
         <v>1</v>
@@ -16839,7 +17002,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="61" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B61" s="65"/>
       <c r="C61" s="3">
         <v>1</v>
@@ -16912,7 +17075,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="62" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B62" s="65"/>
       <c r="C62" s="3">
         <v>1</v>
@@ -16985,7 +17148,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="63" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B63" s="65"/>
       <c r="C63" s="3">
         <v>1</v>
@@ -17058,7 +17221,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="64" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B64" s="65"/>
       <c r="C64" s="3">
         <v>1</v>
@@ -17131,7 +17294,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="65" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B65" s="65"/>
       <c r="C65" s="3">
         <v>1</v>
@@ -17204,7 +17367,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="66" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B66" s="65"/>
       <c r="C66" s="3">
         <v>1</v>
@@ -17277,7 +17440,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="67" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B67" s="65"/>
       <c r="C67" s="3">
         <v>1</v>
@@ -17350,7 +17513,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="68" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B68" s="65"/>
       <c r="C68" s="3">
         <v>1</v>
@@ -17423,7 +17586,7 @@
         <v>9A7C</v>
       </c>
     </row>
-    <row r="69" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B69" s="67"/>
       <c r="C69" s="68">
         <v>1</v>
@@ -17514,26 +17677,26 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F461F9F-87D6-4C96-820F-6111A3E2F850}">
-  <dimension ref="C4:S33"/>
+  <dimension ref="C4:S37"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="P31" sqref="P31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="18.44140625" customWidth="1"/>
-    <col min="15" max="15" width="19.44140625" customWidth="1"/>
-    <col min="17" max="18" width="12.44140625" customWidth="1"/>
-    <col min="19" max="19" width="16.6640625" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="15" max="15" width="19.42578125" customWidth="1"/>
+    <col min="17" max="18" width="12.42578125" customWidth="1"/>
+    <col min="19" max="19" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="5" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:19" x14ac:dyDescent="0.25">
       <c r="D5" s="119" t="s">
         <v>132</v>
       </c>
@@ -17560,7 +17723,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="6" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:19" x14ac:dyDescent="0.25">
       <c r="D6" s="45">
         <v>0</v>
       </c>
@@ -17596,7 +17759,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="7" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:19" x14ac:dyDescent="0.25">
       <c r="D7" s="45">
         <v>0</v>
       </c>
@@ -17635,7 +17798,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="8" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:19" x14ac:dyDescent="0.25">
       <c r="D8" s="45">
         <v>1</v>
       </c>
@@ -17674,7 +17837,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="9" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:19" x14ac:dyDescent="0.25">
       <c r="D9" s="45">
         <v>1</v>
       </c>
@@ -17710,7 +17873,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="10" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:19" x14ac:dyDescent="0.25">
       <c r="H10" s="45">
         <v>1</v>
       </c>
@@ -17737,7 +17900,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="11" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:19" x14ac:dyDescent="0.25">
       <c r="H11" s="45">
         <v>1</v>
       </c>
@@ -17755,7 +17918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:19" x14ac:dyDescent="0.25">
       <c r="H12" s="45">
         <v>1</v>
       </c>
@@ -17773,7 +17936,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="13" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:19" x14ac:dyDescent="0.25">
       <c r="H13" s="45">
         <v>1</v>
       </c>
@@ -17791,12 +17954,12 @@
         <v>141</v>
       </c>
     </row>
-    <row r="15" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:19" x14ac:dyDescent="0.25">
       <c r="Q15" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="16" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:19" x14ac:dyDescent="0.25">
       <c r="Q16">
         <v>0</v>
       </c>
@@ -17804,7 +17967,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="17" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>174</v>
       </c>
@@ -17815,7 +17978,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="18" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D18" s="240" t="s">
         <v>175</v>
       </c>
@@ -17831,7 +17994,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="19" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D19" s="45">
         <v>0</v>
       </c>
@@ -17851,7 +18014,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="20" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
         <v>176</v>
       </c>
@@ -17865,7 +18028,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="23" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C23" s="45" t="s">
         <v>199</v>
       </c>
@@ -17879,7 +18042,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="24" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C24" s="45">
         <v>0</v>
       </c>
@@ -17902,7 +18065,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="25" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C25" s="45">
         <v>0</v>
       </c>
@@ -17916,7 +18079,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="26" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C26" s="45">
         <v>0</v>
       </c>
@@ -17930,7 +18093,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="27" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C27" s="45">
         <v>0</v>
       </c>
@@ -17944,10 +18107,10 @@
         <v>200</v>
       </c>
     </row>
-    <row r="28" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C28" s="45"/>
     </row>
-    <row r="29" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C29" s="45">
         <v>1</v>
       </c>
@@ -17961,7 +18124,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="30" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C30" s="45">
         <v>1</v>
       </c>
@@ -17975,7 +18138,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="31" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C31" s="45">
         <v>1</v>
       </c>
@@ -17989,7 +18152,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C32" s="45">
         <v>1</v>
       </c>
@@ -18002,9 +18165,35 @@
       <c r="F32" s="45" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="O32" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="33" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C33" s="45"/>
+      <c r="O33" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="34" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O34" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="35" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O35" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="36" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O36" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="37" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O37" t="s">
+        <v>208</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Implemented Stack Pointer Part
</commit_message>
<xml_diff>
--- a/Documentation/CPU_DOC.xlsx
+++ b/Documentation/CPU_DOC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Desktop\CPU_8Bit\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D449B87-208F-4B69-9654-9869B46E1749}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D3C4A8-5703-49D3-82EC-9462678F7AC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{5BA4E079-EFAB-4B55-B322-C6522B3056FF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="2" xr2:uid="{5BA4E079-EFAB-4B55-B322-C6522B3056FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Control-Unit" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="236">
   <si>
     <t>1=Read</t>
   </si>
@@ -725,6 +725,27 @@
   </si>
   <si>
     <t>G2:0</t>
+  </si>
+  <si>
+    <t>PUSH</t>
+  </si>
+  <si>
+    <t>POP</t>
+  </si>
+  <si>
+    <t>CALL</t>
+  </si>
+  <si>
+    <t>RET</t>
+  </si>
+  <si>
+    <t>RCO-1</t>
+  </si>
+  <si>
+    <t>RCO+1</t>
+  </si>
+  <si>
+    <t>0000</t>
   </si>
 </sst>
 </file>
@@ -1739,7 +1760,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="253">
+  <cellXfs count="254">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2329,6 +2350,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2829,8 +2851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0373F33-972A-4E8D-B1CE-9C5EF0708B27}">
   <dimension ref="A2:AI157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2857,50 +2879,50 @@
     </row>
     <row r="4" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="211" t="s">
+      <c r="C5" s="212" t="s">
         <v>109</v>
       </c>
-      <c r="D5" s="212"/>
-      <c r="E5" s="212"/>
-      <c r="F5" s="212"/>
-      <c r="G5" s="212"/>
-      <c r="H5" s="212"/>
-      <c r="I5" s="212"/>
-      <c r="J5" s="212"/>
-      <c r="K5" s="212"/>
-      <c r="L5" s="213"/>
+      <c r="D5" s="213"/>
+      <c r="E5" s="213"/>
+      <c r="F5" s="213"/>
+      <c r="G5" s="213"/>
+      <c r="H5" s="213"/>
+      <c r="I5" s="213"/>
+      <c r="J5" s="213"/>
+      <c r="K5" s="213"/>
+      <c r="L5" s="214"/>
       <c r="M5" s="128"/>
-      <c r="N5" s="225" t="s">
+      <c r="N5" s="226" t="s">
         <v>108</v>
       </c>
-      <c r="O5" s="225"/>
-      <c r="P5" s="225"/>
-      <c r="Q5" s="225"/>
-      <c r="R5" s="225"/>
-      <c r="S5" s="225"/>
-      <c r="T5" s="225"/>
-      <c r="U5" s="225"/>
-      <c r="V5" s="225"/>
-      <c r="W5" s="225"/>
-      <c r="X5" s="225"/>
-      <c r="Y5" s="225"/>
-      <c r="Z5" s="225"/>
-      <c r="AA5" s="225"/>
-      <c r="AB5" s="225"/>
-      <c r="AC5" s="226"/>
-      <c r="AD5" s="209"/>
+      <c r="O5" s="226"/>
+      <c r="P5" s="226"/>
+      <c r="Q5" s="226"/>
+      <c r="R5" s="226"/>
+      <c r="S5" s="226"/>
+      <c r="T5" s="226"/>
+      <c r="U5" s="226"/>
+      <c r="V5" s="226"/>
+      <c r="W5" s="226"/>
+      <c r="X5" s="226"/>
+      <c r="Y5" s="226"/>
+      <c r="Z5" s="226"/>
+      <c r="AA5" s="226"/>
+      <c r="AB5" s="226"/>
+      <c r="AC5" s="227"/>
+      <c r="AD5" s="210"/>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="C6" s="214"/>
-      <c r="D6" s="215"/>
-      <c r="E6" s="215"/>
-      <c r="F6" s="215"/>
-      <c r="G6" s="215"/>
-      <c r="H6" s="215"/>
-      <c r="I6" s="215"/>
-      <c r="J6" s="215"/>
-      <c r="K6" s="215"/>
-      <c r="L6" s="216"/>
+      <c r="C6" s="215"/>
+      <c r="D6" s="216"/>
+      <c r="E6" s="216"/>
+      <c r="F6" s="216"/>
+      <c r="G6" s="216"/>
+      <c r="H6" s="216"/>
+      <c r="I6" s="216"/>
+      <c r="J6" s="216"/>
+      <c r="K6" s="216"/>
+      <c r="L6" s="217"/>
       <c r="M6" s="14"/>
       <c r="N6" s="4">
         <v>0</v>
@@ -2950,7 +2972,7 @@
       <c r="AC6" s="129">
         <v>15</v>
       </c>
-      <c r="AD6" s="210"/>
+      <c r="AD6" s="211"/>
       <c r="AE6" s="4"/>
       <c r="AF6" s="4"/>
       <c r="AG6" s="4"/>
@@ -2958,11 +2980,11 @@
       <c r="AI6" s="2"/>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="C7" s="217"/>
-      <c r="D7" s="218"/>
-      <c r="E7" s="218"/>
-      <c r="F7" s="218"/>
-      <c r="G7" s="218"/>
+      <c r="C7" s="218"/>
+      <c r="D7" s="219"/>
+      <c r="E7" s="219"/>
+      <c r="F7" s="219"/>
+      <c r="G7" s="219"/>
       <c r="H7" s="12"/>
       <c r="I7" s="28" t="s">
         <v>93</v>
@@ -2973,12 +2995,12 @@
       <c r="K7" s="22"/>
       <c r="L7" s="29"/>
       <c r="M7" s="126"/>
-      <c r="N7" s="227"/>
-      <c r="O7" s="227"/>
-      <c r="P7" s="227"/>
-      <c r="Q7" s="227"/>
-      <c r="R7" s="227"/>
-      <c r="S7" s="227"/>
+      <c r="N7" s="228"/>
+      <c r="O7" s="228"/>
+      <c r="P7" s="228"/>
+      <c r="Q7" s="228"/>
+      <c r="R7" s="228"/>
+      <c r="S7" s="228"/>
       <c r="T7" s="5" t="s">
         <v>137</v>
       </c>
@@ -3003,57 +3025,57 @@
       <c r="AA7" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="AB7" s="228" t="s">
+      <c r="AB7" s="229" t="s">
         <v>143</v>
       </c>
-      <c r="AC7" s="229"/>
-      <c r="AD7" s="210"/>
+      <c r="AC7" s="230"/>
+      <c r="AD7" s="211"/>
       <c r="AE7" s="2"/>
       <c r="AF7" s="3"/>
       <c r="AG7" s="3"/>
       <c r="AH7" s="2"/>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="C8" s="219"/>
-      <c r="D8" s="220"/>
-      <c r="E8" s="220"/>
-      <c r="F8" s="220"/>
-      <c r="G8" s="220"/>
+      <c r="C8" s="220"/>
+      <c r="D8" s="221"/>
+      <c r="E8" s="221"/>
+      <c r="F8" s="221"/>
+      <c r="G8" s="221"/>
       <c r="H8"/>
-      <c r="I8" s="221" t="s">
+      <c r="I8" s="222" t="s">
         <v>82</v>
       </c>
-      <c r="J8" s="222"/>
-      <c r="K8" s="222"/>
-      <c r="L8" s="223"/>
-      <c r="M8" s="224" t="s">
+      <c r="J8" s="223"/>
+      <c r="K8" s="223"/>
+      <c r="L8" s="224"/>
+      <c r="M8" s="225" t="s">
         <v>2</v>
       </c>
-      <c r="N8" s="224"/>
-      <c r="O8" s="224"/>
-      <c r="P8" s="224"/>
-      <c r="Q8" s="224"/>
-      <c r="R8" s="224"/>
-      <c r="S8" s="224"/>
-      <c r="T8" s="233" t="s">
+      <c r="N8" s="225"/>
+      <c r="O8" s="225"/>
+      <c r="P8" s="225"/>
+      <c r="Q8" s="225"/>
+      <c r="R8" s="225"/>
+      <c r="S8" s="225"/>
+      <c r="T8" s="234" t="s">
         <v>146</v>
       </c>
-      <c r="U8" s="233"/>
-      <c r="V8" s="234" t="s">
+      <c r="U8" s="234"/>
+      <c r="V8" s="235" t="s">
         <v>147</v>
       </c>
-      <c r="W8" s="234"/>
-      <c r="X8" s="234"/>
-      <c r="Y8" s="234"/>
-      <c r="Z8" s="232" t="s">
+      <c r="W8" s="235"/>
+      <c r="X8" s="235"/>
+      <c r="Y8" s="235"/>
+      <c r="Z8" s="233" t="s">
         <v>144</v>
       </c>
-      <c r="AA8" s="232"/>
-      <c r="AB8" s="230" t="s">
+      <c r="AA8" s="233"/>
+      <c r="AB8" s="231" t="s">
         <v>145</v>
       </c>
-      <c r="AC8" s="231"/>
-      <c r="AD8" s="210"/>
+      <c r="AC8" s="232"/>
+      <c r="AD8" s="211"/>
       <c r="AE8" s="123"/>
       <c r="AF8" s="123"/>
       <c r="AG8" s="123"/>
@@ -7965,7 +7987,9 @@
         <v>55</v>
       </c>
       <c r="E65" s="203"/>
-      <c r="F65" s="46"/>
+      <c r="F65" s="46" t="s">
+        <v>229</v>
+      </c>
       <c r="G65" s="10"/>
       <c r="H65" s="16"/>
       <c r="L65" s="9"/>
@@ -8046,7 +8070,9 @@
         <v>56</v>
       </c>
       <c r="E66" s="203"/>
-      <c r="F66" s="46"/>
+      <c r="F66" s="46" t="s">
+        <v>230</v>
+      </c>
       <c r="G66" s="10"/>
       <c r="H66" s="16"/>
       <c r="L66" s="9"/>
@@ -8127,7 +8153,9 @@
         <v>57</v>
       </c>
       <c r="E67" s="203"/>
-      <c r="F67" s="46"/>
+      <c r="F67" s="46" t="s">
+        <v>231</v>
+      </c>
       <c r="G67" s="10"/>
       <c r="H67" s="16"/>
       <c r="L67" s="9"/>
@@ -8208,7 +8236,9 @@
         <v>58</v>
       </c>
       <c r="E68" s="203"/>
-      <c r="F68" s="46"/>
+      <c r="F68" s="46" t="s">
+        <v>232</v>
+      </c>
       <c r="G68" s="10"/>
       <c r="H68" s="16"/>
       <c r="L68" s="9"/>
@@ -12558,31 +12588,31 @@
   <sheetData>
     <row r="2" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B3" s="239"/>
-      <c r="C3" s="240"/>
-      <c r="D3" s="240"/>
-      <c r="E3" s="240"/>
-      <c r="F3" s="240"/>
-      <c r="G3" s="240"/>
-      <c r="H3" s="241"/>
-      <c r="I3" s="245" t="s">
+      <c r="B3" s="240"/>
+      <c r="C3" s="241"/>
+      <c r="D3" s="241"/>
+      <c r="E3" s="241"/>
+      <c r="F3" s="241"/>
+      <c r="G3" s="241"/>
+      <c r="H3" s="242"/>
+      <c r="I3" s="246" t="s">
         <v>97</v>
       </c>
-      <c r="J3" s="246"/>
-      <c r="K3" s="246"/>
-      <c r="L3" s="246"/>
-      <c r="M3" s="246"/>
-      <c r="N3" s="246"/>
-      <c r="O3" s="246"/>
-      <c r="P3" s="246"/>
-      <c r="Q3" s="246"/>
-      <c r="R3" s="246"/>
-      <c r="S3" s="246"/>
-      <c r="T3" s="246"/>
-      <c r="U3" s="246"/>
-      <c r="V3" s="246"/>
-      <c r="W3" s="246"/>
-      <c r="X3" s="247"/>
+      <c r="J3" s="247"/>
+      <c r="K3" s="247"/>
+      <c r="L3" s="247"/>
+      <c r="M3" s="247"/>
+      <c r="N3" s="247"/>
+      <c r="O3" s="247"/>
+      <c r="P3" s="247"/>
+      <c r="Q3" s="247"/>
+      <c r="R3" s="247"/>
+      <c r="S3" s="247"/>
+      <c r="T3" s="247"/>
+      <c r="U3" s="247"/>
+      <c r="V3" s="247"/>
+      <c r="W3" s="247"/>
+      <c r="X3" s="248"/>
       <c r="Y3" s="81"/>
       <c r="Z3" s="56"/>
       <c r="AA3" s="56"/>
@@ -12590,20 +12620,20 @@
       <c r="AC3" s="3"/>
       <c r="AD3" s="2"/>
       <c r="AE3" s="1"/>
-      <c r="AF3" s="235"/>
-      <c r="AG3" s="235"/>
-      <c r="AH3" s="235"/>
-      <c r="AI3" s="235"/>
+      <c r="AF3" s="236"/>
+      <c r="AG3" s="236"/>
+      <c r="AH3" s="236"/>
+      <c r="AI3" s="236"/>
       <c r="AJ3" s="1"/>
     </row>
     <row r="4" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B4" s="242"/>
-      <c r="C4" s="243"/>
-      <c r="D4" s="243"/>
-      <c r="E4" s="243"/>
-      <c r="F4" s="243"/>
-      <c r="G4" s="243"/>
-      <c r="H4" s="244"/>
+      <c r="B4" s="243"/>
+      <c r="C4" s="244"/>
+      <c r="D4" s="244"/>
+      <c r="E4" s="244"/>
+      <c r="F4" s="244"/>
+      <c r="G4" s="244"/>
+      <c r="H4" s="245"/>
       <c r="I4" s="57">
         <v>0</v>
       </c>
@@ -12652,7 +12682,7 @@
       <c r="X4" s="58">
         <v>15</v>
       </c>
-      <c r="Y4" s="251" t="s">
+      <c r="Y4" s="252" t="s">
         <v>116</v>
       </c>
       <c r="Z4" s="50"/>
@@ -12671,28 +12701,28 @@
       <c r="B5" s="59" t="s">
         <v>98</v>
       </c>
-      <c r="C5" s="248" t="s">
+      <c r="C5" s="249" t="s">
         <v>99</v>
       </c>
-      <c r="D5" s="249"/>
-      <c r="E5" s="249"/>
-      <c r="F5" s="249"/>
-      <c r="G5" s="249"/>
-      <c r="H5" s="250"/>
-      <c r="I5" s="236" t="s">
+      <c r="D5" s="250"/>
+      <c r="E5" s="250"/>
+      <c r="F5" s="250"/>
+      <c r="G5" s="250"/>
+      <c r="H5" s="251"/>
+      <c r="I5" s="237" t="s">
         <v>100</v>
       </c>
-      <c r="J5" s="237"/>
-      <c r="K5" s="237"/>
-      <c r="L5" s="237"/>
-      <c r="M5" s="237"/>
-      <c r="N5" s="238"/>
-      <c r="O5" s="236" t="s">
+      <c r="J5" s="238"/>
+      <c r="K5" s="238"/>
+      <c r="L5" s="238"/>
+      <c r="M5" s="238"/>
+      <c r="N5" s="239"/>
+      <c r="O5" s="237" t="s">
         <v>101</v>
       </c>
-      <c r="P5" s="237"/>
-      <c r="Q5" s="237"/>
-      <c r="R5" s="238"/>
+      <c r="P5" s="238"/>
+      <c r="Q5" s="238"/>
+      <c r="R5" s="239"/>
       <c r="S5" s="24" t="s">
         <v>102</v>
       </c>
@@ -12711,7 +12741,7 @@
       <c r="X5" s="60" t="s">
         <v>111</v>
       </c>
-      <c r="Y5" s="252"/>
+      <c r="Y5" s="253"/>
       <c r="Z5" s="3"/>
       <c r="AA5" s="3"/>
       <c r="AB5" s="3"/>
@@ -17916,26 +17946,27 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F461F9F-87D6-4C96-820F-6111A3E2F850}">
-  <dimension ref="C4:S37"/>
+  <dimension ref="C4:AA37"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P31" sqref="P31"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
     <col min="15" max="15" width="19.42578125" customWidth="1"/>
     <col min="17" max="18" width="12.42578125" customWidth="1"/>
     <col min="19" max="19" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D5" s="119" t="s">
         <v>123</v>
       </c>
@@ -17962,7 +17993,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D6" s="45">
         <v>0</v>
       </c>
@@ -17997,8 +18028,27 @@
       <c r="S6" s="45" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="7" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="U6" s="45" t="s">
+        <v>234</v>
+      </c>
+      <c r="V6" s="119" t="s">
+        <v>134</v>
+      </c>
+      <c r="W6" s="120" t="s">
+        <v>133</v>
+      </c>
+      <c r="X6" s="119" t="s">
+        <v>233</v>
+      </c>
+      <c r="Y6" s="119"/>
+      <c r="Z6" s="119" t="s">
+        <v>131</v>
+      </c>
+      <c r="AA6" s="120" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D7" s="45">
         <v>0</v>
       </c>
@@ -18036,8 +18086,27 @@
       <c r="S7" s="45" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="8" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="U7" s="45">
+        <v>0</v>
+      </c>
+      <c r="V7" s="45">
+        <v>0</v>
+      </c>
+      <c r="W7" s="45">
+        <v>0</v>
+      </c>
+      <c r="X7" s="45">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="45"/>
+      <c r="Z7" s="45">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D8" s="45">
         <v>1</v>
       </c>
@@ -18075,8 +18144,27 @@
       <c r="S8" s="45" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="9" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="U8" s="45">
+        <v>0</v>
+      </c>
+      <c r="V8" s="45">
+        <v>0</v>
+      </c>
+      <c r="W8" s="45">
+        <v>0</v>
+      </c>
+      <c r="X8" s="45">
+        <v>1</v>
+      </c>
+      <c r="Y8" s="45"/>
+      <c r="Z8" s="45">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D9" s="45">
         <v>1</v>
       </c>
@@ -18111,8 +18199,27 @@
       <c r="S9" s="45" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="10" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="U9" s="45">
+        <v>0</v>
+      </c>
+      <c r="V9" s="45">
+        <v>0</v>
+      </c>
+      <c r="W9" s="45">
+        <v>1</v>
+      </c>
+      <c r="X9" s="45">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="45"/>
+      <c r="Z9" s="45">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="3:27" x14ac:dyDescent="0.25">
       <c r="H10" s="45">
         <v>1</v>
       </c>
@@ -18138,8 +18245,27 @@
       <c r="S10" s="45" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="11" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="U10" s="45">
+        <v>0</v>
+      </c>
+      <c r="V10" s="45">
+        <v>0</v>
+      </c>
+      <c r="W10" s="45">
+        <v>1</v>
+      </c>
+      <c r="X10" s="45">
+        <v>1</v>
+      </c>
+      <c r="Y10" s="45"/>
+      <c r="Z10" s="45">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="3:27" x14ac:dyDescent="0.25">
       <c r="H11" s="45">
         <v>1</v>
       </c>
@@ -18156,8 +18282,27 @@
       <c r="M11" s="45">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="U11" s="45">
+        <v>0</v>
+      </c>
+      <c r="V11" s="45">
+        <v>1</v>
+      </c>
+      <c r="W11" s="45">
+        <v>0</v>
+      </c>
+      <c r="X11" s="45">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="45"/>
+      <c r="Z11" s="45">
+        <v>1</v>
+      </c>
+      <c r="AA11" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="3:27" x14ac:dyDescent="0.25">
       <c r="H12" s="45">
         <v>1</v>
       </c>
@@ -18174,8 +18319,27 @@
       <c r="M12" s="45" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="13" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="U12" s="45">
+        <v>0</v>
+      </c>
+      <c r="V12" s="45">
+        <v>1</v>
+      </c>
+      <c r="W12" s="45">
+        <v>0</v>
+      </c>
+      <c r="X12" s="45">
+        <v>1</v>
+      </c>
+      <c r="Y12" s="45"/>
+      <c r="Z12" s="45">
+        <v>1</v>
+      </c>
+      <c r="AA12" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="3:27" x14ac:dyDescent="0.25">
       <c r="H13" s="45">
         <v>1</v>
       </c>
@@ -18192,21 +18356,80 @@
       <c r="M13" s="45" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="15" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="U13" s="45">
+        <v>0</v>
+      </c>
+      <c r="V13" s="45">
+        <v>1</v>
+      </c>
+      <c r="W13" s="45">
+        <v>1</v>
+      </c>
+      <c r="X13" s="45">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="45"/>
+      <c r="Z13" s="45">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="U14" s="45">
+        <v>0</v>
+      </c>
+      <c r="V14" s="45">
+        <v>1</v>
+      </c>
+      <c r="W14" s="45">
+        <v>1</v>
+      </c>
+      <c r="X14" s="45">
+        <v>1</v>
+      </c>
+      <c r="Y14" s="45"/>
+      <c r="Z14" s="45">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="3:27" x14ac:dyDescent="0.25">
       <c r="Q15" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="16" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="U15" s="45"/>
+    </row>
+    <row r="16" spans="3:27" x14ac:dyDescent="0.25">
       <c r="Q16">
         <v>0</v>
       </c>
       <c r="R16" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="17" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="U16" s="45">
+        <v>1</v>
+      </c>
+      <c r="V16" s="45">
+        <v>0</v>
+      </c>
+      <c r="W16" s="45">
+        <v>0</v>
+      </c>
+      <c r="X16" s="45">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="45">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>165</v>
       </c>
@@ -18216,24 +18439,60 @@
       <c r="R17" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="18" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="D18" s="243" t="s">
+      <c r="U17" s="45">
+        <v>1</v>
+      </c>
+      <c r="V17" s="45">
+        <v>0</v>
+      </c>
+      <c r="W17" s="45">
+        <v>0</v>
+      </c>
+      <c r="X17" s="45">
+        <v>1</v>
+      </c>
+      <c r="Z17" s="45">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="D18" s="244" t="s">
         <v>166</v>
       </c>
-      <c r="E18" s="243"/>
-      <c r="G18" s="243" t="s">
+      <c r="E18" s="244"/>
+      <c r="G18" s="244" t="s">
         <v>169</v>
       </c>
-      <c r="H18" s="243"/>
+      <c r="H18" s="244"/>
       <c r="Q18">
         <v>2</v>
       </c>
       <c r="R18" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="19" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="U18" s="45">
+        <v>1</v>
+      </c>
+      <c r="V18" s="45">
+        <v>0</v>
+      </c>
+      <c r="W18" s="45">
+        <v>1</v>
+      </c>
+      <c r="X18" s="45">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="45">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D19" s="45">
         <v>0</v>
       </c>
@@ -18252,8 +18511,26 @@
       <c r="R19" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="20" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="U19" s="45">
+        <v>1</v>
+      </c>
+      <c r="V19" s="45">
+        <v>0</v>
+      </c>
+      <c r="W19" s="45">
+        <v>1</v>
+      </c>
+      <c r="X19" s="45">
+        <v>1</v>
+      </c>
+      <c r="Z19" s="45">
+        <v>0</v>
+      </c>
+      <c r="AA19" s="45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
         <v>167</v>
       </c>
@@ -18266,8 +18543,66 @@
       <c r="H20" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="23" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="U20" s="45">
+        <v>1</v>
+      </c>
+      <c r="V20" s="45">
+        <v>1</v>
+      </c>
+      <c r="W20" s="45">
+        <v>0</v>
+      </c>
+      <c r="X20" s="45">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="45">
+        <v>1</v>
+      </c>
+      <c r="AA20" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="U21" s="45">
+        <v>1</v>
+      </c>
+      <c r="V21" s="45">
+        <v>1</v>
+      </c>
+      <c r="W21" s="45">
+        <v>0</v>
+      </c>
+      <c r="X21" s="45">
+        <v>1</v>
+      </c>
+      <c r="Z21" s="45">
+        <v>1</v>
+      </c>
+      <c r="AA21" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="U22" s="45">
+        <v>1</v>
+      </c>
+      <c r="V22" s="45">
+        <v>1</v>
+      </c>
+      <c r="W22" s="45">
+        <v>1</v>
+      </c>
+      <c r="X22" s="45">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="45">
+        <v>1</v>
+      </c>
+      <c r="AA22" s="45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C23" s="45" t="s">
         <v>190</v>
       </c>
@@ -18280,8 +18615,26 @@
       <c r="F23" s="119" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="24" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="U23" s="45">
+        <v>1</v>
+      </c>
+      <c r="V23" s="45">
+        <v>1</v>
+      </c>
+      <c r="W23" s="45">
+        <v>1</v>
+      </c>
+      <c r="X23" s="45">
+        <v>1</v>
+      </c>
+      <c r="Z23" s="45">
+        <v>1</v>
+      </c>
+      <c r="AA23" s="45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C24" s="45">
         <v>0</v>
       </c>
@@ -18304,7 +18657,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="25" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C25" s="45">
         <v>0</v>
       </c>
@@ -18318,7 +18671,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="26" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C26" s="45">
         <v>0</v>
       </c>
@@ -18332,7 +18685,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="27" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C27" s="45">
         <v>0</v>
       </c>
@@ -18345,11 +18698,14 @@
       <c r="F27" s="45" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="28" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="G27" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="28" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C28" s="45"/>
     </row>
-    <row r="29" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C29" s="45">
         <v>1</v>
       </c>
@@ -18363,7 +18719,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="30" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C30" s="45">
         <v>1</v>
       </c>
@@ -18377,7 +18733,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="31" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C31" s="45">
         <v>1</v>
       </c>
@@ -18391,7 +18747,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C32" s="45">
         <v>1</v>
       </c>
@@ -18408,28 +18764,40 @@
         <v>194</v>
       </c>
     </row>
-    <row r="33" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C33" s="45"/>
       <c r="O33" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="34" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="U33" s="209" t="s">
+        <v>235</v>
+      </c>
+      <c r="V33" s="209" t="s">
+        <v>235</v>
+      </c>
+      <c r="W33" s="209" t="s">
+        <v>235</v>
+      </c>
+      <c r="X33" s="209" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="34" spans="3:24" x14ac:dyDescent="0.25">
       <c r="O34" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="35" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:24" x14ac:dyDescent="0.25">
       <c r="O35" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="36" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:24" x14ac:dyDescent="0.25">
       <c r="O36" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="37" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:24" x14ac:dyDescent="0.25">
       <c r="O37" t="s">
         <v>198</v>
       </c>

</xml_diff>

<commit_message>
Implemented Stack -> revisit Pop
</commit_message>
<xml_diff>
--- a/Documentation/CPU_DOC.xlsx
+++ b/Documentation/CPU_DOC.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Desktop\CPU_8Bit\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D3C4A8-5703-49D3-82EC-9462678F7AC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A3C255-8FD6-4264-A41A-A32640F8F2E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="2" xr2:uid="{5BA4E079-EFAB-4B55-B322-C6522B3056FF}"/>
+    <workbookView xWindow="38280" yWindow="3585" windowWidth="29040" windowHeight="16440" xr2:uid="{5BA4E079-EFAB-4B55-B322-C6522B3056FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Control-Unit" sheetId="1" r:id="rId1"/>
-    <sheet name="ALU-PROM" sheetId="2" r:id="rId2"/>
-    <sheet name="Schmierblatt" sheetId="3" r:id="rId3"/>
+    <sheet name="Memory" sheetId="4" r:id="rId2"/>
+    <sheet name="ALU-PROM" sheetId="2" r:id="rId3"/>
+    <sheet name="Schmierblatt" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="254">
   <si>
     <t>1=Read</t>
   </si>
@@ -746,6 +747,64 @@
   </si>
   <si>
     <t>0000</t>
+  </si>
+  <si>
+    <t>*SP++ = ACC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memory 65.536 Byte </t>
+  </si>
+  <si>
+    <t>ADDRESS</t>
+  </si>
+  <si>
+    <t>0x0000</t>
+  </si>
+  <si>
+    <t>0x4000</t>
+  </si>
+  <si>
+    <t>Program
+[16kB]</t>
+  </si>
+  <si>
+    <t>System
+[2kB]</t>
+  </si>
+  <si>
+    <t>0x3FFF</t>
+  </si>
+  <si>
+    <t>0X47FF</t>
+  </si>
+  <si>
+    <t>0x4800</t>
+  </si>
+  <si>
+    <t>0x57FF</t>
+  </si>
+  <si>
+    <t>Stack
+[4kB]</t>
+  </si>
+  <si>
+    <t>0x5800</t>
+  </si>
+  <si>
+    <t>0x87FF</t>
+  </si>
+  <si>
+    <t>0x8800</t>
+  </si>
+  <si>
+    <t>Heap
+[12kB]</t>
+  </si>
+  <si>
+    <t>0xFFFF</t>
+  </si>
+  <si>
+    <t>ACC = *--SP</t>
   </si>
 </sst>
 </file>
@@ -937,7 +996,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="72">
+  <borders count="73">
     <border>
       <left/>
       <right/>
@@ -1756,11 +1815,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="254">
+  <cellXfs count="269">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2480,6 +2550,51 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="72" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2851,8 +2966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0373F33-972A-4E8D-B1CE-9C5EF0708B27}">
   <dimension ref="A2:AI157"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F65" sqref="F65"/>
+    <sheetView tabSelected="1" topLeftCell="F51" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K70" sqref="K70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7738,7 +7853,7 @@
         <v>34</v>
       </c>
       <c r="C62" s="132" t="str">
-        <f t="shared" si="4"/>
+        <f>DEC2BIN(D62)</f>
         <v>110100</v>
       </c>
       <c r="D62" s="2">
@@ -7987,10 +8102,7 @@
         <v>55</v>
       </c>
       <c r="E65" s="203"/>
-      <c r="F65" s="46" t="s">
-        <v>229</v>
-      </c>
-      <c r="G65" s="10"/>
+      <c r="F65" s="46"/>
       <c r="H65" s="16"/>
       <c r="L65" s="9"/>
       <c r="M65" s="165">
@@ -8071,11 +8183,24 @@
       </c>
       <c r="E66" s="203"/>
       <c r="F66" s="46" t="s">
-        <v>230</v>
-      </c>
-      <c r="G66" s="10"/>
+        <v>229</v>
+      </c>
+      <c r="G66" s="10" t="s">
+        <v>236</v>
+      </c>
       <c r="H66" s="16"/>
-      <c r="L66" s="9"/>
+      <c r="I66" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="J66" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="K66" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="L66" s="9" t="s">
+        <v>90</v>
+      </c>
       <c r="M66" s="165">
         <v>1</v>
       </c>
@@ -8098,10 +8223,10 @@
         <v>0</v>
       </c>
       <c r="T66" s="45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U66" s="46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V66" s="45">
         <v>1</v>
@@ -8113,7 +8238,7 @@
         <v>0</v>
       </c>
       <c r="Y66" s="46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z66" s="45">
         <v>0</v>
@@ -8129,15 +8254,15 @@
       </c>
       <c r="AD66" s="168" t="str">
         <f t="shared" si="1"/>
-        <v>CBC0</v>
+        <v>C300</v>
       </c>
       <c r="AE66" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>CB</v>
+        <v>C3</v>
       </c>
       <c r="AF66" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>C0</v>
+        <v>00</v>
       </c>
     </row>
     <row r="67" spans="1:32" x14ac:dyDescent="0.25">
@@ -8154,11 +8279,24 @@
       </c>
       <c r="E67" s="203"/>
       <c r="F67" s="46" t="s">
-        <v>231</v>
-      </c>
-      <c r="G67" s="10"/>
+        <v>230</v>
+      </c>
+      <c r="G67" s="10" t="s">
+        <v>253</v>
+      </c>
       <c r="H67" s="16"/>
-      <c r="L67" s="9"/>
+      <c r="I67" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="J67" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="K67" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="L67" s="9" t="s">
+        <v>90</v>
+      </c>
       <c r="M67" s="165">
         <v>1</v>
       </c>
@@ -8181,7 +8319,7 @@
         <v>0</v>
       </c>
       <c r="T67" s="45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U67" s="46">
         <v>1</v>
@@ -8190,7 +8328,7 @@
         <v>1</v>
       </c>
       <c r="W67" s="45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X67" s="45">
         <v>0</v>
@@ -8212,15 +8350,15 @@
       </c>
       <c r="AD67" s="168" t="str">
         <f t="shared" si="1"/>
-        <v>CBC0</v>
+        <v>C980</v>
       </c>
       <c r="AE67" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>CB</v>
+        <v>C9</v>
       </c>
       <c r="AF67" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>C0</v>
+        <v>80</v>
       </c>
     </row>
     <row r="68" spans="1:32" x14ac:dyDescent="0.25">
@@ -8237,7 +8375,7 @@
       </c>
       <c r="E68" s="203"/>
       <c r="F68" s="46" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G68" s="10"/>
       <c r="H68" s="16"/>
@@ -8319,7 +8457,9 @@
         <v>59</v>
       </c>
       <c r="E69" s="203"/>
-      <c r="F69" s="46"/>
+      <c r="F69" s="46" t="s">
+        <v>232</v>
+      </c>
       <c r="G69" s="10"/>
       <c r="H69" s="16"/>
       <c r="L69" s="9"/>
@@ -9641,10 +9781,16 @@
       <c r="S85" s="45">
         <v>0</v>
       </c>
-      <c r="U85" s="11"/>
-      <c r="Y85" s="11"/>
-      <c r="AA85" s="11"/>
-      <c r="AC85" s="135"/>
+      <c r="T85" s="45"/>
+      <c r="U85" s="46"/>
+      <c r="V85" s="45"/>
+      <c r="W85" s="45"/>
+      <c r="X85" s="45"/>
+      <c r="Y85" s="46"/>
+      <c r="Z85" s="45"/>
+      <c r="AA85" s="46"/>
+      <c r="AB85" s="45"/>
+      <c r="AC85" s="148"/>
       <c r="AD85" s="168" t="str">
         <f t="shared" si="6"/>
         <v>0000</v>
@@ -12567,6 +12713,267 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69115442-7425-4F0D-B9B2-16B86C1ECAC6}">
+  <dimension ref="F4:G54"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N44" sqref="N44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="6.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="31.5703125" style="45" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="6:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F4" s="45" t="s">
+        <v>238</v>
+      </c>
+      <c r="G4" s="45" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="5" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F5" s="255" t="s">
+        <v>239</v>
+      </c>
+      <c r="G5" s="258" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="6" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F6" s="254"/>
+      <c r="G6" s="259"/>
+    </row>
+    <row r="7" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F7" s="254"/>
+      <c r="G7" s="259"/>
+    </row>
+    <row r="8" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F8" s="254"/>
+      <c r="G8" s="259"/>
+    </row>
+    <row r="9" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F9" s="254"/>
+      <c r="G9" s="259"/>
+    </row>
+    <row r="10" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F10" s="254"/>
+      <c r="G10" s="259"/>
+    </row>
+    <row r="11" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F11" s="254"/>
+      <c r="G11" s="259"/>
+    </row>
+    <row r="12" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F12" s="254"/>
+      <c r="G12" s="259"/>
+    </row>
+    <row r="13" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F13" s="254"/>
+      <c r="G13" s="259"/>
+    </row>
+    <row r="14" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F14" s="254"/>
+      <c r="G14" s="259"/>
+    </row>
+    <row r="15" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F15" s="254"/>
+      <c r="G15" s="259"/>
+    </row>
+    <row r="16" spans="6:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F16" s="257" t="s">
+        <v>243</v>
+      </c>
+      <c r="G16" s="260"/>
+    </row>
+    <row r="17" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F17" s="254" t="s">
+        <v>240</v>
+      </c>
+      <c r="G17" s="261" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="18" spans="6:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F18" s="257" t="s">
+        <v>244</v>
+      </c>
+      <c r="G18" s="262"/>
+    </row>
+    <row r="19" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F19" s="254" t="s">
+        <v>245</v>
+      </c>
+      <c r="G19" s="263" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="20" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F20" s="254"/>
+      <c r="G20" s="264"/>
+    </row>
+    <row r="21" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F21" s="254"/>
+      <c r="G21" s="264"/>
+    </row>
+    <row r="22" spans="6:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F22" s="257" t="s">
+        <v>246</v>
+      </c>
+      <c r="G22" s="265"/>
+    </row>
+    <row r="23" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F23" s="254" t="s">
+        <v>248</v>
+      </c>
+      <c r="G23" s="268" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="24" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F24" s="254"/>
+      <c r="G24" s="266"/>
+    </row>
+    <row r="25" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F25" s="254"/>
+      <c r="G25" s="266"/>
+    </row>
+    <row r="26" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F26" s="254"/>
+      <c r="G26" s="266"/>
+    </row>
+    <row r="27" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F27" s="254"/>
+      <c r="G27" s="266"/>
+    </row>
+    <row r="28" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F28" s="254"/>
+      <c r="G28" s="266"/>
+    </row>
+    <row r="29" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F29" s="254"/>
+      <c r="G29" s="266"/>
+    </row>
+    <row r="30" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F30" s="254"/>
+      <c r="G30" s="266"/>
+    </row>
+    <row r="31" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F31" s="254"/>
+      <c r="G31" s="266"/>
+    </row>
+    <row r="32" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F32" s="254"/>
+      <c r="G32" s="266"/>
+    </row>
+    <row r="33" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F33" s="254"/>
+      <c r="G33" s="266"/>
+    </row>
+    <row r="34" spans="6:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F34" s="257" t="s">
+        <v>249</v>
+      </c>
+      <c r="G34" s="267"/>
+    </row>
+    <row r="35" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F35" s="254" t="s">
+        <v>250</v>
+      </c>
+      <c r="G35" s="83"/>
+    </row>
+    <row r="36" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F36" s="254"/>
+      <c r="G36" s="83"/>
+    </row>
+    <row r="37" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F37" s="254"/>
+      <c r="G37" s="83"/>
+    </row>
+    <row r="38" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F38" s="254"/>
+      <c r="G38" s="83"/>
+    </row>
+    <row r="39" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F39" s="254"/>
+      <c r="G39" s="83"/>
+    </row>
+    <row r="40" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F40" s="254"/>
+      <c r="G40" s="83"/>
+    </row>
+    <row r="41" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F41" s="254"/>
+      <c r="G41" s="83"/>
+    </row>
+    <row r="42" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F42" s="254"/>
+      <c r="G42" s="83"/>
+    </row>
+    <row r="43" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F43" s="254"/>
+      <c r="G43" s="83"/>
+    </row>
+    <row r="44" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F44" s="254"/>
+      <c r="G44" s="83"/>
+    </row>
+    <row r="45" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F45" s="254"/>
+      <c r="G45" s="83"/>
+    </row>
+    <row r="46" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F46" s="254"/>
+      <c r="G46" s="83"/>
+    </row>
+    <row r="47" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F47" s="254"/>
+      <c r="G47" s="83"/>
+    </row>
+    <row r="48" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F48" s="254"/>
+      <c r="G48" s="83"/>
+    </row>
+    <row r="49" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F49" s="254"/>
+      <c r="G49" s="83"/>
+    </row>
+    <row r="50" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F50" s="254"/>
+      <c r="G50" s="83"/>
+    </row>
+    <row r="51" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F51" s="254"/>
+      <c r="G51" s="83"/>
+    </row>
+    <row r="52" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F52" s="254"/>
+      <c r="G52" s="83"/>
+    </row>
+    <row r="53" spans="6:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F53" s="257" t="s">
+        <v>252</v>
+      </c>
+      <c r="G53" s="84"/>
+    </row>
+    <row r="54" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="G54" s="256"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="G5:G16"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="G19:G22"/>
+    <mergeCell ref="G23:G34"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE962138-36AF-4A36-ABB3-AE05CD0A9894}">
   <dimension ref="A2:AX69"/>
   <sheetViews>
@@ -17944,11 +18351,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F461F9F-87D6-4C96-820F-6111A3E2F850}">
   <dimension ref="C4:AA37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>

</xml_diff>